<commit_message>
Added IPT coverage data points
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -1112,7 +1112,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1167,6 +1167,7 @@
     <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2238,13 +2239,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AB16"/>
+  <dimension ref="A1:AI16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB2" sqref="AB2"/>
+      <selection pane="bottomRight" activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2260,15 +2261,15 @@
     <col min="12" max="12" width="7.140625" style="1" customWidth="1"/>
     <col min="13" max="14" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="7" style="1" customWidth="1"/>
-    <col min="17" max="18" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.85546875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="14" style="1" customWidth="1"/>
-    <col min="21" max="28" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="1"/>
+    <col min="16" max="17" width="7" style="1" customWidth="1"/>
+    <col min="18" max="19" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="26" width="7.85546875" style="1" customWidth="1"/>
+    <col min="27" max="27" width="14" style="1" customWidth="1"/>
+    <col min="28" max="35" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -2318,43 +2319,64 @@
         <v>2001</v>
       </c>
       <c r="Q1" s="5">
+        <v>2011</v>
+      </c>
+      <c r="R1" s="5">
         <v>2012</v>
       </c>
-      <c r="R1" s="5">
+      <c r="S1" s="5">
         <v>2013</v>
       </c>
-      <c r="S1" s="5">
+      <c r="T1" s="5">
         <v>2014</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5">
+        <v>2015</v>
+      </c>
+      <c r="V1" s="5">
+        <v>2016</v>
+      </c>
+      <c r="W1" s="5">
+        <v>2017</v>
+      </c>
+      <c r="X1" s="5">
+        <v>2018</v>
+      </c>
+      <c r="Y1" s="5">
+        <v>2019</v>
+      </c>
+      <c r="Z1" s="5">
+        <v>2035</v>
+      </c>
+      <c r="AA1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AI1" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>4</v>
       </c>
@@ -2383,14 +2405,21 @@
       <c r="Q2" s="25"/>
       <c r="R2" s="25"/>
       <c r="S2" s="25"/>
-      <c r="Y2" s="7">
+      <c r="T2" s="25"/>
+      <c r="U2" s="50"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="50"/>
+      <c r="X2" s="50"/>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="50"/>
+      <c r="AF2" s="7">
         <v>100</v>
       </c>
-      <c r="AB2" s="7">
+      <c r="AI2" s="7">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>5</v>
       </c>
@@ -2415,20 +2444,27 @@
       <c r="P3" s="26"/>
       <c r="Q3" s="26"/>
       <c r="R3" s="26"/>
-      <c r="S3" s="26">
+      <c r="S3" s="26"/>
+      <c r="T3" s="26">
         <v>50</v>
       </c>
-      <c r="V3" s="9">
+      <c r="U3" s="50"/>
+      <c r="V3" s="50"/>
+      <c r="W3" s="50"/>
+      <c r="X3" s="50"/>
+      <c r="Y3" s="50"/>
+      <c r="Z3" s="50"/>
+      <c r="AC3" s="9">
         <v>60</v>
       </c>
-      <c r="W3" s="9">
+      <c r="AD3" s="9">
         <v>75</v>
       </c>
-      <c r="AB3" s="9">
+      <c r="AI3" s="9">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>36</v>
       </c>
@@ -2441,17 +2477,77 @@
       <c r="D4" s="8" t="s">
         <v>9</v>
       </c>
+      <c r="E4" s="9">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0</v>
+      </c>
+      <c r="K4" s="9">
+        <v>0</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0</v>
+      </c>
+      <c r="N4" s="9">
+        <v>0</v>
+      </c>
+      <c r="O4" s="9">
+        <v>0</v>
+      </c>
+      <c r="P4" s="9">
+        <v>0</v>
+      </c>
       <c r="Q4" s="9">
         <v>0</v>
       </c>
-      <c r="AA4" s="9">
+      <c r="R4" s="9">
+        <v>7</v>
+      </c>
+      <c r="T4" s="9">
+        <v>23.6</v>
+      </c>
+      <c r="U4" s="9">
+        <v>34</v>
+      </c>
+      <c r="V4" s="9">
+        <v>44</v>
+      </c>
+      <c r="W4" s="9">
+        <v>54</v>
+      </c>
+      <c r="X4" s="9">
+        <v>64</v>
+      </c>
+      <c r="Y4" s="9">
+        <v>74</v>
+      </c>
+      <c r="Z4" s="9">
+        <v>99.99</v>
+      </c>
+      <c r="AH4" s="9">
         <v>50</v>
       </c>
-      <c r="AB4" s="9">
+      <c r="AI4" s="9">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>6</v>
       </c>
@@ -2476,17 +2572,17 @@
       <c r="P5" s="11">
         <v>84</v>
       </c>
-      <c r="R5" s="11">
+      <c r="S5" s="11">
         <v>85</v>
       </c>
-      <c r="X5" s="11">
+      <c r="AE5" s="11">
         <v>90</v>
       </c>
-      <c r="AB5" s="11">
+      <c r="AI5" s="11">
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -2508,11 +2604,11 @@
       <c r="M6" s="13">
         <v>40</v>
       </c>
-      <c r="AB6" s="13">
+      <c r="AI6" s="13">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>7</v>
       </c>
@@ -2535,7 +2631,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>8</v>
       </c>
@@ -2558,7 +2654,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>14</v>
       </c>
@@ -2583,23 +2679,24 @@
       <c r="N9" s="27"/>
       <c r="O9" s="27"/>
       <c r="P9" s="27"/>
-      <c r="Q9" s="27">
+      <c r="Q9" s="27"/>
+      <c r="R9" s="27">
         <v>93</v>
       </c>
-      <c r="R9" s="27">
+      <c r="S9" s="27">
         <v>85</v>
       </c>
-      <c r="T9" s="13">
+      <c r="AA9" s="13">
         <v>91.1</v>
-      </c>
-      <c r="U9" s="13">
-        <v>96</v>
       </c>
       <c r="AB9" s="13">
         <v>96</v>
       </c>
+      <c r="AI9" s="13">
+        <v>96</v>
+      </c>
     </row>
-    <row r="10" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>15</v>
       </c>
@@ -2626,20 +2723,21 @@
       <c r="P10" s="27"/>
       <c r="Q10" s="27"/>
       <c r="R10" s="27"/>
-      <c r="S10" s="13">
+      <c r="S10" s="27"/>
+      <c r="T10" s="13">
         <v>5</v>
       </c>
-      <c r="T10" s="13">
+      <c r="AA10" s="13">
         <v>1.6</v>
-      </c>
-      <c r="U10" s="13">
-        <v>1.25</v>
       </c>
       <c r="AB10" s="13">
         <v>1.25</v>
       </c>
+      <c r="AI10" s="13">
+        <v>1.25</v>
+      </c>
     </row>
-    <row r="11" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>16</v>
       </c>
@@ -2666,11 +2764,12 @@
       <c r="P11" s="28"/>
       <c r="Q11" s="28"/>
       <c r="R11" s="28"/>
-      <c r="S11" s="24">
+      <c r="S11" s="28"/>
+      <c r="T11" s="24">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>17</v>
       </c>
@@ -2697,11 +2796,12 @@
       <c r="P12" s="28"/>
       <c r="Q12" s="28"/>
       <c r="R12" s="28"/>
-      <c r="S12" s="24">
+      <c r="S12" s="28"/>
+      <c r="T12" s="24">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>18</v>
       </c>
@@ -2728,11 +2828,12 @@
       <c r="P13" s="26"/>
       <c r="Q13" s="26"/>
       <c r="R13" s="26"/>
-      <c r="S13" s="9">
+      <c r="S13" s="26"/>
+      <c r="T13" s="9">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>19</v>
       </c>
@@ -2759,11 +2860,12 @@
       <c r="P14" s="26"/>
       <c r="Q14" s="26"/>
       <c r="R14" s="26"/>
-      <c r="S14" s="9">
+      <c r="S14" s="26"/>
+      <c r="T14" s="9">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:28" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
         <v>30</v>
       </c>
@@ -2781,14 +2883,15 @@
       <c r="P15" s="35"/>
       <c r="Q15" s="35"/>
       <c r="R15" s="35"/>
-      <c r="S15" s="34">
+      <c r="S15" s="35"/>
+      <c r="T15" s="34">
         <v>0</v>
       </c>
-      <c r="Z15" s="34">
+      <c r="AG15" s="34">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="E16" s="36"/>
       <c r="F16" s="36"/>
       <c r="G16" s="36"/>
@@ -2798,7 +2901,7 @@
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="4">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T15:U15 E4:U4">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA15:AB15 E4:AB4">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
@@ -2807,7 +2910,7 @@
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:U14 E15:S15 E2:U3">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:AB14 E15:Z15 E2:AB3">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Get test_full_models running again
Debug as Tan's entries stopped the test script running.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -1112,7 +1112,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1167,7 +1167,6 @@
     <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2239,13 +2238,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AI16"/>
+  <dimension ref="A1:AC16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z4" sqref="Z4"/>
+      <selection pane="bottomRight" activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2263,13 +2262,13 @@
     <col min="15" max="15" width="7.5703125" style="1" customWidth="1"/>
     <col min="16" max="17" width="7" style="1" customWidth="1"/>
     <col min="18" max="19" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="26" width="7.85546875" style="1" customWidth="1"/>
-    <col min="27" max="27" width="14" style="1" customWidth="1"/>
-    <col min="28" max="35" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="16384" width="9.140625" style="1"/>
+    <col min="20" max="20" width="7.85546875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="14" style="1" customWidth="1"/>
+    <col min="22" max="29" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -2330,53 +2329,35 @@
       <c r="T1" s="5">
         <v>2014</v>
       </c>
-      <c r="U1" s="5">
-        <v>2015</v>
-      </c>
-      <c r="V1" s="5">
-        <v>2016</v>
-      </c>
-      <c r="W1" s="5">
-        <v>2017</v>
-      </c>
-      <c r="X1" s="5">
-        <v>2018</v>
-      </c>
-      <c r="Y1" s="5">
-        <v>2019</v>
-      </c>
-      <c r="Z1" s="5">
-        <v>2035</v>
+      <c r="U1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="AA1" s="5" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="AB1" s="5" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="AC1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AG1" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="AH1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="AI1" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:35" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>4</v>
       </c>
@@ -2406,20 +2387,14 @@
       <c r="R2" s="25"/>
       <c r="S2" s="25"/>
       <c r="T2" s="25"/>
-      <c r="U2" s="50"/>
-      <c r="V2" s="50"/>
-      <c r="W2" s="50"/>
-      <c r="X2" s="50"/>
-      <c r="Y2" s="50"/>
-      <c r="Z2" s="50"/>
-      <c r="AF2" s="7">
+      <c r="Z2" s="7">
         <v>100</v>
       </c>
-      <c r="AI2" s="7">
+      <c r="AC2" s="7">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>5</v>
       </c>
@@ -2448,23 +2423,17 @@
       <c r="T3" s="26">
         <v>50</v>
       </c>
-      <c r="U3" s="50"/>
-      <c r="V3" s="50"/>
-      <c r="W3" s="50"/>
-      <c r="X3" s="50"/>
-      <c r="Y3" s="50"/>
-      <c r="Z3" s="50"/>
+      <c r="W3" s="9">
+        <v>60</v>
+      </c>
+      <c r="X3" s="9">
+        <v>75</v>
+      </c>
       <c r="AC3" s="9">
-        <v>60</v>
-      </c>
-      <c r="AD3" s="9">
         <v>75</v>
       </c>
-      <c r="AI3" s="9">
-        <v>75</v>
-      </c>
     </row>
-    <row r="4" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>36</v>
       </c>
@@ -2522,32 +2491,14 @@
       <c r="T4" s="9">
         <v>23.6</v>
       </c>
-      <c r="U4" s="9">
-        <v>34</v>
-      </c>
-      <c r="V4" s="9">
-        <v>44</v>
-      </c>
-      <c r="W4" s="9">
-        <v>54</v>
-      </c>
-      <c r="X4" s="9">
-        <v>64</v>
-      </c>
-      <c r="Y4" s="9">
-        <v>74</v>
-      </c>
-      <c r="Z4" s="9">
-        <v>99.99</v>
-      </c>
-      <c r="AH4" s="9">
+      <c r="AB4" s="9">
         <v>50</v>
       </c>
-      <c r="AI4" s="9">
+      <c r="AC4" s="9">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:35" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>6</v>
       </c>
@@ -2575,14 +2526,14 @@
       <c r="S5" s="11">
         <v>85</v>
       </c>
-      <c r="AE5" s="11">
+      <c r="Y5" s="11">
         <v>90</v>
       </c>
-      <c r="AI5" s="11">
+      <c r="AC5" s="11">
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:35" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -2604,11 +2555,11 @@
       <c r="M6" s="13">
         <v>40</v>
       </c>
-      <c r="AI6" s="13">
+      <c r="AC6" s="13">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>7</v>
       </c>
@@ -2631,7 +2582,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>8</v>
       </c>
@@ -2654,7 +2605,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:35" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>14</v>
       </c>
@@ -2686,17 +2637,17 @@
       <c r="S9" s="27">
         <v>85</v>
       </c>
-      <c r="AA9" s="13">
+      <c r="U9" s="13">
         <v>91.1</v>
       </c>
-      <c r="AB9" s="13">
+      <c r="V9" s="13">
         <v>96</v>
       </c>
-      <c r="AI9" s="13">
+      <c r="AC9" s="13">
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:35" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>15</v>
       </c>
@@ -2727,17 +2678,17 @@
       <c r="T10" s="13">
         <v>5</v>
       </c>
-      <c r="AA10" s="13">
+      <c r="U10" s="13">
         <v>1.6</v>
       </c>
-      <c r="AB10" s="13">
+      <c r="V10" s="13">
         <v>1.25</v>
       </c>
-      <c r="AI10" s="13">
+      <c r="AC10" s="13">
         <v>1.25</v>
       </c>
     </row>
-    <row r="11" spans="1:35" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>16</v>
       </c>
@@ -2769,7 +2720,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:35" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>17</v>
       </c>
@@ -2801,7 +2752,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>18</v>
       </c>
@@ -2833,7 +2784,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>19</v>
       </c>
@@ -2865,7 +2816,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:35" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
         <v>30</v>
       </c>
@@ -2887,11 +2838,11 @@
       <c r="T15" s="34">
         <v>0</v>
       </c>
-      <c r="AG15" s="34">
+      <c r="AA15" s="34">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E16" s="36"/>
       <c r="F16" s="36"/>
       <c r="G16" s="36"/>
@@ -2901,7 +2852,7 @@
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="4">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA15:AB15 E4:AB4">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U15:V15 E4:V4">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
@@ -2910,7 +2861,7 @@
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:AB14 E15:Z15 E2:AB3">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E15:T15 E2:V3 E5:V14">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Age stratification of IPT
Possibly needs one last round of checking and needs comments, but seems
to be running OK.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
   <si>
     <t>program_prop_lowquality</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>age_unstratified</t>
+  </si>
+  <si>
+    <t>scenario_12</t>
+  </si>
+  <si>
+    <t>program_prop_ipt_age0to5</t>
+  </si>
+  <si>
+    <t>program_prop_ipt_age5to15</t>
   </si>
 </sst>
 </file>
@@ -2234,13 +2243,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AO18"/>
+  <dimension ref="A1:AP20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P14" sqref="P14"/>
+      <selection pane="bottomRight" activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2261,12 +2270,12 @@
     <col min="20" max="20" width="7.85546875" style="1" customWidth="1"/>
     <col min="21" max="21" width="14" style="1" customWidth="1"/>
     <col min="22" max="28" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="14.42578125" style="1" customWidth="1"/>
-    <col min="31" max="31" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="9.140625" style="1"/>
+    <col min="29" max="31" width="14.42578125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -2360,8 +2369,11 @@
       <c r="AE1" s="5" t="s">
         <v>43</v>
       </c>
+      <c r="AF1" s="5" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="2" spans="1:41" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>4</v>
       </c>
@@ -2394,11 +2406,11 @@
       <c r="Z2" s="7">
         <v>100</v>
       </c>
-      <c r="AE2" s="7">
+      <c r="AF2" s="7">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:41" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>5</v>
       </c>
@@ -2433,11 +2445,11 @@
       <c r="X3" s="9">
         <v>75</v>
       </c>
-      <c r="AE3" s="9">
+      <c r="AF3" s="9">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:41" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>34</v>
       </c>
@@ -2453,499 +2465,513 @@
       <c r="E4" s="9">
         <v>0</v>
       </c>
-      <c r="F4" s="9">
+      <c r="T4" s="9">
         <v>0</v>
-      </c>
-      <c r="G4" s="9">
-        <v>0</v>
-      </c>
-      <c r="H4" s="9">
-        <v>0</v>
-      </c>
-      <c r="I4" s="9">
-        <v>0</v>
-      </c>
-      <c r="J4" s="9">
-        <v>0</v>
-      </c>
-      <c r="K4" s="9">
-        <v>0</v>
-      </c>
-      <c r="L4" s="9">
-        <v>0</v>
-      </c>
-      <c r="M4" s="9">
-        <v>0</v>
-      </c>
-      <c r="N4" s="9">
-        <v>0</v>
-      </c>
-      <c r="O4" s="9">
-        <v>0</v>
-      </c>
-      <c r="P4" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="9">
-        <v>0</v>
-      </c>
-      <c r="R4" s="9">
-        <v>7</v>
-      </c>
-      <c r="T4" s="9">
-        <v>23.6</v>
       </c>
       <c r="AB4" s="9">
         <v>50</v>
       </c>
-      <c r="AE4" s="9">
+      <c r="AF4" s="9">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:41" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>0</v>
+      </c>
+      <c r="R5" s="9">
+        <v>7</v>
+      </c>
+      <c r="T5" s="9">
+        <v>23.6</v>
+      </c>
+      <c r="AC5" s="9">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0</v>
+      </c>
+      <c r="T6" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C7" s="10">
         <v>1</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="11">
+      <c r="D7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="11">
         <v>70</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H7" s="11">
         <v>80</v>
       </c>
-      <c r="L5" s="11">
+      <c r="L7" s="11">
         <v>82</v>
       </c>
-      <c r="P5" s="11">
+      <c r="P7" s="11">
         <v>84</v>
       </c>
-      <c r="S5" s="11">
+      <c r="S7" s="11">
         <v>85</v>
       </c>
-      <c r="Y5" s="11">
+      <c r="Y7" s="11">
         <v>90</v>
       </c>
-      <c r="AE5" s="11">
+      <c r="AF7" s="11">
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:41" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+    <row r="8" spans="1:32" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C8" s="12">
         <v>1</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="13">
+      <c r="D8" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="13">
         <v>30</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I8" s="13">
         <v>40</v>
       </c>
-      <c r="M6" s="13">
+      <c r="M8" s="13">
         <v>40</v>
       </c>
-      <c r="AE6" s="13">
+      <c r="AF8" s="13">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:41" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+    <row r="9" spans="1:32" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C9" s="14">
         <v>1</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="15">
+      <c r="D9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="15">
         <v>30</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M9" s="15">
         <v>40</v>
       </c>
-      <c r="O7" s="15">
+      <c r="O9" s="15">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:41" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+    <row r="10" spans="1:32" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B10" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C10" s="14">
         <v>1</v>
       </c>
-      <c r="D8" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="15">
+      <c r="D10" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="15">
         <v>7</v>
       </c>
-      <c r="N8" s="15">
+      <c r="N10" s="15">
         <v>50</v>
       </c>
-      <c r="O8" s="15">
+      <c r="O10" s="15">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:41" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+    <row r="11" spans="1:32" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="12">
+      <c r="B11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="12">
         <v>1</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="13">
+      <c r="D11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="13">
         <v>0</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J11" s="13">
         <v>40</v>
       </c>
-      <c r="K9" s="13">
+      <c r="K11" s="13">
         <v>65</v>
       </c>
-      <c r="N9" s="27"/>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="27">
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27">
         <v>93</v>
       </c>
-      <c r="S9" s="27">
+      <c r="S11" s="27">
         <v>85</v>
       </c>
-      <c r="V9" s="13">
+      <c r="V11" s="13">
         <v>96</v>
       </c>
-      <c r="AE9" s="13">
+      <c r="AF11" s="13">
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:41" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+    <row r="12" spans="1:32" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="12">
+      <c r="B12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="12">
         <v>3</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="13">
+      <c r="D12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="13">
         <v>0</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J12" s="13">
         <v>10</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K12" s="13">
         <v>8</v>
       </c>
-      <c r="N10" s="27"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="27"/>
-      <c r="Q10" s="27"/>
-      <c r="R10" s="27"/>
-      <c r="S10" s="27"/>
-      <c r="T10" s="13">
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
+      <c r="Q12" s="27"/>
+      <c r="R12" s="27"/>
+      <c r="S12" s="27"/>
+      <c r="T12" s="13">
         <v>5</v>
       </c>
-      <c r="V10" s="13">
+      <c r="V12" s="13">
         <v>1.25</v>
       </c>
-      <c r="AE10" s="13">
+      <c r="AF12" s="13">
         <v>1.25</v>
       </c>
     </row>
-    <row r="11" spans="1:41" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+    <row r="13" spans="1:32" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="23">
+      <c r="B13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="23">
         <v>1</v>
       </c>
-      <c r="D11" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="24">
+      <c r="D13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="24">
         <v>0</v>
       </c>
-      <c r="J11" s="24">
+      <c r="J13" s="24">
         <v>15</v>
       </c>
-      <c r="K11" s="24">
+      <c r="K13" s="24">
         <v>30</v>
       </c>
-      <c r="N11" s="28"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="28"/>
-      <c r="R11" s="28"/>
-      <c r="S11" s="28"/>
-      <c r="T11" s="24">
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="24">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:41" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+    <row r="14" spans="1:32" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="23">
+      <c r="B14" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="23">
         <v>1</v>
       </c>
-      <c r="D12" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="24">
+      <c r="D14" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="24">
         <v>0</v>
       </c>
-      <c r="J12" s="24">
+      <c r="J14" s="24">
         <v>55</v>
       </c>
-      <c r="K12" s="24">
+      <c r="K14" s="24">
         <v>50</v>
       </c>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="28"/>
-      <c r="R12" s="28"/>
-      <c r="S12" s="28"/>
-      <c r="T12" s="24">
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="24">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:41" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+    <row r="15" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="8">
+      <c r="B15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="8">
         <v>1</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="9">
+      <c r="D15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="9">
         <v>0</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J15" s="9">
         <v>5</v>
       </c>
-      <c r="K13" s="9">
+      <c r="K15" s="9">
         <v>15</v>
       </c>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="26"/>
-      <c r="S13" s="26"/>
-      <c r="T13" s="9">
+      <c r="N15" s="26"/>
+      <c r="O15" s="26"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="26"/>
+      <c r="R15" s="26"/>
+      <c r="S15" s="26"/>
+      <c r="T15" s="9">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:41" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+    <row r="16" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="8">
+      <c r="B16" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="8">
         <v>1</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="9">
+      <c r="D16" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="9">
         <v>0</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J16" s="9">
         <v>65</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K16" s="9">
         <v>62</v>
       </c>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="26"/>
-      <c r="R14" s="26"/>
-      <c r="S14" s="26"/>
-      <c r="T14" s="9">
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="26"/>
+      <c r="S16" s="26"/>
+      <c r="T16" s="9">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:41" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
+    <row r="17" spans="1:42" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="33">
+      <c r="B17" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="33">
         <v>1</v>
       </c>
-      <c r="D15" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="35"/>
-      <c r="S15" s="35"/>
-      <c r="T15" s="34">
+      <c r="D17" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="N17" s="35"/>
+      <c r="O17" s="35"/>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="35"/>
+      <c r="R17" s="35"/>
+      <c r="S17" s="35"/>
+      <c r="T17" s="34">
         <v>0</v>
       </c>
-      <c r="AA15" s="34">
+      <c r="AA17" s="34">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:41" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+    <row r="18" spans="1:42" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B18" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C18" s="14">
         <v>1</v>
       </c>
-      <c r="D16" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="46">
+      <c r="D18" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="46">
         <v>0</v>
       </c>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="46"/>
-      <c r="M16" s="46"/>
-      <c r="N16" s="46"/>
-      <c r="O16" s="46"/>
-      <c r="P16" s="46"/>
-      <c r="Q16" s="46"/>
-      <c r="R16" s="46"/>
-      <c r="S16" s="46"/>
-      <c r="T16" s="46">
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="46"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="46"/>
+      <c r="Q18" s="46"/>
+      <c r="R18" s="46"/>
+      <c r="S18" s="46"/>
+      <c r="T18" s="46">
         <v>0</v>
       </c>
-      <c r="U16" s="46">
+      <c r="U18" s="46">
         <v>100</v>
       </c>
-      <c r="V16" s="46"/>
-      <c r="W16" s="46"/>
-      <c r="X16" s="46"/>
-      <c r="Y16" s="46"/>
-      <c r="Z16" s="46"/>
-      <c r="AA16" s="46"/>
-      <c r="AB16" s="46"/>
-      <c r="AC16" s="46"/>
-      <c r="AD16" s="46"/>
-      <c r="AE16" s="46"/>
-      <c r="AF16" s="46"/>
-      <c r="AG16" s="46"/>
-      <c r="AH16" s="46"/>
-      <c r="AI16" s="46"/>
-      <c r="AJ16" s="46"/>
-      <c r="AK16" s="46"/>
-      <c r="AL16" s="46"/>
-      <c r="AM16" s="46"/>
-      <c r="AN16" s="46"/>
-      <c r="AO16" s="46"/>
+      <c r="V18" s="46"/>
+      <c r="W18" s="46"/>
+      <c r="X18" s="46"/>
+      <c r="Y18" s="46"/>
+      <c r="Z18" s="46"/>
+      <c r="AA18" s="46"/>
+      <c r="AB18" s="46"/>
+      <c r="AC18" s="46"/>
+      <c r="AD18" s="46"/>
+      <c r="AE18" s="46"/>
+      <c r="AF18" s="46"/>
+      <c r="AG18" s="46"/>
+      <c r="AH18" s="46"/>
+      <c r="AI18" s="46"/>
+      <c r="AJ18" s="46"/>
+      <c r="AK18" s="46"/>
+      <c r="AL18" s="46"/>
+      <c r="AM18" s="46"/>
+      <c r="AN18" s="46"/>
+      <c r="AO18" s="46"/>
+      <c r="AP18" s="46"/>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C19" s="2">
         <v>1</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="1">
+      <c r="D19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="1">
         <v>0</v>
       </c>
-      <c r="T17" s="1">
+      <c r="T19" s="1">
         <v>0</v>
       </c>
-      <c r="AC17" s="1">
+      <c r="AD19" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A20" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C20" s="2">
         <v>1</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="1">
+      <c r="D20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="1">
         <v>0</v>
       </c>
-      <c r="T18" s="1">
+      <c r="T20" s="1">
         <v>0</v>
       </c>
-      <c r="AD18" s="1">
+      <c r="AE20" s="1">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="4">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U15:V15 E4:V4">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U17:V17 E4:V6">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
@@ -2954,7 +2980,7 @@
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E15:T15 E2:V3 E5:V14">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E17:T17 E2:V3 E7:V16">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -2968,7 +2994,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B15</xm:sqref>
+          <xm:sqref>B2:B17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time-variant?" prompt="If no, the most recent value will be selected.">
           <x14:formula1>

</xml_diff>

<commit_message>
Minor tidying of files
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -2249,7 +2249,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X12" sqref="X12"/>
+      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2462,9 +2462,6 @@
       <c r="D4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="9">
-        <v>0</v>
-      </c>
       <c r="T4" s="9">
         <v>0</v>
       </c>
@@ -2488,9 +2485,6 @@
       <c r="D5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="9">
-        <v>0</v>
-      </c>
       <c r="Q5" s="9">
         <v>0</v>
       </c>
@@ -2516,9 +2510,6 @@
       </c>
       <c r="D6" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="E6" s="9">
-        <v>0</v>
       </c>
       <c r="T6" s="9">
         <v>0</v>
@@ -2878,9 +2869,7 @@
       <c r="D18" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="46">
-        <v>0</v>
-      </c>
+      <c r="E18" s="46"/>
       <c r="F18" s="46"/>
       <c r="G18" s="46"/>
       <c r="H18" s="46"/>
@@ -2936,9 +2925,6 @@
       <c r="D19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
       <c r="T19" s="1">
         <v>0</v>
       </c>
@@ -2958,9 +2944,6 @@
       </c>
       <c r="D20" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0</v>
       </c>
       <c r="T20" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
Calibrated value for TB n contact when there is diabetes
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="495" windowWidth="20370" windowHeight="7350" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="495" windowWidth="20370" windowHeight="7350" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -1944,7 +1949,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1979,7 +1984,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2193,8 +2198,8 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2233,7 +2238,7 @@
         <v>6.82</v>
       </c>
       <c r="E2" s="63">
-        <v>6.78</v>
+        <v>6.82</v>
       </c>
       <c r="F2" s="63">
         <v>7.85</v>
@@ -2325,11 +2330,11 @@
   </sheetPr>
   <dimension ref="A1:CA21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Polish off stacked economics plotting
Economics plotting now completely finished I think.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -2327,10 +2327,10 @@
   <dimension ref="A1:CA23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="BG2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="BQ21" sqref="BQ21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2632,7 +2632,7 @@
         <v>100</v>
       </c>
       <c r="BQ2" s="7">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2731,9 +2731,6 @@
       <c r="BI3" s="9">
         <v>75</v>
       </c>
-      <c r="BQ3" s="9">
-        <v>75</v>
-      </c>
     </row>
     <row r="4" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
@@ -2785,6 +2782,9 @@
       <c r="BN5" s="9">
         <v>75</v>
       </c>
+      <c r="BQ5" s="9">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
@@ -2806,6 +2806,9 @@
       <c r="BN6" s="9">
         <v>40</v>
       </c>
+      <c r="BQ6" s="9">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:69" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
@@ -2839,9 +2842,6 @@
       <c r="BJ7" s="11">
         <v>90</v>
       </c>
-      <c r="BQ7" s="11">
-        <v>90</v>
-      </c>
     </row>
     <row r="8" spans="1:69" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
@@ -2865,9 +2865,6 @@
       </c>
       <c r="AF8" s="13">
         <v>40</v>
-      </c>
-      <c r="BQ8" s="13">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -2963,9 +2960,6 @@
       </c>
       <c r="BC11" s="27">
         <v>85</v>
-      </c>
-      <c r="BQ11" s="13">
-        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:69" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -3012,9 +3006,6 @@
       <c r="BC12" s="27"/>
       <c r="BD12" s="13">
         <v>5</v>
-      </c>
-      <c r="BQ12" s="13">
-        <v>1.25</v>
       </c>
     </row>
     <row r="13" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -3239,6 +3230,9 @@
       </c>
       <c r="BL17" s="34">
         <v>100</v>
+      </c>
+      <c r="BQ17" s="34">
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:79" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -3354,6 +3348,9 @@
       <c r="BO19" s="54">
         <v>50</v>
       </c>
+      <c r="BQ19" s="54">
+        <v>40</v>
+      </c>
     </row>
     <row r="20" spans="1:79" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="51" t="s">
@@ -3373,6 +3370,9 @@
         <v>0</v>
       </c>
       <c r="BP20" s="54">
+        <v>50</v>
+      </c>
+      <c r="BQ20" s="54">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modify time-variant loading for demo params
Time-variant demographic parameters (such as comorbidity/risk-group
proportions) can now be loaded from Excel sheets.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="495" windowWidth="20370" windowHeight="7350" tabRatio="807" activeTab="1"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="58">
   <si>
     <t>parameter</t>
   </si>
@@ -194,7 +189,7 @@
     <t>scenario_14</t>
   </si>
   <si>
-    <t>age_breakpoints</t>
+    <t>demo_perc_diabetes</t>
   </si>
 </sst>
 </file>
@@ -1965,7 +1960,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2000,7 +1995,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2212,10 +2207,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2312,20 +2307,6 @@
       </c>
       <c r="H5">
         <v>280000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="37">
-        <v>5</v>
-      </c>
-      <c r="C6" s="29">
-        <v>15</v>
-      </c>
-      <c r="D6" s="29">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2358,13 +2339,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:CC24"/>
+  <dimension ref="A1:CC25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="AH2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BD3" sqref="BD3"/>
+      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3771,6 +3752,32 @@
       <c r="E24" s="49"/>
       <c r="BG24" s="34">
         <v>2010</v>
+      </c>
+    </row>
+    <row r="25" spans="1:81" x14ac:dyDescent="0.25">
+      <c r="A25" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="50">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF25" s="1">
+        <v>10</v>
+      </c>
+      <c r="AT25" s="1">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Time-variant diabetes prevalence for Fiji
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="495" windowWidth="20370" windowHeight="7350" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="495" windowWidth="20370" windowHeight="7350" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -1963,7 +1968,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1998,7 +2003,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2212,8 +2217,8 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2358,11 +2363,11 @@
   </sheetPr>
   <dimension ref="A1:CC25"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="AL2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
+      <selection pane="bottomRight" activeCell="BI25" sqref="BI25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3776,7 +3781,7 @@
         <v>57</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C25" s="2">
         <v>1</v>
@@ -3787,14 +3792,35 @@
       <c r="E25" s="50">
         <v>0</v>
       </c>
-      <c r="Y25" s="1">
+      <c r="K25" s="1">
         <v>0</v>
       </c>
-      <c r="AF25" s="1">
-        <v>10</v>
+      <c r="T25" s="1">
+        <v>0</v>
+      </c>
+      <c r="V25" s="1">
+        <v>7.7</v>
+      </c>
+      <c r="AI25" s="1">
+        <v>11.1</v>
+      </c>
+      <c r="AR25" s="1">
+        <v>16.5</v>
       </c>
       <c r="AT25" s="1">
-        <v>20</v>
+        <v>14.5</v>
+      </c>
+      <c r="AY25" s="1">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="BA25" s="1">
+        <v>15.6</v>
+      </c>
+      <c r="BC25" s="1">
+        <v>15.6</v>
+      </c>
+      <c r="BE25" s="1">
+        <v>15.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small adjustments of parameters for better epi cure fit
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -2218,7 +2218,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2254,7 +2254,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="59">
-        <v>7.93</v>
+        <v>7.91</v>
       </c>
       <c r="F2" s="59">
         <v>7.85</v>
@@ -2367,7 +2367,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="AL2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BI25" sqref="BI25"/>
+      <selection pane="bottomRight" activeCell="BD3" sqref="BD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2765,7 +2765,7 @@
       <c r="BB3" s="26"/>
       <c r="BC3" s="26"/>
       <c r="BD3" s="26">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="BE3" s="26"/>
       <c r="BH3" s="9">

</xml_diff>

<commit_message>
Changed scenarios to reflect table 2 in report
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -2364,10 +2364,10 @@
   <dimension ref="A1:CC25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="BB2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomRight" activeCell="BM24" sqref="BM24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2671,12 +2671,6 @@
       <c r="BC2" s="25"/>
       <c r="BD2" s="25"/>
       <c r="BE2" s="25"/>
-      <c r="BK2" s="7">
-        <v>100</v>
-      </c>
-      <c r="BS2" s="7">
-        <v>99</v>
-      </c>
     </row>
     <row r="3" spans="1:71" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
@@ -2774,6 +2768,12 @@
       <c r="BI3" s="9">
         <v>75</v>
       </c>
+      <c r="BK3" s="9">
+        <v>77.5</v>
+      </c>
+      <c r="BM3" s="9">
+        <v>77.5</v>
+      </c>
     </row>
     <row r="4" spans="1:71" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
@@ -2792,12 +2792,6 @@
       <c r="BD4" s="9">
         <v>0</v>
       </c>
-      <c r="BM4" s="9">
-        <v>50</v>
-      </c>
-      <c r="BS4" s="9">
-        <v>50</v>
-      </c>
     </row>
     <row r="5" spans="1:71" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -2822,11 +2816,11 @@
       <c r="BD5" s="9">
         <v>23.6</v>
       </c>
-      <c r="BN5" s="9">
-        <v>75</v>
-      </c>
-      <c r="BS5" s="9">
-        <v>20</v>
+      <c r="BL5" s="9">
+        <v>80</v>
+      </c>
+      <c r="BM5" s="9">
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:71" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2846,11 +2840,11 @@
       <c r="BD6" s="9">
         <v>0</v>
       </c>
-      <c r="BN6" s="9">
-        <v>40</v>
-      </c>
-      <c r="BS6" s="9">
-        <v>25</v>
+      <c r="BL6" s="9">
+        <v>80</v>
+      </c>
+      <c r="BM6" s="9">
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:71" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -2883,6 +2877,12 @@
         <v>85</v>
       </c>
       <c r="BJ7" s="11">
+        <v>90</v>
+      </c>
+      <c r="BK7" s="11">
+        <v>90</v>
+      </c>
+      <c r="BM7" s="11">
         <v>90</v>
       </c>
     </row>
@@ -3003,6 +3003,15 @@
       </c>
       <c r="BC11" s="27">
         <v>85</v>
+      </c>
+      <c r="BF11" s="13">
+        <v>91.1</v>
+      </c>
+      <c r="BG11" s="13">
+        <v>96</v>
+      </c>
+      <c r="BM11" s="13">
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:71" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -3049,6 +3058,15 @@
       <c r="BC12" s="27"/>
       <c r="BD12" s="13">
         <v>5</v>
+      </c>
+      <c r="BF12" s="13">
+        <v>1.6</v>
+      </c>
+      <c r="BG12" s="13">
+        <v>1.3</v>
+      </c>
+      <c r="BM12" s="13">
+        <v>1.3</v>
       </c>
     </row>
     <row r="13" spans="1:71" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -3271,11 +3289,11 @@
       <c r="BD17" s="34">
         <v>0</v>
       </c>
-      <c r="BL17" s="34">
+      <c r="BJ17" s="34">
         <v>100</v>
       </c>
-      <c r="BS17" s="34">
-        <v>40</v>
+      <c r="BM17" s="34">
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:81" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -3349,13 +3367,17 @@
       <c r="BF18" s="42">
         <v>100</v>
       </c>
-      <c r="BG18" s="42"/>
+      <c r="BG18" s="42">
+        <v>100</v>
+      </c>
       <c r="BH18" s="42"/>
       <c r="BI18" s="42"/>
       <c r="BJ18" s="42"/>
       <c r="BK18" s="42"/>
       <c r="BL18" s="42"/>
-      <c r="BM18" s="42"/>
+      <c r="BM18" s="42">
+        <v>100</v>
+      </c>
       <c r="BN18" s="42"/>
       <c r="BO18" s="42"/>
       <c r="BP18" s="42"/>
@@ -3445,21 +3467,23 @@
       <c r="BE19" s="42"/>
       <c r="BF19" s="42"/>
       <c r="BG19" s="42"/>
-      <c r="BH19" s="42"/>
-      <c r="BI19" s="42"/>
+      <c r="BH19" s="42">
+        <v>75</v>
+      </c>
+      <c r="BI19" s="42">
+        <v>75</v>
+      </c>
       <c r="BJ19" s="42"/>
       <c r="BK19" s="42"/>
       <c r="BL19" s="42"/>
-      <c r="BM19" s="42"/>
+      <c r="BM19" s="42">
+        <v>75</v>
+      </c>
       <c r="BN19" s="42"/>
       <c r="BO19" s="42"/>
       <c r="BP19" s="42"/>
-      <c r="BQ19" s="64">
-        <v>50</v>
-      </c>
-      <c r="BR19" s="64">
-        <v>75</v>
-      </c>
+      <c r="BQ19" s="64"/>
+      <c r="BR19" s="64"/>
       <c r="BS19" s="42"/>
       <c r="BT19" s="42"/>
       <c r="BU19" s="42"/>
@@ -3489,12 +3513,6 @@
       <c r="BD20" s="54">
         <v>0</v>
       </c>
-      <c r="BO20" s="54">
-        <v>50</v>
-      </c>
-      <c r="BS20" s="54">
-        <v>40</v>
-      </c>
     </row>
     <row r="21" spans="1:81" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="51" t="s">
@@ -3513,10 +3531,10 @@
       <c r="BD21" s="54">
         <v>0</v>
       </c>
-      <c r="BP21" s="54">
+      <c r="BK21" s="54">
         <v>50</v>
       </c>
-      <c r="BS21" s="54">
+      <c r="BM21" s="54">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Whoops, forgot changes with last commit
Forgot changes to Fiji country sheet.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="495" windowWidth="20370" windowHeight="7350" tabRatio="807" activeTab="1"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="63">
   <si>
     <t>parameter</t>
   </si>
@@ -204,6 +199,12 @@
   </si>
   <si>
     <t>transmission_modifier</t>
+  </si>
+  <si>
+    <t>scenario_12</t>
+  </si>
+  <si>
+    <t>program_perc_community_ipt</t>
   </si>
 </sst>
 </file>
@@ -2005,7 +2006,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2040,7 +2041,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2398,13 +2399,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BX30"/>
+  <dimension ref="A1:BX31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="BE2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BM25" sqref="BM25"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2436,7 +2437,7 @@
     <col min="69" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:69" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -2641,8 +2642,11 @@
       <c r="BP1" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="BQ1" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="2" spans="1:68" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:69" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>32</v>
       </c>
@@ -2710,7 +2714,7 @@
       <c r="BO2" s="65"/>
       <c r="BP2" s="65"/>
     </row>
-    <row r="3" spans="1:68" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:69" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>59</v>
       </c>
@@ -2778,7 +2782,7 @@
       </c>
       <c r="BP3" s="65"/>
     </row>
-    <row r="4" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>33</v>
       </c>
@@ -2880,7 +2884,7 @@
       <c r="BO4" s="66"/>
       <c r="BP4" s="66"/>
     </row>
-    <row r="5" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>34</v>
       </c>
@@ -2909,7 +2913,7 @@
       <c r="BO5" s="66"/>
       <c r="BP5" s="66"/>
     </row>
-    <row r="6" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>35</v>
       </c>
@@ -2948,7 +2952,7 @@
       <c r="BO6" s="66"/>
       <c r="BP6" s="66"/>
     </row>
-    <row r="7" spans="1:68" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>36</v>
       </c>
@@ -2981,42 +2985,41 @@
       <c r="BO7" s="66"/>
       <c r="BP7" s="66"/>
     </row>
-    <row r="8" spans="1:68" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="51" t="s">
+    <row r="8" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="44"/>
+      <c r="BD8" s="9">
+        <v>0</v>
+      </c>
+      <c r="BF8" s="66"/>
+      <c r="BG8" s="66"/>
+      <c r="BH8" s="66"/>
+      <c r="BI8" s="66"/>
+      <c r="BJ8" s="66"/>
+      <c r="BK8" s="66"/>
+      <c r="BL8" s="66"/>
+      <c r="BM8" s="66"/>
+      <c r="BN8" s="66"/>
+      <c r="BO8" s="66"/>
+      <c r="BP8" s="66"/>
+      <c r="BQ8" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:69" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="51" t="s">
         <v>56</v>
-      </c>
-      <c r="B8" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="52">
-        <v>1</v>
-      </c>
-      <c r="D8" s="52" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="53">
-        <v>0</v>
-      </c>
-      <c r="BD8" s="54">
-        <v>0</v>
-      </c>
-      <c r="BF8" s="67"/>
-      <c r="BG8" s="67"/>
-      <c r="BH8" s="67"/>
-      <c r="BI8" s="67"/>
-      <c r="BJ8" s="67"/>
-      <c r="BK8" s="67"/>
-      <c r="BL8" s="67"/>
-      <c r="BM8" s="67"/>
-      <c r="BN8" s="67">
-        <v>10</v>
-      </c>
-      <c r="BO8" s="67"/>
-      <c r="BP8" s="67"/>
-    </row>
-    <row r="9" spans="1:68" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="51" t="s">
-        <v>57</v>
       </c>
       <c r="B9" s="52" t="s">
         <v>4</v>
@@ -3041,13 +3044,15 @@
       <c r="BK9" s="67"/>
       <c r="BL9" s="67"/>
       <c r="BM9" s="67"/>
-      <c r="BN9" s="67"/>
+      <c r="BN9" s="67">
+        <v>10</v>
+      </c>
       <c r="BO9" s="67"/>
       <c r="BP9" s="67"/>
     </row>
-    <row r="10" spans="1:68" s="54" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:69" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" s="52" t="s">
         <v>4</v>
@@ -3076,120 +3081,116 @@
       <c r="BO10" s="67"/>
       <c r="BP10" s="67"/>
     </row>
-    <row r="11" spans="1:68" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:69" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="52">
+        <v>1</v>
+      </c>
+      <c r="D11" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="53">
+        <v>0</v>
+      </c>
+      <c r="BD11" s="54">
+        <v>0</v>
+      </c>
+      <c r="BF11" s="67"/>
+      <c r="BG11" s="67"/>
+      <c r="BH11" s="67"/>
+      <c r="BI11" s="67"/>
+      <c r="BJ11" s="67"/>
+      <c r="BK11" s="67"/>
+      <c r="BL11" s="67"/>
+      <c r="BM11" s="67"/>
+      <c r="BN11" s="67"/>
+      <c r="BO11" s="67"/>
+      <c r="BP11" s="67"/>
+    </row>
+    <row r="12" spans="1:69" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B12" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="10">
-        <v>1</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="45"/>
-      <c r="F11" s="11">
+      <c r="C12" s="10">
+        <v>1</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="45"/>
+      <c r="F12" s="11">
         <v>70</v>
       </c>
-      <c r="J11" s="11">
+      <c r="J12" s="11">
         <v>80</v>
       </c>
-      <c r="AD11" s="11">
+      <c r="AD12" s="11">
         <v>82</v>
       </c>
-      <c r="AQ11" s="11">
+      <c r="AQ12" s="11">
         <v>84</v>
       </c>
-      <c r="BC11" s="11">
+      <c r="BC12" s="11">
         <v>85</v>
       </c>
-      <c r="BF11" s="68"/>
-      <c r="BG11" s="68"/>
-      <c r="BH11" s="68"/>
-      <c r="BI11" s="68"/>
-      <c r="BJ11" s="68"/>
-      <c r="BK11" s="68"/>
-      <c r="BL11" s="68"/>
-      <c r="BM11" s="68"/>
-      <c r="BN11" s="68"/>
-      <c r="BO11" s="68"/>
-      <c r="BP11" s="68"/>
+      <c r="BF12" s="68"/>
+      <c r="BG12" s="68"/>
+      <c r="BH12" s="68"/>
+      <c r="BI12" s="68"/>
+      <c r="BJ12" s="68"/>
+      <c r="BK12" s="68"/>
+      <c r="BL12" s="68"/>
+      <c r="BM12" s="68"/>
+      <c r="BN12" s="68"/>
+      <c r="BO12" s="68"/>
+      <c r="BP12" s="68"/>
     </row>
-    <row r="12" spans="1:68" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+    <row r="13" spans="1:69" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B13" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="12">
-        <v>1</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="46"/>
-      <c r="H12" s="13">
+      <c r="C13" s="12">
+        <v>1</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="46"/>
+      <c r="H13" s="13">
         <v>30</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K13" s="13">
         <v>40</v>
       </c>
-      <c r="AF12" s="13">
+      <c r="AF13" s="13">
         <v>40</v>
       </c>
-      <c r="BF12" s="69"/>
-      <c r="BG12" s="69"/>
-      <c r="BH12" s="69"/>
-      <c r="BI12" s="69"/>
-      <c r="BJ12" s="69"/>
-      <c r="BK12" s="69"/>
-      <c r="BL12" s="69"/>
-      <c r="BM12" s="69"/>
-      <c r="BN12" s="69"/>
-      <c r="BO12" s="69"/>
-      <c r="BP12" s="69"/>
+      <c r="BF13" s="69"/>
+      <c r="BG13" s="69"/>
+      <c r="BH13" s="69"/>
+      <c r="BI13" s="69"/>
+      <c r="BJ13" s="69"/>
+      <c r="BK13" s="69"/>
+      <c r="BL13" s="69"/>
+      <c r="BM13" s="69"/>
+      <c r="BN13" s="69"/>
+      <c r="BO13" s="69"/>
+      <c r="BP13" s="69"/>
     </row>
-    <row r="13" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+    <row r="14" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
         <v>39</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="14">
-        <v>1</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="47"/>
-      <c r="V13" s="15">
-        <v>30</v>
-      </c>
-      <c r="AF13" s="15">
-        <v>40</v>
-      </c>
-      <c r="AP13" s="15">
-        <v>50</v>
-      </c>
-      <c r="BF13" s="70"/>
-      <c r="BG13" s="70"/>
-      <c r="BH13" s="70"/>
-      <c r="BI13" s="70"/>
-      <c r="BJ13" s="70"/>
-      <c r="BK13" s="70"/>
-      <c r="BL13" s="70"/>
-      <c r="BM13" s="70"/>
-      <c r="BN13" s="70"/>
-      <c r="BO13" s="70"/>
-      <c r="BP13" s="70"/>
-    </row>
-    <row r="14" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>40</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>4</v>
@@ -3201,14 +3202,14 @@
         <v>3</v>
       </c>
       <c r="E14" s="47"/>
-      <c r="I14" s="15">
-        <v>7</v>
-      </c>
-      <c r="AK14" s="15">
+      <c r="V14" s="15">
+        <v>30</v>
+      </c>
+      <c r="AF14" s="15">
+        <v>40</v>
+      </c>
+      <c r="AP14" s="15">
         <v>50</v>
-      </c>
-      <c r="AP14" s="15">
-        <v>70</v>
       </c>
       <c r="BF14" s="70"/>
       <c r="BG14" s="70"/>
@@ -3222,75 +3223,50 @@
       <c r="BO14" s="70"/>
       <c r="BP14" s="70"/>
     </row>
-    <row r="15" spans="1:68" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+    <row r="15" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="14">
+        <v>1</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="47"/>
+      <c r="I15" s="15">
+        <v>7</v>
+      </c>
+      <c r="AK15" s="15">
+        <v>50</v>
+      </c>
+      <c r="AP15" s="15">
+        <v>70</v>
+      </c>
+      <c r="BF15" s="70"/>
+      <c r="BG15" s="70"/>
+      <c r="BH15" s="70"/>
+      <c r="BI15" s="70"/>
+      <c r="BJ15" s="70"/>
+      <c r="BK15" s="70"/>
+      <c r="BL15" s="70"/>
+      <c r="BM15" s="70"/>
+      <c r="BN15" s="70"/>
+      <c r="BO15" s="70"/>
+      <c r="BP15" s="70"/>
+    </row>
+    <row r="16" spans="1:69" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="12">
-        <v>1</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="46"/>
-      <c r="I15" s="13">
-        <v>0</v>
-      </c>
-      <c r="V15" s="13">
-        <v>40</v>
-      </c>
-      <c r="AB15" s="13">
-        <v>65</v>
-      </c>
-      <c r="AK15" s="27"/>
-      <c r="AL15" s="27"/>
-      <c r="AM15" s="27"/>
-      <c r="AN15" s="27"/>
-      <c r="AO15" s="27"/>
-      <c r="AP15" s="27"/>
-      <c r="AQ15" s="27"/>
-      <c r="AR15" s="27"/>
-      <c r="AS15" s="27"/>
-      <c r="AT15" s="27"/>
-      <c r="AU15" s="27"/>
-      <c r="AV15" s="27"/>
-      <c r="AW15" s="27"/>
-      <c r="AX15" s="27"/>
-      <c r="AY15" s="27"/>
-      <c r="AZ15" s="27"/>
-      <c r="BA15" s="27"/>
-      <c r="BB15" s="27">
-        <v>93</v>
-      </c>
-      <c r="BC15" s="27">
-        <v>85</v>
-      </c>
-      <c r="BF15" s="69"/>
-      <c r="BG15" s="69">
-        <v>96</v>
-      </c>
-      <c r="BH15" s="69"/>
-      <c r="BI15" s="69"/>
-      <c r="BJ15" s="69"/>
-      <c r="BK15" s="69"/>
-      <c r="BL15" s="69"/>
-      <c r="BM15" s="69"/>
-      <c r="BN15" s="69"/>
-      <c r="BO15" s="69"/>
-      <c r="BP15" s="69"/>
-    </row>
-    <row r="16" spans="1:68" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>46</v>
-      </c>
       <c r="B16" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>3</v>
@@ -3300,10 +3276,10 @@
         <v>0</v>
       </c>
       <c r="V16" s="13">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="AB16" s="13">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="AK16" s="27"/>
       <c r="AL16" s="27"/>
@@ -3322,14 +3298,15 @@
       <c r="AY16" s="27"/>
       <c r="AZ16" s="27"/>
       <c r="BA16" s="27"/>
-      <c r="BB16" s="27"/>
-      <c r="BC16" s="27"/>
-      <c r="BD16" s="13">
-        <v>5</v>
+      <c r="BB16" s="27">
+        <v>93</v>
+      </c>
+      <c r="BC16" s="27">
+        <v>85</v>
       </c>
       <c r="BF16" s="69"/>
       <c r="BG16" s="69">
-        <v>1.3</v>
+        <v>96</v>
       </c>
       <c r="BH16" s="69"/>
       <c r="BI16" s="69"/>
@@ -3341,66 +3318,68 @@
       <c r="BO16" s="69"/>
       <c r="BP16" s="69"/>
     </row>
-    <row r="17" spans="1:76" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="23">
-        <v>1</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="48"/>
-      <c r="I17" s="24">
+    <row r="17" spans="1:76" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="12">
+        <v>3</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="46"/>
+      <c r="I17" s="13">
         <v>0</v>
       </c>
-      <c r="V17" s="24">
-        <v>15</v>
-      </c>
-      <c r="AB17" s="24">
-        <v>30</v>
-      </c>
-      <c r="AK17" s="28"/>
-      <c r="AL17" s="28"/>
-      <c r="AM17" s="28"/>
-      <c r="AN17" s="28"/>
-      <c r="AO17" s="28"/>
-      <c r="AP17" s="28"/>
-      <c r="AQ17" s="28"/>
-      <c r="AR17" s="28"/>
-      <c r="AS17" s="28"/>
-      <c r="AT17" s="28"/>
-      <c r="AU17" s="28"/>
-      <c r="AV17" s="28"/>
-      <c r="AW17" s="28"/>
-      <c r="AX17" s="28"/>
-      <c r="AY17" s="28"/>
-      <c r="AZ17" s="28"/>
-      <c r="BA17" s="28"/>
-      <c r="BB17" s="28"/>
-      <c r="BC17" s="28"/>
-      <c r="BD17" s="24">
-        <v>50</v>
-      </c>
-      <c r="BF17" s="71"/>
-      <c r="BG17" s="71"/>
-      <c r="BH17" s="71"/>
-      <c r="BI17" s="71"/>
-      <c r="BJ17" s="71"/>
-      <c r="BK17" s="71"/>
-      <c r="BL17" s="71"/>
-      <c r="BM17" s="71"/>
-      <c r="BN17" s="71"/>
-      <c r="BO17" s="71"/>
-      <c r="BP17" s="71"/>
+      <c r="V17" s="13">
+        <v>10</v>
+      </c>
+      <c r="AB17" s="13">
+        <v>8</v>
+      </c>
+      <c r="AK17" s="27"/>
+      <c r="AL17" s="27"/>
+      <c r="AM17" s="27"/>
+      <c r="AN17" s="27"/>
+      <c r="AO17" s="27"/>
+      <c r="AP17" s="27"/>
+      <c r="AQ17" s="27"/>
+      <c r="AR17" s="27"/>
+      <c r="AS17" s="27"/>
+      <c r="AT17" s="27"/>
+      <c r="AU17" s="27"/>
+      <c r="AV17" s="27"/>
+      <c r="AW17" s="27"/>
+      <c r="AX17" s="27"/>
+      <c r="AY17" s="27"/>
+      <c r="AZ17" s="27"/>
+      <c r="BA17" s="27"/>
+      <c r="BB17" s="27"/>
+      <c r="BC17" s="27"/>
+      <c r="BD17" s="13">
+        <v>5</v>
+      </c>
+      <c r="BF17" s="69"/>
+      <c r="BG17" s="69">
+        <v>1.3</v>
+      </c>
+      <c r="BH17" s="69"/>
+      <c r="BI17" s="69"/>
+      <c r="BJ17" s="69"/>
+      <c r="BK17" s="69"/>
+      <c r="BL17" s="69"/>
+      <c r="BM17" s="69"/>
+      <c r="BN17" s="69"/>
+      <c r="BO17" s="69"/>
+      <c r="BP17" s="69"/>
     </row>
     <row r="18" spans="1:76" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" s="23" t="s">
         <v>3</v>
@@ -3416,10 +3395,10 @@
         <v>0</v>
       </c>
       <c r="V18" s="24">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="AB18" s="24">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="AK18" s="28"/>
       <c r="AL18" s="28"/>
@@ -3441,7 +3420,7 @@
       <c r="BB18" s="28"/>
       <c r="BC18" s="28"/>
       <c r="BD18" s="24">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="BF18" s="71"/>
       <c r="BG18" s="71"/>
@@ -3455,66 +3434,66 @@
       <c r="BO18" s="71"/>
       <c r="BP18" s="71"/>
     </row>
-    <row r="19" spans="1:76" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="8">
-        <v>1</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="44"/>
-      <c r="I19" s="9">
+    <row r="19" spans="1:76" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="23">
+        <v>1</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="48"/>
+      <c r="I19" s="24">
         <v>0</v>
       </c>
-      <c r="V19" s="9">
-        <v>5</v>
-      </c>
-      <c r="AB19" s="9">
-        <v>15</v>
-      </c>
-      <c r="AK19" s="26"/>
-      <c r="AL19" s="26"/>
-      <c r="AM19" s="26"/>
-      <c r="AN19" s="26"/>
-      <c r="AO19" s="26"/>
-      <c r="AP19" s="26"/>
-      <c r="AQ19" s="26"/>
-      <c r="AR19" s="26"/>
-      <c r="AS19" s="26"/>
-      <c r="AT19" s="26"/>
-      <c r="AU19" s="26"/>
-      <c r="AV19" s="26"/>
-      <c r="AW19" s="26"/>
-      <c r="AX19" s="26"/>
-      <c r="AY19" s="26"/>
-      <c r="AZ19" s="26"/>
-      <c r="BA19" s="26"/>
-      <c r="BB19" s="26"/>
-      <c r="BC19" s="26"/>
-      <c r="BD19" s="9">
-        <v>30</v>
-      </c>
-      <c r="BF19" s="66"/>
-      <c r="BG19" s="66"/>
-      <c r="BH19" s="66"/>
-      <c r="BI19" s="66"/>
-      <c r="BJ19" s="66"/>
-      <c r="BK19" s="66"/>
-      <c r="BL19" s="66"/>
-      <c r="BM19" s="66"/>
-      <c r="BN19" s="66"/>
-      <c r="BO19" s="66"/>
-      <c r="BP19" s="66"/>
+      <c r="V19" s="24">
+        <v>55</v>
+      </c>
+      <c r="AB19" s="24">
+        <v>50</v>
+      </c>
+      <c r="AK19" s="28"/>
+      <c r="AL19" s="28"/>
+      <c r="AM19" s="28"/>
+      <c r="AN19" s="28"/>
+      <c r="AO19" s="28"/>
+      <c r="AP19" s="28"/>
+      <c r="AQ19" s="28"/>
+      <c r="AR19" s="28"/>
+      <c r="AS19" s="28"/>
+      <c r="AT19" s="28"/>
+      <c r="AU19" s="28"/>
+      <c r="AV19" s="28"/>
+      <c r="AW19" s="28"/>
+      <c r="AX19" s="28"/>
+      <c r="AY19" s="28"/>
+      <c r="AZ19" s="28"/>
+      <c r="BA19" s="28"/>
+      <c r="BB19" s="28"/>
+      <c r="BC19" s="28"/>
+      <c r="BD19" s="24">
+        <v>20</v>
+      </c>
+      <c r="BF19" s="71"/>
+      <c r="BG19" s="71"/>
+      <c r="BH19" s="71"/>
+      <c r="BI19" s="71"/>
+      <c r="BJ19" s="71"/>
+      <c r="BK19" s="71"/>
+      <c r="BL19" s="71"/>
+      <c r="BM19" s="71"/>
+      <c r="BN19" s="71"/>
+      <c r="BO19" s="71"/>
+      <c r="BP19" s="71"/>
     </row>
     <row r="20" spans="1:76" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>3</v>
@@ -3530,10 +3509,10 @@
         <v>0</v>
       </c>
       <c r="V20" s="9">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="AB20" s="9">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="AK20" s="26"/>
       <c r="AL20" s="26"/>
@@ -3555,7 +3534,7 @@
       <c r="BB20" s="26"/>
       <c r="BC20" s="26"/>
       <c r="BD20" s="9">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="BF20" s="66"/>
       <c r="BG20" s="66"/>
@@ -3569,153 +3548,118 @@
       <c r="BO20" s="66"/>
       <c r="BP20" s="66"/>
     </row>
-    <row r="21" spans="1:76" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
+    <row r="21" spans="1:76" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="8">
+        <v>1</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="44"/>
+      <c r="I21" s="9">
+        <v>0</v>
+      </c>
+      <c r="V21" s="9">
+        <v>65</v>
+      </c>
+      <c r="AB21" s="9">
+        <v>62</v>
+      </c>
+      <c r="AK21" s="26"/>
+      <c r="AL21" s="26"/>
+      <c r="AM21" s="26"/>
+      <c r="AN21" s="26"/>
+      <c r="AO21" s="26"/>
+      <c r="AP21" s="26"/>
+      <c r="AQ21" s="26"/>
+      <c r="AR21" s="26"/>
+      <c r="AS21" s="26"/>
+      <c r="AT21" s="26"/>
+      <c r="AU21" s="26"/>
+      <c r="AV21" s="26"/>
+      <c r="AW21" s="26"/>
+      <c r="AX21" s="26"/>
+      <c r="AY21" s="26"/>
+      <c r="AZ21" s="26"/>
+      <c r="BA21" s="26"/>
+      <c r="BB21" s="26"/>
+      <c r="BC21" s="26"/>
+      <c r="BD21" s="9">
+        <v>35</v>
+      </c>
+      <c r="BF21" s="66"/>
+      <c r="BG21" s="66"/>
+      <c r="BH21" s="66"/>
+      <c r="BI21" s="66"/>
+      <c r="BJ21" s="66"/>
+      <c r="BK21" s="66"/>
+      <c r="BL21" s="66"/>
+      <c r="BM21" s="66"/>
+      <c r="BN21" s="66"/>
+      <c r="BO21" s="66"/>
+      <c r="BP21" s="66"/>
+    </row>
+    <row r="22" spans="1:76" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="33">
-        <v>1</v>
-      </c>
-      <c r="D21" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="49"/>
-      <c r="AK21" s="35"/>
-      <c r="AL21" s="35"/>
-      <c r="AM21" s="35"/>
-      <c r="AN21" s="35"/>
-      <c r="AO21" s="35"/>
-      <c r="AP21" s="35"/>
-      <c r="AQ21" s="35"/>
-      <c r="AR21" s="35"/>
-      <c r="AS21" s="35"/>
-      <c r="AT21" s="35"/>
-      <c r="AU21" s="35"/>
-      <c r="AV21" s="35"/>
-      <c r="AW21" s="35"/>
-      <c r="AX21" s="35"/>
-      <c r="AY21" s="35"/>
-      <c r="AZ21" s="35"/>
-      <c r="BA21" s="35"/>
-      <c r="BB21" s="35"/>
-      <c r="BC21" s="35"/>
-      <c r="BD21" s="34">
+      <c r="B22" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="33">
+        <v>1</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="49"/>
+      <c r="AK22" s="35"/>
+      <c r="AL22" s="35"/>
+      <c r="AM22" s="35"/>
+      <c r="AN22" s="35"/>
+      <c r="AO22" s="35"/>
+      <c r="AP22" s="35"/>
+      <c r="AQ22" s="35"/>
+      <c r="AR22" s="35"/>
+      <c r="AS22" s="35"/>
+      <c r="AT22" s="35"/>
+      <c r="AU22" s="35"/>
+      <c r="AV22" s="35"/>
+      <c r="AW22" s="35"/>
+      <c r="AX22" s="35"/>
+      <c r="AY22" s="35"/>
+      <c r="AZ22" s="35"/>
+      <c r="BA22" s="35"/>
+      <c r="BB22" s="35"/>
+      <c r="BC22" s="35"/>
+      <c r="BD22" s="34">
         <v>0</v>
       </c>
-      <c r="BF21" s="72"/>
-      <c r="BG21" s="72"/>
-      <c r="BH21" s="72"/>
-      <c r="BI21" s="72"/>
-      <c r="BJ21" s="72">
+      <c r="BF22" s="72"/>
+      <c r="BG22" s="72"/>
+      <c r="BH22" s="72"/>
+      <c r="BI22" s="72"/>
+      <c r="BJ22" s="72">
         <v>100</v>
       </c>
-      <c r="BK21" s="72"/>
-      <c r="BL21" s="72"/>
-      <c r="BM21" s="72">
+      <c r="BK22" s="72"/>
+      <c r="BL22" s="72"/>
+      <c r="BM22" s="72">
         <v>100</v>
       </c>
-      <c r="BN21" s="72"/>
-      <c r="BO21" s="72"/>
-      <c r="BP21" s="72"/>
-    </row>
-    <row r="22" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="14">
-        <v>1</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="47"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="42"/>
-      <c r="P22" s="42"/>
-      <c r="Q22" s="42"/>
-      <c r="R22" s="42"/>
-      <c r="S22" s="42"/>
-      <c r="T22" s="42"/>
-      <c r="U22" s="42"/>
-      <c r="V22" s="42"/>
-      <c r="W22" s="42"/>
-      <c r="X22" s="42"/>
-      <c r="Y22" s="42"/>
-      <c r="Z22" s="42"/>
-      <c r="AA22" s="42"/>
-      <c r="AB22" s="42"/>
-      <c r="AC22" s="42"/>
-      <c r="AD22" s="42"/>
-      <c r="AE22" s="42"/>
-      <c r="AF22" s="42"/>
-      <c r="AG22" s="42"/>
-      <c r="AH22" s="42"/>
-      <c r="AI22" s="42"/>
-      <c r="AJ22" s="42"/>
-      <c r="AK22" s="42"/>
-      <c r="AL22" s="42"/>
-      <c r="AM22" s="42"/>
-      <c r="AN22" s="42"/>
-      <c r="AO22" s="42"/>
-      <c r="AP22" s="42"/>
-      <c r="AQ22" s="42"/>
-      <c r="AR22" s="42"/>
-      <c r="AS22" s="42"/>
-      <c r="AT22" s="42"/>
-      <c r="AU22" s="42"/>
-      <c r="AV22" s="42"/>
-      <c r="AW22" s="42"/>
-      <c r="AX22" s="42"/>
-      <c r="AY22" s="42"/>
-      <c r="AZ22" s="42"/>
-      <c r="BA22" s="42"/>
-      <c r="BB22" s="42"/>
-      <c r="BC22" s="42"/>
-      <c r="BD22" s="42">
-        <v>0</v>
-      </c>
-      <c r="BE22" s="42"/>
-      <c r="BF22" s="73">
-        <v>100</v>
-      </c>
-      <c r="BG22" s="73"/>
-      <c r="BH22" s="73"/>
-      <c r="BI22" s="73"/>
-      <c r="BJ22" s="73"/>
-      <c r="BK22" s="73"/>
-      <c r="BL22" s="73"/>
-      <c r="BM22" s="73">
-        <v>100</v>
-      </c>
-      <c r="BN22" s="73"/>
-      <c r="BO22" s="73"/>
-      <c r="BP22" s="73"/>
-      <c r="BQ22" s="42"/>
-      <c r="BR22" s="42"/>
-      <c r="BS22" s="42"/>
-      <c r="BT22" s="42"/>
-      <c r="BU22" s="42"/>
-      <c r="BV22" s="42"/>
-      <c r="BW22" s="42"/>
-      <c r="BX22" s="42"/>
+      <c r="BN22" s="72"/>
+      <c r="BO22" s="72"/>
+      <c r="BP22" s="72"/>
     </row>
     <row r="23" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>3</v>
@@ -3726,9 +3670,7 @@
       <c r="D23" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="47">
-        <v>0</v>
-      </c>
+      <c r="E23" s="47"/>
       <c r="F23" s="42"/>
       <c r="G23" s="42"/>
       <c r="H23" s="42"/>
@@ -3783,19 +3725,17 @@
         <v>0</v>
       </c>
       <c r="BE23" s="42"/>
-      <c r="BF23" s="73"/>
+      <c r="BF23" s="73">
+        <v>100</v>
+      </c>
       <c r="BG23" s="73"/>
-      <c r="BH23" s="73">
-        <v>17</v>
-      </c>
-      <c r="BI23" s="73">
-        <v>70</v>
-      </c>
+      <c r="BH23" s="73"/>
+      <c r="BI23" s="73"/>
       <c r="BJ23" s="73"/>
       <c r="BK23" s="73"/>
       <c r="BL23" s="73"/>
       <c r="BM23" s="73">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="BN23" s="73"/>
       <c r="BO23" s="73"/>
@@ -3809,38 +3749,105 @@
       <c r="BW23" s="42"/>
       <c r="BX23" s="42"/>
     </row>
-    <row r="24" spans="1:76" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="52" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="52">
-        <v>1</v>
-      </c>
-      <c r="D24" s="52" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="53"/>
-      <c r="BD24" s="54">
+    <row r="24" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="14">
+        <v>1</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="47">
         <v>0</v>
       </c>
-      <c r="BF24" s="67"/>
-      <c r="BG24" s="67"/>
-      <c r="BH24" s="67"/>
-      <c r="BI24" s="67"/>
-      <c r="BJ24" s="67"/>
-      <c r="BK24" s="67"/>
-      <c r="BL24" s="67"/>
-      <c r="BM24" s="67"/>
-      <c r="BN24" s="67"/>
-      <c r="BO24" s="67"/>
-      <c r="BP24" s="67"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="42"/>
+      <c r="Q24" s="42"/>
+      <c r="R24" s="42"/>
+      <c r="S24" s="42"/>
+      <c r="T24" s="42"/>
+      <c r="U24" s="42"/>
+      <c r="V24" s="42"/>
+      <c r="W24" s="42"/>
+      <c r="X24" s="42"/>
+      <c r="Y24" s="42"/>
+      <c r="Z24" s="42"/>
+      <c r="AA24" s="42"/>
+      <c r="AB24" s="42"/>
+      <c r="AC24" s="42"/>
+      <c r="AD24" s="42"/>
+      <c r="AE24" s="42"/>
+      <c r="AF24" s="42"/>
+      <c r="AG24" s="42"/>
+      <c r="AH24" s="42"/>
+      <c r="AI24" s="42"/>
+      <c r="AJ24" s="42"/>
+      <c r="AK24" s="42"/>
+      <c r="AL24" s="42"/>
+      <c r="AM24" s="42"/>
+      <c r="AN24" s="42"/>
+      <c r="AO24" s="42"/>
+      <c r="AP24" s="42"/>
+      <c r="AQ24" s="42"/>
+      <c r="AR24" s="42"/>
+      <c r="AS24" s="42"/>
+      <c r="AT24" s="42"/>
+      <c r="AU24" s="42"/>
+      <c r="AV24" s="42"/>
+      <c r="AW24" s="42"/>
+      <c r="AX24" s="42"/>
+      <c r="AY24" s="42"/>
+      <c r="AZ24" s="42"/>
+      <c r="BA24" s="42"/>
+      <c r="BB24" s="42"/>
+      <c r="BC24" s="42"/>
+      <c r="BD24" s="42">
+        <v>0</v>
+      </c>
+      <c r="BE24" s="42"/>
+      <c r="BF24" s="73"/>
+      <c r="BG24" s="73"/>
+      <c r="BH24" s="73">
+        <v>17</v>
+      </c>
+      <c r="BI24" s="73">
+        <v>70</v>
+      </c>
+      <c r="BJ24" s="73"/>
+      <c r="BK24" s="73"/>
+      <c r="BL24" s="73"/>
+      <c r="BM24" s="73">
+        <v>70</v>
+      </c>
+      <c r="BN24" s="73"/>
+      <c r="BO24" s="73"/>
+      <c r="BP24" s="73"/>
+      <c r="BQ24" s="42"/>
+      <c r="BR24" s="42"/>
+      <c r="BS24" s="42"/>
+      <c r="BT24" s="42"/>
+      <c r="BU24" s="42"/>
+      <c r="BV24" s="42"/>
+      <c r="BW24" s="42"/>
+      <c r="BX24" s="42"/>
     </row>
     <row r="25" spans="1:76" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="51" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="52" t="s">
         <v>3</v>
@@ -3860,322 +3867,320 @@
       <c r="BH25" s="67"/>
       <c r="BI25" s="67"/>
       <c r="BJ25" s="67"/>
-      <c r="BK25" s="67">
-        <v>50</v>
-      </c>
+      <c r="BK25" s="67"/>
       <c r="BL25" s="67"/>
-      <c r="BM25" s="67">
-        <v>50</v>
-      </c>
+      <c r="BM25" s="67"/>
       <c r="BN25" s="67"/>
       <c r="BO25" s="67"/>
       <c r="BP25" s="67"/>
     </row>
-    <row r="26" spans="1:76" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="55" t="s">
+    <row r="26" spans="1:76" s="54" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="52">
+        <v>1</v>
+      </c>
+      <c r="D26" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="53"/>
+      <c r="BD26" s="54">
+        <v>0</v>
+      </c>
+      <c r="BF26" s="67"/>
+      <c r="BG26" s="67"/>
+      <c r="BH26" s="67"/>
+      <c r="BI26" s="67"/>
+      <c r="BJ26" s="67"/>
+      <c r="BK26" s="67">
+        <v>50</v>
+      </c>
+      <c r="BL26" s="67"/>
+      <c r="BM26" s="67">
+        <v>50</v>
+      </c>
+      <c r="BN26" s="67"/>
+      <c r="BO26" s="67"/>
+      <c r="BP26" s="67"/>
+    </row>
+    <row r="27" spans="1:76" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="56" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="56">
-        <v>1</v>
-      </c>
-      <c r="D26" s="56" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" s="57">
+      <c r="B27" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="56">
+        <v>1</v>
+      </c>
+      <c r="D27" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="57">
         <v>4.3099999999999996</v>
       </c>
-      <c r="F26" s="58">
+      <c r="F27" s="58">
         <v>4.84</v>
       </c>
-      <c r="G26" s="58">
+      <c r="G27" s="58">
         <v>5.44</v>
       </c>
-      <c r="H26" s="58">
+      <c r="H27" s="58">
         <v>6.11</v>
       </c>
-      <c r="I26" s="58">
+      <c r="I27" s="58">
         <v>6.86</v>
       </c>
-      <c r="J26" s="58">
+      <c r="J27" s="58">
         <v>7.7</v>
       </c>
-      <c r="K26" s="58">
+      <c r="K27" s="58">
         <v>8.68</v>
       </c>
-      <c r="L26" s="58">
+      <c r="L27" s="58">
         <v>9.0399999999999991</v>
       </c>
-      <c r="M26" s="58">
+      <c r="M27" s="58">
         <v>9.41</v>
       </c>
-      <c r="N26" s="58">
+      <c r="N27" s="58">
         <v>11.48</v>
       </c>
-      <c r="O26" s="58">
+      <c r="O27" s="58">
         <v>12.75</v>
       </c>
-      <c r="P26" s="58">
+      <c r="P27" s="58">
         <v>14.6</v>
       </c>
-      <c r="Q26" s="58">
+      <c r="Q27" s="58">
         <v>16.5</v>
       </c>
-      <c r="R26" s="58">
+      <c r="R27" s="58">
         <v>18.38</v>
       </c>
-      <c r="S26" s="58">
+      <c r="S27" s="58">
         <v>19.670000000000002</v>
       </c>
-      <c r="T26" s="58">
+      <c r="T27" s="58">
         <v>20.87</v>
       </c>
-      <c r="U26" s="58">
+      <c r="U27" s="58">
         <v>22.5</v>
       </c>
-      <c r="V26" s="58">
+      <c r="V27" s="58">
         <v>25.9</v>
       </c>
-      <c r="W26" s="58">
+      <c r="W27" s="58">
         <v>28.8</v>
       </c>
-      <c r="X26" s="58">
+      <c r="X27" s="58">
         <v>30.8</v>
       </c>
-      <c r="Y26" s="58">
+      <c r="Y27" s="58">
         <v>32.9</v>
       </c>
-      <c r="Z26" s="58">
+      <c r="Z27" s="58">
         <v>34.6</v>
       </c>
-      <c r="AA26" s="58">
+      <c r="AA27" s="58">
         <v>36.1</v>
       </c>
-      <c r="AB26" s="58">
+      <c r="AB27" s="58">
         <v>36.799999999999997</v>
       </c>
-      <c r="AC26" s="58">
+      <c r="AC27" s="58">
         <v>38.9</v>
       </c>
-      <c r="AD26" s="58">
+      <c r="AD27" s="58">
         <v>43.4</v>
       </c>
-      <c r="AE26" s="58">
+      <c r="AE27" s="58">
         <v>46.1</v>
       </c>
-      <c r="AF26" s="58">
+      <c r="AF27" s="58">
         <v>49.9</v>
       </c>
-      <c r="AG26" s="58">
+      <c r="AG27" s="58">
         <v>53.1</v>
       </c>
-      <c r="AH26" s="58">
+      <c r="AH27" s="58">
         <v>55.7</v>
       </c>
-      <c r="AI26" s="58">
+      <c r="AI27" s="58">
         <v>58.6</v>
       </c>
-      <c r="AJ26" s="58">
+      <c r="AJ27" s="58">
         <v>59.1</v>
       </c>
-      <c r="AK26" s="58">
+      <c r="AK27" s="58">
         <v>60.4</v>
       </c>
-      <c r="AL26" s="58">
+      <c r="AL27" s="58">
         <v>62.2</v>
       </c>
-      <c r="AM26" s="58">
+      <c r="AM27" s="58">
         <v>64.3</v>
       </c>
-      <c r="AN26" s="58">
+      <c r="AN27" s="58">
         <v>68</v>
       </c>
-      <c r="AO26" s="58">
+      <c r="AO27" s="58">
         <v>69.3</v>
       </c>
-      <c r="AP26" s="58">
+      <c r="AP27" s="58">
         <v>70.099999999999994</v>
       </c>
-      <c r="AQ26" s="58">
+      <c r="AQ27" s="58">
         <v>73.099999999999994</v>
       </c>
-      <c r="AR26" s="58">
+      <c r="AR27" s="58">
         <v>73.599999999999994</v>
       </c>
-      <c r="AS26" s="58">
+      <c r="AS27" s="58">
         <v>76.7</v>
       </c>
-      <c r="AT26" s="58">
+      <c r="AT27" s="58">
         <v>78.900000000000006</v>
       </c>
-      <c r="AU26" s="58">
+      <c r="AU27" s="58">
         <v>80.8</v>
       </c>
-      <c r="AV26" s="58">
+      <c r="AV27" s="58">
         <v>82.8</v>
       </c>
-      <c r="AW26" s="58">
+      <c r="AW27" s="58">
         <v>86.7</v>
       </c>
-      <c r="AX26" s="58">
+      <c r="AX27" s="58">
         <v>93.4</v>
       </c>
-      <c r="AY26" s="58">
+      <c r="AY27" s="58">
         <v>96.5</v>
       </c>
-      <c r="AZ26" s="58">
+      <c r="AZ27" s="58">
         <v>100</v>
       </c>
-      <c r="BA26" s="58">
+      <c r="BA27" s="58">
         <v>107.3</v>
       </c>
-      <c r="BB26" s="58">
+      <c r="BB27" s="58">
         <v>110.9</v>
       </c>
-      <c r="BC26" s="58">
+      <c r="BC27" s="58">
         <v>114.2</v>
       </c>
-      <c r="BD26" s="58">
+      <c r="BD27" s="58">
         <v>114.8</v>
       </c>
-      <c r="BE26" s="58">
+      <c r="BE27" s="58">
         <v>116.4</v>
       </c>
-      <c r="BF26" s="74"/>
-      <c r="BG26" s="74"/>
-      <c r="BH26" s="74"/>
-      <c r="BI26" s="74"/>
-      <c r="BJ26" s="74"/>
-      <c r="BK26" s="74"/>
-      <c r="BL26" s="74"/>
-      <c r="BM26" s="74"/>
-      <c r="BN26" s="74"/>
-      <c r="BO26" s="74"/>
-      <c r="BP26" s="74"/>
+      <c r="BF27" s="74"/>
+      <c r="BG27" s="74"/>
+      <c r="BH27" s="74"/>
+      <c r="BI27" s="74"/>
+      <c r="BJ27" s="74"/>
+      <c r="BK27" s="74"/>
+      <c r="BL27" s="74"/>
+      <c r="BM27" s="74"/>
+      <c r="BN27" s="74"/>
+      <c r="BO27" s="74"/>
+      <c r="BP27" s="74"/>
     </row>
-    <row r="27" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
+    <row r="28" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="14">
-        <v>1</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" s="47">
-        <v>1</v>
-      </c>
-      <c r="F27" s="15">
-        <v>1</v>
-      </c>
-      <c r="G27" s="15">
-        <v>1</v>
-      </c>
-      <c r="H27" s="15">
-        <v>1</v>
-      </c>
-      <c r="I27" s="15">
-        <v>1</v>
-      </c>
-      <c r="J27" s="15">
-        <v>1</v>
-      </c>
-      <c r="K27" s="15">
-        <v>1</v>
-      </c>
-      <c r="L27" s="15">
-        <v>1</v>
-      </c>
-      <c r="M27" s="15">
-        <v>1</v>
-      </c>
-      <c r="N27" s="15">
-        <v>1</v>
-      </c>
-      <c r="O27" s="15">
-        <v>1</v>
-      </c>
-      <c r="P27" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q27" s="15">
-        <v>1</v>
-      </c>
-      <c r="R27" s="15">
-        <v>1</v>
-      </c>
-      <c r="S27" s="15">
-        <v>1</v>
-      </c>
-      <c r="T27" s="15">
-        <v>1</v>
-      </c>
-      <c r="U27" s="15">
-        <v>1</v>
-      </c>
-      <c r="V27" s="15">
+      <c r="B28" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="14">
+        <v>1</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="47">
+        <v>1</v>
+      </c>
+      <c r="F28" s="15">
+        <v>1</v>
+      </c>
+      <c r="G28" s="15">
+        <v>1</v>
+      </c>
+      <c r="H28" s="15">
+        <v>1</v>
+      </c>
+      <c r="I28" s="15">
+        <v>1</v>
+      </c>
+      <c r="J28" s="15">
+        <v>1</v>
+      </c>
+      <c r="K28" s="15">
+        <v>1</v>
+      </c>
+      <c r="L28" s="15">
+        <v>1</v>
+      </c>
+      <c r="M28" s="15">
+        <v>1</v>
+      </c>
+      <c r="N28" s="15">
+        <v>1</v>
+      </c>
+      <c r="O28" s="15">
+        <v>1</v>
+      </c>
+      <c r="P28" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="15">
+        <v>1</v>
+      </c>
+      <c r="R28" s="15">
+        <v>1</v>
+      </c>
+      <c r="S28" s="15">
+        <v>1</v>
+      </c>
+      <c r="T28" s="15">
+        <v>1</v>
+      </c>
+      <c r="U28" s="15">
+        <v>1</v>
+      </c>
+      <c r="V28" s="15">
         <v>1.1000000000000001</v>
       </c>
-      <c r="BA27" s="15">
+      <c r="BA28" s="15">
         <v>3.11</v>
       </c>
-      <c r="BF27" s="70"/>
-      <c r="BG27" s="70"/>
-      <c r="BH27" s="70"/>
-      <c r="BI27" s="70"/>
-      <c r="BJ27" s="70"/>
-      <c r="BK27" s="70"/>
-      <c r="BL27" s="70"/>
-      <c r="BM27" s="70"/>
-      <c r="BN27" s="70"/>
-      <c r="BO27" s="70"/>
-      <c r="BP27" s="70"/>
-    </row>
-    <row r="28" spans="1:76" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" s="63"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="49"/>
-      <c r="BF28" s="72"/>
-      <c r="BG28" s="72"/>
-      <c r="BH28" s="72"/>
-      <c r="BI28" s="72"/>
-      <c r="BJ28" s="72"/>
-      <c r="BK28" s="72"/>
-      <c r="BL28" s="72"/>
-      <c r="BM28" s="72"/>
-      <c r="BN28" s="72"/>
-      <c r="BO28" s="72"/>
-      <c r="BP28" s="72"/>
+      <c r="BF28" s="70"/>
+      <c r="BG28" s="70"/>
+      <c r="BH28" s="70"/>
+      <c r="BI28" s="70"/>
+      <c r="BJ28" s="70"/>
+      <c r="BK28" s="70"/>
+      <c r="BL28" s="70"/>
+      <c r="BM28" s="70"/>
+      <c r="BN28" s="70"/>
+      <c r="BO28" s="70"/>
+      <c r="BP28" s="70"/>
     </row>
     <row r="29" spans="1:76" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" s="63" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="33">
-        <v>1</v>
-      </c>
-      <c r="D29" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="E29" s="49">
-        <v>1</v>
-      </c>
-      <c r="BD29" s="34">
-        <v>1</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="B29" s="63"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="49"/>
       <c r="BF29" s="72"/>
       <c r="BG29" s="72"/>
       <c r="BH29" s="72"/>
@@ -4186,101 +4191,132 @@
       <c r="BM29" s="72"/>
       <c r="BN29" s="72"/>
       <c r="BO29" s="72"/>
-      <c r="BP29" s="72">
+      <c r="BP29" s="72"/>
+    </row>
+    <row r="30" spans="1:76" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="33">
+        <v>1</v>
+      </c>
+      <c r="D30" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="49">
+        <v>1</v>
+      </c>
+      <c r="BD30" s="34">
+        <v>1</v>
+      </c>
+      <c r="BF30" s="72"/>
+      <c r="BG30" s="72"/>
+      <c r="BH30" s="72"/>
+      <c r="BI30" s="72"/>
+      <c r="BJ30" s="72"/>
+      <c r="BK30" s="72"/>
+      <c r="BL30" s="72"/>
+      <c r="BM30" s="72"/>
+      <c r="BN30" s="72"/>
+      <c r="BO30" s="72"/>
+      <c r="BP30" s="72">
         <v>0.01</v>
       </c>
     </row>
-    <row r="30" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="A30" s="21" t="s">
+    <row r="31" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A31" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="2">
-        <v>1</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30" s="50">
+      <c r="B31" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="50">
         <v>0</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K31" s="1">
         <v>0</v>
       </c>
-      <c r="T30" s="1">
+      <c r="T31" s="1">
         <v>0</v>
       </c>
-      <c r="V30" s="1">
+      <c r="V31" s="1">
         <v>7.7</v>
       </c>
-      <c r="AI30" s="1">
+      <c r="AI31" s="1">
         <v>11.1</v>
       </c>
-      <c r="AR30" s="1">
+      <c r="AR31" s="1">
         <v>16.5</v>
       </c>
-      <c r="AT30" s="1">
+      <c r="AT31" s="1">
         <v>14.5</v>
       </c>
-      <c r="AY30" s="1">
+      <c r="AY31" s="1">
         <v>16.100000000000001</v>
       </c>
-      <c r="BA30" s="1">
+      <c r="BA31" s="1">
         <v>15.6</v>
       </c>
-      <c r="BC30" s="1">
+      <c r="BC31" s="1">
         <v>15.6</v>
       </c>
-      <c r="BE30" s="1">
+      <c r="BE31" s="1">
         <v>15.6</v>
       </c>
-      <c r="BF30" s="75"/>
-      <c r="BG30" s="75"/>
-      <c r="BH30" s="75"/>
-      <c r="BI30" s="75"/>
-      <c r="BJ30" s="75"/>
-      <c r="BK30" s="75"/>
-      <c r="BL30" s="75"/>
-      <c r="BM30" s="75"/>
-      <c r="BN30" s="75"/>
-      <c r="BO30" s="75"/>
-      <c r="BP30" s="75"/>
+      <c r="BF31" s="75"/>
+      <c r="BG31" s="75"/>
+      <c r="BH31" s="75"/>
+      <c r="BI31" s="75"/>
+      <c r="BJ31" s="75"/>
+      <c r="BK31" s="75"/>
+      <c r="BL31" s="75"/>
+      <c r="BM31" s="75"/>
+      <c r="BN31" s="75"/>
+      <c r="BO31" s="75"/>
+      <c r="BP31" s="75"/>
     </row>
   </sheetData>
-  <dataValidations xWindow="382" yWindow="552" count="5">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF21:BG21 F5:BG7">
+  <dataValidations disablePrompts="1" xWindow="382" yWindow="552" count="5">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF22:BG22 F5:BG8">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:D1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11:BG20 F21:BE21 F2:BG4">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F12:BG21 F22:BE22 F2:BG4">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C30:C1048576 C2:C27">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C31:C1048576 C2:C28">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Leave blank" sqref="B28:D29"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Leave blank" sqref="B29:D30"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="382" yWindow="552" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" xWindow="382" yWindow="552" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B7 B11:B21</xm:sqref>
+          <xm:sqref>B2:B8 B12:B22</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time-variant?" prompt="If no, the most recent value will be selected.">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D30:D1048576 D2:D27</xm:sqref>
+          <xm:sqref>D31:D1048576 D2:D28</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Remove some unnecessary time variants from Fiji
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="59">
   <si>
     <t>parameter</t>
   </si>
@@ -157,18 +157,6 @@
   </si>
   <si>
     <t>program_perc_treatment_death</t>
-  </si>
-  <si>
-    <t>program_perc_treatment_success_mdr</t>
-  </si>
-  <si>
-    <t>program_perc_treatment_death_mdr</t>
-  </si>
-  <si>
-    <t>program_perc_treatment_success_xdr</t>
-  </si>
-  <si>
-    <t>program_perc_treatment_death_xdr</t>
   </si>
   <si>
     <t>epi_rr_diabetes</t>
@@ -314,7 +302,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -383,12 +371,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1180,7 +1162,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1203,27 +1185,23 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1231,24 +1209,23 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1256,7 +1233,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1268,16 +1245,13 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2261,43 +2235,43 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.5703125" style="30" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="37" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="29"/>
-    <col min="6" max="6" width="13.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="29"/>
+    <col min="1" max="1" width="51.5703125" style="26" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="33" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="25"/>
+    <col min="6" max="6" width="13.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="31" t="s">
+      <c r="B1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="27" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="59">
+      <c r="B2" s="54">
         <v>7.55</v>
       </c>
-      <c r="F2" s="59">
+      <c r="F2" s="54">
         <v>7.55</v>
       </c>
-      <c r="G2" s="59">
+      <c r="G2" s="54">
         <v>7.85</v>
       </c>
       <c r="H2">
@@ -2305,16 +2279,16 @@
       </c>
     </row>
     <row r="3" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="60">
+      <c r="B3" s="55">
         <v>0.22</v>
       </c>
-      <c r="F3" s="60">
+      <c r="F3" s="55">
         <v>0.22</v>
       </c>
-      <c r="G3" s="60">
+      <c r="G3" s="55">
         <v>0.22</v>
       </c>
       <c r="H3">
@@ -2322,16 +2296,16 @@
       </c>
     </row>
     <row r="4" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="61">
+      <c r="B4" s="56">
         <v>1865</v>
       </c>
-      <c r="F4" s="61">
+      <c r="F4" s="56">
         <v>1865</v>
       </c>
-      <c r="G4" s="61">
+      <c r="G4" s="56">
         <v>1865</v>
       </c>
       <c r="H4">
@@ -2339,16 +2313,16 @@
       </c>
     </row>
     <row r="5" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="62">
+      <c r="B5" s="57">
         <v>190000</v>
       </c>
-      <c r="F5" s="62">
+      <c r="F5" s="57">
         <v>190000</v>
       </c>
-      <c r="G5" s="62">
+      <c r="G5" s="57">
         <v>190000</v>
       </c>
       <c r="H5">
@@ -2356,16 +2330,16 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="37">
+      <c r="A6" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="33">
         <v>5</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="25">
         <v>15</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="25">
         <v>25</v>
       </c>
     </row>
@@ -2399,13 +2373,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BX31"/>
+  <dimension ref="A1:BX27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="BB2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BL22" sqref="BL22"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2413,7 +2387,7 @@
     <col min="1" max="1" width="56" style="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11" style="50" customWidth="1"/>
+    <col min="5" max="5" width="11" style="45" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.42578125" style="1" customWidth="1"/>
     <col min="8" max="9" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -2643,7 +2617,7 @@
         <v>27</v>
       </c>
       <c r="BQ1" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:69" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2659,64 +2633,64 @@
       <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="43"/>
+      <c r="E2" s="39"/>
       <c r="H2" s="7">
         <v>0</v>
       </c>
       <c r="J2" s="7">
         <v>25</v>
       </c>
-      <c r="V2" s="25"/>
-      <c r="W2" s="25"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="25"/>
-      <c r="Z2" s="25"/>
-      <c r="AA2" s="25"/>
-      <c r="AB2" s="25"/>
-      <c r="AC2" s="25"/>
-      <c r="AD2" s="25"/>
-      <c r="AE2" s="25"/>
-      <c r="AF2" s="25"/>
-      <c r="AG2" s="25"/>
-      <c r="AH2" s="25"/>
-      <c r="AI2" s="25"/>
-      <c r="AJ2" s="25"/>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
-      <c r="AM2" s="25"/>
-      <c r="AN2" s="25"/>
-      <c r="AO2" s="25"/>
-      <c r="AP2" s="25"/>
-      <c r="AQ2" s="25"/>
-      <c r="AR2" s="25"/>
-      <c r="AS2" s="25"/>
-      <c r="AT2" s="25"/>
-      <c r="AU2" s="25"/>
-      <c r="AV2" s="25"/>
-      <c r="AW2" s="25"/>
-      <c r="AX2" s="25"/>
-      <c r="AY2" s="25"/>
-      <c r="AZ2" s="25"/>
-      <c r="BA2" s="25"/>
-      <c r="BB2" s="25"/>
-      <c r="BC2" s="25"/>
-      <c r="BD2" s="25"/>
-      <c r="BE2" s="25"/>
-      <c r="BF2" s="65"/>
-      <c r="BG2" s="65"/>
-      <c r="BH2" s="65"/>
-      <c r="BI2" s="65"/>
-      <c r="BJ2" s="65"/>
-      <c r="BK2" s="65"/>
-      <c r="BL2" s="65"/>
-      <c r="BM2" s="65"/>
-      <c r="BN2" s="65"/>
-      <c r="BO2" s="65"/>
-      <c r="BP2" s="65"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="22"/>
+      <c r="AA2" s="22"/>
+      <c r="AB2" s="22"/>
+      <c r="AC2" s="22"/>
+      <c r="AD2" s="22"/>
+      <c r="AE2" s="22"/>
+      <c r="AF2" s="22"/>
+      <c r="AG2" s="22"/>
+      <c r="AH2" s="22"/>
+      <c r="AI2" s="22"/>
+      <c r="AJ2" s="22"/>
+      <c r="AK2" s="22"/>
+      <c r="AL2" s="22"/>
+      <c r="AM2" s="22"/>
+      <c r="AN2" s="22"/>
+      <c r="AO2" s="22"/>
+      <c r="AP2" s="22"/>
+      <c r="AQ2" s="22"/>
+      <c r="AR2" s="22"/>
+      <c r="AS2" s="22"/>
+      <c r="AT2" s="22"/>
+      <c r="AU2" s="22"/>
+      <c r="AV2" s="22"/>
+      <c r="AW2" s="22"/>
+      <c r="AX2" s="22"/>
+      <c r="AY2" s="22"/>
+      <c r="AZ2" s="22"/>
+      <c r="BA2" s="22"/>
+      <c r="BB2" s="22"/>
+      <c r="BC2" s="22"/>
+      <c r="BD2" s="22"/>
+      <c r="BE2" s="22"/>
+      <c r="BF2" s="60"/>
+      <c r="BG2" s="60"/>
+      <c r="BH2" s="60"/>
+      <c r="BI2" s="60"/>
+      <c r="BJ2" s="60"/>
+      <c r="BK2" s="60"/>
+      <c r="BL2" s="60"/>
+      <c r="BM2" s="60"/>
+      <c r="BN2" s="60"/>
+      <c r="BO2" s="60"/>
+      <c r="BP2" s="60"/>
     </row>
     <row r="3" spans="1:69" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>4</v>
@@ -2727,60 +2701,60 @@
       <c r="D3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="43">
+      <c r="E3" s="39">
         <v>0</v>
       </c>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
-      <c r="X3" s="64"/>
-      <c r="Y3" s="64"/>
-      <c r="Z3" s="64"/>
-      <c r="AA3" s="64"/>
-      <c r="AB3" s="64"/>
-      <c r="AC3" s="64"/>
-      <c r="AD3" s="64"/>
-      <c r="AE3" s="64"/>
-      <c r="AF3" s="64"/>
-      <c r="AG3" s="64"/>
-      <c r="AH3" s="64"/>
-      <c r="AI3" s="64"/>
-      <c r="AJ3" s="64"/>
-      <c r="AK3" s="64"/>
-      <c r="AL3" s="64"/>
-      <c r="AM3" s="64"/>
-      <c r="AN3" s="64"/>
-      <c r="AO3" s="64"/>
-      <c r="AP3" s="64"/>
-      <c r="AQ3" s="64"/>
-      <c r="AR3" s="64"/>
-      <c r="AS3" s="64"/>
-      <c r="AT3" s="64"/>
-      <c r="AU3" s="64"/>
-      <c r="AV3" s="64"/>
-      <c r="AW3" s="64"/>
-      <c r="AX3" s="64"/>
-      <c r="AY3" s="64"/>
-      <c r="AZ3" s="64"/>
-      <c r="BA3" s="64"/>
-      <c r="BB3" s="64"/>
-      <c r="BC3" s="64"/>
-      <c r="BD3" s="64">
+      <c r="V3" s="59"/>
+      <c r="W3" s="59"/>
+      <c r="X3" s="59"/>
+      <c r="Y3" s="59"/>
+      <c r="Z3" s="59"/>
+      <c r="AA3" s="59"/>
+      <c r="AB3" s="59"/>
+      <c r="AC3" s="59"/>
+      <c r="AD3" s="59"/>
+      <c r="AE3" s="59"/>
+      <c r="AF3" s="59"/>
+      <c r="AG3" s="59"/>
+      <c r="AH3" s="59"/>
+      <c r="AI3" s="59"/>
+      <c r="AJ3" s="59"/>
+      <c r="AK3" s="59"/>
+      <c r="AL3" s="59"/>
+      <c r="AM3" s="59"/>
+      <c r="AN3" s="59"/>
+      <c r="AO3" s="59"/>
+      <c r="AP3" s="59"/>
+      <c r="AQ3" s="59"/>
+      <c r="AR3" s="59"/>
+      <c r="AS3" s="59"/>
+      <c r="AT3" s="59"/>
+      <c r="AU3" s="59"/>
+      <c r="AV3" s="59"/>
+      <c r="AW3" s="59"/>
+      <c r="AX3" s="59"/>
+      <c r="AY3" s="59"/>
+      <c r="AZ3" s="59"/>
+      <c r="BA3" s="59"/>
+      <c r="BB3" s="59"/>
+      <c r="BC3" s="59"/>
+      <c r="BD3" s="59">
         <v>0</v>
       </c>
-      <c r="BE3" s="64"/>
-      <c r="BF3" s="65"/>
-      <c r="BG3" s="65"/>
-      <c r="BH3" s="65"/>
-      <c r="BI3" s="65"/>
-      <c r="BJ3" s="65"/>
-      <c r="BK3" s="65"/>
-      <c r="BL3" s="65"/>
-      <c r="BM3" s="65"/>
-      <c r="BN3" s="65"/>
-      <c r="BO3" s="65">
+      <c r="BE3" s="59"/>
+      <c r="BF3" s="60"/>
+      <c r="BG3" s="60"/>
+      <c r="BH3" s="60"/>
+      <c r="BI3" s="60"/>
+      <c r="BJ3" s="60"/>
+      <c r="BK3" s="60"/>
+      <c r="BL3" s="60"/>
+      <c r="BM3" s="60"/>
+      <c r="BN3" s="60"/>
+      <c r="BO3" s="60">
         <v>90</v>
       </c>
-      <c r="BP3" s="65"/>
+      <c r="BP3" s="60"/>
     </row>
     <row r="4" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
@@ -2795,94 +2769,94 @@
       <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="44"/>
+      <c r="E4" s="40"/>
       <c r="F4" s="9">
         <v>0</v>
       </c>
       <c r="K4" s="9">
         <v>10</v>
       </c>
-      <c r="AF4" s="26">
+      <c r="AF4" s="23">
         <v>40</v>
       </c>
-      <c r="AG4" s="26">
+      <c r="AG4" s="23">
         <v>40</v>
       </c>
-      <c r="AH4" s="26">
+      <c r="AH4" s="23">
         <v>40</v>
       </c>
-      <c r="AI4" s="26">
+      <c r="AI4" s="23">
         <v>40</v>
       </c>
-      <c r="AJ4" s="26">
+      <c r="AJ4" s="23">
         <v>40</v>
       </c>
-      <c r="AK4" s="26">
+      <c r="AK4" s="23">
         <v>40</v>
       </c>
-      <c r="AL4" s="26">
+      <c r="AL4" s="23">
         <v>40</v>
       </c>
-      <c r="AM4" s="26">
+      <c r="AM4" s="23">
         <v>40</v>
       </c>
-      <c r="AN4" s="26">
+      <c r="AN4" s="23">
         <v>40</v>
       </c>
-      <c r="AO4" s="26">
+      <c r="AO4" s="23">
         <v>40</v>
       </c>
-      <c r="AP4" s="26">
+      <c r="AP4" s="23">
         <v>40</v>
       </c>
-      <c r="AQ4" s="26">
+      <c r="AQ4" s="23">
         <v>40</v>
       </c>
-      <c r="AR4" s="26">
+      <c r="AR4" s="23">
         <v>40</v>
       </c>
-      <c r="AS4" s="26">
+      <c r="AS4" s="23">
         <v>40</v>
       </c>
-      <c r="AT4" s="26">
+      <c r="AT4" s="23">
         <v>40</v>
       </c>
-      <c r="AU4" s="26">
+      <c r="AU4" s="23">
         <v>40</v>
       </c>
-      <c r="AV4" s="26">
+      <c r="AV4" s="23">
         <v>10</v>
       </c>
-      <c r="AW4" s="26">
+      <c r="AW4" s="23">
         <v>10</v>
       </c>
-      <c r="AX4" s="26">
+      <c r="AX4" s="23">
         <v>10</v>
       </c>
-      <c r="AY4" s="26"/>
-      <c r="AZ4" s="26">
+      <c r="AY4" s="23"/>
+      <c r="AZ4" s="23">
         <v>30</v>
       </c>
-      <c r="BA4" s="26">
+      <c r="BA4" s="23">
         <v>30</v>
       </c>
-      <c r="BB4" s="26"/>
-      <c r="BC4" s="26"/>
-      <c r="BD4" s="26">
+      <c r="BB4" s="23"/>
+      <c r="BC4" s="23"/>
+      <c r="BD4" s="23">
         <v>55</v>
       </c>
-      <c r="BE4" s="26"/>
-      <c r="BF4" s="66"/>
-      <c r="BG4" s="66"/>
-      <c r="BH4" s="66"/>
-      <c r="BI4" s="66"/>
-      <c r="BJ4" s="66"/>
-      <c r="BK4" s="66"/>
-      <c r="BL4" s="66"/>
-      <c r="BM4" s="66"/>
-      <c r="BN4" s="66"/>
-      <c r="BO4" s="66"/>
-      <c r="BP4" s="66"/>
+      <c r="BE4" s="23"/>
+      <c r="BF4" s="61"/>
+      <c r="BG4" s="61"/>
+      <c r="BH4" s="61"/>
+      <c r="BI4" s="61"/>
+      <c r="BJ4" s="61"/>
+      <c r="BK4" s="61"/>
+      <c r="BL4" s="61"/>
+      <c r="BM4" s="61"/>
+      <c r="BN4" s="61"/>
+      <c r="BO4" s="61"/>
+      <c r="BP4" s="61"/>
     </row>
     <row r="5" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -2897,21 +2871,21 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="44"/>
+      <c r="E5" s="40"/>
       <c r="BD5" s="9">
         <v>0</v>
       </c>
-      <c r="BF5" s="66"/>
-      <c r="BG5" s="66"/>
-      <c r="BH5" s="66"/>
-      <c r="BI5" s="66"/>
-      <c r="BJ5" s="66"/>
-      <c r="BK5" s="66"/>
-      <c r="BL5" s="66"/>
-      <c r="BM5" s="66"/>
-      <c r="BN5" s="66"/>
-      <c r="BO5" s="66"/>
-      <c r="BP5" s="66"/>
+      <c r="BF5" s="61"/>
+      <c r="BG5" s="61"/>
+      <c r="BH5" s="61"/>
+      <c r="BI5" s="61"/>
+      <c r="BJ5" s="61"/>
+      <c r="BK5" s="61"/>
+      <c r="BL5" s="61"/>
+      <c r="BM5" s="61"/>
+      <c r="BN5" s="61"/>
+      <c r="BO5" s="61"/>
+      <c r="BP5" s="61"/>
     </row>
     <row r="6" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
@@ -2926,7 +2900,7 @@
       <c r="D6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="44"/>
+      <c r="E6" s="40"/>
       <c r="BA6" s="9">
         <v>0</v>
       </c>
@@ -2936,21 +2910,21 @@
       <c r="BD6" s="9">
         <v>23.6</v>
       </c>
-      <c r="BF6" s="66"/>
-      <c r="BG6" s="66"/>
-      <c r="BH6" s="66"/>
-      <c r="BI6" s="66"/>
-      <c r="BJ6" s="66"/>
-      <c r="BK6" s="66"/>
-      <c r="BL6" s="66">
+      <c r="BF6" s="61"/>
+      <c r="BG6" s="61"/>
+      <c r="BH6" s="61"/>
+      <c r="BI6" s="61"/>
+      <c r="BJ6" s="61"/>
+      <c r="BK6" s="61"/>
+      <c r="BL6" s="61">
         <v>80</v>
       </c>
-      <c r="BM6" s="66">
+      <c r="BM6" s="61">
         <v>80</v>
       </c>
-      <c r="BN6" s="66"/>
-      <c r="BO6" s="66"/>
-      <c r="BP6" s="66">
+      <c r="BN6" s="61"/>
+      <c r="BO6" s="61"/>
+      <c r="BP6" s="61">
         <v>80</v>
       </c>
     </row>
@@ -2967,31 +2941,31 @@
       <c r="D7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="44"/>
+      <c r="E7" s="40"/>
       <c r="BD7" s="9">
         <v>0</v>
       </c>
-      <c r="BF7" s="66"/>
-      <c r="BG7" s="66"/>
-      <c r="BH7" s="66"/>
-      <c r="BI7" s="66"/>
-      <c r="BJ7" s="66"/>
-      <c r="BK7" s="66"/>
-      <c r="BL7" s="66">
+      <c r="BF7" s="61"/>
+      <c r="BG7" s="61"/>
+      <c r="BH7" s="61"/>
+      <c r="BI7" s="61"/>
+      <c r="BJ7" s="61"/>
+      <c r="BK7" s="61"/>
+      <c r="BL7" s="61">
         <v>80</v>
       </c>
-      <c r="BM7" s="66">
+      <c r="BM7" s="61">
         <v>80</v>
       </c>
-      <c r="BN7" s="66"/>
-      <c r="BO7" s="66"/>
-      <c r="BP7" s="66">
+      <c r="BN7" s="61"/>
+      <c r="BO7" s="61"/>
+      <c r="BP7" s="61">
         <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>4</v>
@@ -3002,20 +2976,20 @@
       <c r="D8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="44"/>
+      <c r="E8" s="40"/>
       <c r="BD8" s="9">
         <v>0</v>
       </c>
-      <c r="BF8" s="66"/>
-      <c r="BG8" s="66"/>
-      <c r="BH8" s="66"/>
-      <c r="BI8" s="66"/>
-      <c r="BJ8" s="66"/>
-      <c r="BK8" s="66"/>
-      <c r="BL8" s="66"/>
-      <c r="BM8" s="66"/>
-      <c r="BN8" s="66"/>
-      <c r="BO8" s="66"/>
+      <c r="BF8" s="61"/>
+      <c r="BG8" s="61"/>
+      <c r="BH8" s="61"/>
+      <c r="BI8" s="61"/>
+      <c r="BJ8" s="61"/>
+      <c r="BK8" s="61"/>
+      <c r="BL8" s="61"/>
+      <c r="BM8" s="61"/>
+      <c r="BN8" s="61"/>
+      <c r="BO8" s="61"/>
       <c r="BP8" s="9">
         <v>10</v>
       </c>
@@ -3023,100 +2997,100 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:69" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="52" t="s">
+    <row r="9" spans="1:69" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="52">
-        <v>1</v>
-      </c>
-      <c r="D9" s="52" t="s">
+      <c r="C9" s="47">
+        <v>1</v>
+      </c>
+      <c r="D9" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="53">
+      <c r="E9" s="48">
         <v>0</v>
       </c>
-      <c r="BD9" s="54">
+      <c r="BD9" s="49">
         <v>0</v>
       </c>
-      <c r="BF9" s="67"/>
-      <c r="BG9" s="67"/>
-      <c r="BH9" s="67"/>
-      <c r="BI9" s="67"/>
-      <c r="BJ9" s="67"/>
-      <c r="BK9" s="67"/>
-      <c r="BL9" s="67"/>
-      <c r="BM9" s="67"/>
-      <c r="BN9" s="67">
+      <c r="BF9" s="62"/>
+      <c r="BG9" s="62"/>
+      <c r="BH9" s="62"/>
+      <c r="BI9" s="62"/>
+      <c r="BJ9" s="62"/>
+      <c r="BK9" s="62"/>
+      <c r="BL9" s="62"/>
+      <c r="BM9" s="62"/>
+      <c r="BN9" s="62">
         <v>10</v>
       </c>
-      <c r="BO9" s="67"/>
-      <c r="BP9" s="67"/>
+      <c r="BO9" s="62"/>
+      <c r="BP9" s="62"/>
     </row>
-    <row r="10" spans="1:69" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="52" t="s">
+    <row r="10" spans="1:69" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="52">
-        <v>1</v>
-      </c>
-      <c r="D10" s="52" t="s">
+      <c r="C10" s="47">
+        <v>1</v>
+      </c>
+      <c r="D10" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="53">
+      <c r="E10" s="48">
         <v>0</v>
       </c>
-      <c r="BD10" s="54">
+      <c r="BD10" s="49">
         <v>0</v>
       </c>
-      <c r="BF10" s="67"/>
-      <c r="BG10" s="67"/>
-      <c r="BH10" s="67"/>
-      <c r="BI10" s="67"/>
-      <c r="BJ10" s="67"/>
-      <c r="BK10" s="67"/>
-      <c r="BL10" s="67"/>
-      <c r="BM10" s="67"/>
-      <c r="BN10" s="67"/>
-      <c r="BO10" s="67"/>
-      <c r="BP10" s="67"/>
+      <c r="BF10" s="62"/>
+      <c r="BG10" s="62"/>
+      <c r="BH10" s="62"/>
+      <c r="BI10" s="62"/>
+      <c r="BJ10" s="62"/>
+      <c r="BK10" s="62"/>
+      <c r="BL10" s="62"/>
+      <c r="BM10" s="62"/>
+      <c r="BN10" s="62"/>
+      <c r="BO10" s="62"/>
+      <c r="BP10" s="62"/>
     </row>
-    <row r="11" spans="1:69" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="52" t="s">
+    <row r="11" spans="1:69" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="52">
-        <v>1</v>
-      </c>
-      <c r="D11" s="52" t="s">
+      <c r="C11" s="47">
+        <v>1</v>
+      </c>
+      <c r="D11" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="53">
+      <c r="E11" s="48">
         <v>0</v>
       </c>
-      <c r="BD11" s="54">
+      <c r="BD11" s="49">
         <v>0</v>
       </c>
-      <c r="BF11" s="67"/>
-      <c r="BG11" s="67"/>
-      <c r="BH11" s="67"/>
-      <c r="BI11" s="67"/>
-      <c r="BJ11" s="67"/>
-      <c r="BK11" s="67"/>
-      <c r="BL11" s="67"/>
-      <c r="BM11" s="67"/>
-      <c r="BN11" s="67"/>
-      <c r="BO11" s="67"/>
-      <c r="BP11" s="67"/>
+      <c r="BF11" s="62"/>
+      <c r="BG11" s="62"/>
+      <c r="BH11" s="62"/>
+      <c r="BI11" s="62"/>
+      <c r="BJ11" s="62"/>
+      <c r="BK11" s="62"/>
+      <c r="BL11" s="62"/>
+      <c r="BM11" s="62"/>
+      <c r="BN11" s="62"/>
+      <c r="BO11" s="62"/>
+      <c r="BP11" s="62"/>
     </row>
     <row r="12" spans="1:69" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
@@ -3131,7 +3105,7 @@
       <c r="D12" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="45"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="11">
         <v>70</v>
       </c>
@@ -3147,17 +3121,17 @@
       <c r="BC12" s="11">
         <v>85</v>
       </c>
-      <c r="BF12" s="68"/>
-      <c r="BG12" s="68"/>
-      <c r="BH12" s="68"/>
-      <c r="BI12" s="68"/>
-      <c r="BJ12" s="68"/>
-      <c r="BK12" s="68"/>
-      <c r="BL12" s="68"/>
-      <c r="BM12" s="68"/>
-      <c r="BN12" s="68"/>
-      <c r="BO12" s="68"/>
-      <c r="BP12" s="68"/>
+      <c r="BF12" s="63"/>
+      <c r="BG12" s="63"/>
+      <c r="BH12" s="63"/>
+      <c r="BI12" s="63"/>
+      <c r="BJ12" s="63"/>
+      <c r="BK12" s="63"/>
+      <c r="BL12" s="63"/>
+      <c r="BM12" s="63"/>
+      <c r="BN12" s="63"/>
+      <c r="BO12" s="63"/>
+      <c r="BP12" s="63"/>
     </row>
     <row r="13" spans="1:69" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
@@ -3172,7 +3146,7 @@
       <c r="D13" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="46"/>
+      <c r="E13" s="42"/>
       <c r="H13" s="13">
         <v>30</v>
       </c>
@@ -3182,17 +3156,17 @@
       <c r="AF13" s="13">
         <v>40</v>
       </c>
-      <c r="BF13" s="69"/>
-      <c r="BG13" s="69"/>
-      <c r="BH13" s="69"/>
-      <c r="BI13" s="69"/>
-      <c r="BJ13" s="69"/>
-      <c r="BK13" s="69"/>
-      <c r="BL13" s="69"/>
-      <c r="BM13" s="69"/>
-      <c r="BN13" s="69"/>
-      <c r="BO13" s="69"/>
-      <c r="BP13" s="69"/>
+      <c r="BF13" s="64"/>
+      <c r="BG13" s="64"/>
+      <c r="BH13" s="64"/>
+      <c r="BI13" s="64"/>
+      <c r="BJ13" s="64"/>
+      <c r="BK13" s="64"/>
+      <c r="BL13" s="64"/>
+      <c r="BM13" s="64"/>
+      <c r="BN13" s="64"/>
+      <c r="BO13" s="64"/>
+      <c r="BP13" s="64"/>
     </row>
     <row r="14" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
@@ -3207,7 +3181,7 @@
       <c r="D14" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="47"/>
+      <c r="E14" s="43"/>
       <c r="V14" s="15">
         <v>30</v>
       </c>
@@ -3217,17 +3191,17 @@
       <c r="AP14" s="15">
         <v>50</v>
       </c>
-      <c r="BF14" s="70"/>
-      <c r="BG14" s="70"/>
-      <c r="BH14" s="70"/>
-      <c r="BI14" s="70"/>
-      <c r="BJ14" s="70"/>
-      <c r="BK14" s="70"/>
-      <c r="BL14" s="70"/>
-      <c r="BM14" s="70"/>
-      <c r="BN14" s="70"/>
-      <c r="BO14" s="70"/>
-      <c r="BP14" s="70"/>
+      <c r="BF14" s="65"/>
+      <c r="BG14" s="65"/>
+      <c r="BH14" s="65"/>
+      <c r="BI14" s="65"/>
+      <c r="BJ14" s="65"/>
+      <c r="BK14" s="65"/>
+      <c r="BL14" s="65"/>
+      <c r="BM14" s="65"/>
+      <c r="BN14" s="65"/>
+      <c r="BO14" s="65"/>
+      <c r="BP14" s="65"/>
     </row>
     <row r="15" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
@@ -3242,7 +3216,7 @@
       <c r="D15" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="47"/>
+      <c r="E15" s="43"/>
       <c r="I15" s="15">
         <v>7</v>
       </c>
@@ -3252,17 +3226,17 @@
       <c r="AP15" s="15">
         <v>70</v>
       </c>
-      <c r="BF15" s="70"/>
-      <c r="BG15" s="70"/>
-      <c r="BH15" s="70"/>
-      <c r="BI15" s="70"/>
-      <c r="BJ15" s="70"/>
-      <c r="BK15" s="70"/>
-      <c r="BL15" s="70"/>
-      <c r="BM15" s="70"/>
-      <c r="BN15" s="70"/>
-      <c r="BO15" s="70"/>
-      <c r="BP15" s="70"/>
+      <c r="BF15" s="65"/>
+      <c r="BG15" s="65"/>
+      <c r="BH15" s="65"/>
+      <c r="BI15" s="65"/>
+      <c r="BJ15" s="65"/>
+      <c r="BK15" s="65"/>
+      <c r="BL15" s="65"/>
+      <c r="BM15" s="65"/>
+      <c r="BN15" s="65"/>
+      <c r="BO15" s="65"/>
+      <c r="BP15" s="65"/>
     </row>
     <row r="16" spans="1:69" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
@@ -3277,7 +3251,7 @@
       <c r="D16" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="46"/>
+      <c r="E16" s="42"/>
       <c r="I16" s="13">
         <v>0</v>
       </c>
@@ -3287,42 +3261,42 @@
       <c r="AB16" s="13">
         <v>65</v>
       </c>
-      <c r="AK16" s="27"/>
-      <c r="AL16" s="27"/>
-      <c r="AM16" s="27"/>
-      <c r="AN16" s="27"/>
-      <c r="AO16" s="27"/>
-      <c r="AP16" s="27"/>
-      <c r="AQ16" s="27"/>
-      <c r="AR16" s="27"/>
-      <c r="AS16" s="27"/>
-      <c r="AT16" s="27"/>
-      <c r="AU16" s="27"/>
-      <c r="AV16" s="27"/>
-      <c r="AW16" s="27"/>
-      <c r="AX16" s="27"/>
-      <c r="AY16" s="27"/>
-      <c r="AZ16" s="27"/>
-      <c r="BA16" s="27"/>
-      <c r="BB16" s="27">
+      <c r="AK16" s="24"/>
+      <c r="AL16" s="24"/>
+      <c r="AM16" s="24"/>
+      <c r="AN16" s="24"/>
+      <c r="AO16" s="24"/>
+      <c r="AP16" s="24"/>
+      <c r="AQ16" s="24"/>
+      <c r="AR16" s="24"/>
+      <c r="AS16" s="24"/>
+      <c r="AT16" s="24"/>
+      <c r="AU16" s="24"/>
+      <c r="AV16" s="24"/>
+      <c r="AW16" s="24"/>
+      <c r="AX16" s="24"/>
+      <c r="AY16" s="24"/>
+      <c r="AZ16" s="24"/>
+      <c r="BA16" s="24"/>
+      <c r="BB16" s="24">
         <v>93</v>
       </c>
-      <c r="BC16" s="27">
+      <c r="BC16" s="24">
         <v>85</v>
       </c>
-      <c r="BF16" s="69"/>
-      <c r="BG16" s="69">
+      <c r="BF16" s="64"/>
+      <c r="BG16" s="64">
         <v>96</v>
       </c>
-      <c r="BH16" s="69"/>
-      <c r="BI16" s="69"/>
-      <c r="BJ16" s="69"/>
-      <c r="BK16" s="69"/>
-      <c r="BL16" s="69"/>
-      <c r="BM16" s="69"/>
-      <c r="BN16" s="69"/>
-      <c r="BO16" s="69"/>
-      <c r="BP16" s="69"/>
+      <c r="BH16" s="64"/>
+      <c r="BI16" s="64"/>
+      <c r="BJ16" s="64"/>
+      <c r="BK16" s="64"/>
+      <c r="BL16" s="64"/>
+      <c r="BM16" s="64"/>
+      <c r="BN16" s="64"/>
+      <c r="BO16" s="64"/>
+      <c r="BP16" s="64"/>
     </row>
     <row r="17" spans="1:76" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
@@ -3337,7 +3311,7 @@
       <c r="D17" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="46"/>
+      <c r="E17" s="42"/>
       <c r="I17" s="13">
         <v>0</v>
       </c>
@@ -3347,421 +3321,539 @@
       <c r="AB17" s="13">
         <v>8</v>
       </c>
-      <c r="AK17" s="27"/>
-      <c r="AL17" s="27"/>
-      <c r="AM17" s="27"/>
-      <c r="AN17" s="27"/>
-      <c r="AO17" s="27"/>
-      <c r="AP17" s="27"/>
-      <c r="AQ17" s="27"/>
-      <c r="AR17" s="27"/>
-      <c r="AS17" s="27"/>
-      <c r="AT17" s="27"/>
-      <c r="AU17" s="27"/>
-      <c r="AV17" s="27"/>
-      <c r="AW17" s="27"/>
-      <c r="AX17" s="27"/>
-      <c r="AY17" s="27"/>
-      <c r="AZ17" s="27"/>
-      <c r="BA17" s="27"/>
-      <c r="BB17" s="27"/>
-      <c r="BC17" s="27"/>
+      <c r="AK17" s="24"/>
+      <c r="AL17" s="24"/>
+      <c r="AM17" s="24"/>
+      <c r="AN17" s="24"/>
+      <c r="AO17" s="24"/>
+      <c r="AP17" s="24"/>
+      <c r="AQ17" s="24"/>
+      <c r="AR17" s="24"/>
+      <c r="AS17" s="24"/>
+      <c r="AT17" s="24"/>
+      <c r="AU17" s="24"/>
+      <c r="AV17" s="24"/>
+      <c r="AW17" s="24"/>
+      <c r="AX17" s="24"/>
+      <c r="AY17" s="24"/>
+      <c r="AZ17" s="24"/>
+      <c r="BA17" s="24"/>
+      <c r="BB17" s="24"/>
+      <c r="BC17" s="24"/>
       <c r="BD17" s="13">
         <v>5</v>
       </c>
-      <c r="BF17" s="69"/>
-      <c r="BG17" s="69">
+      <c r="BF17" s="64"/>
+      <c r="BG17" s="64">
         <v>1.3</v>
       </c>
-      <c r="BH17" s="69"/>
-      <c r="BI17" s="69"/>
-      <c r="BJ17" s="69"/>
-      <c r="BK17" s="69"/>
-      <c r="BL17" s="69"/>
-      <c r="BM17" s="69"/>
-      <c r="BN17" s="69"/>
-      <c r="BO17" s="69"/>
-      <c r="BP17" s="69"/>
+      <c r="BH17" s="64"/>
+      <c r="BI17" s="64"/>
+      <c r="BJ17" s="64"/>
+      <c r="BK17" s="64"/>
+      <c r="BL17" s="64"/>
+      <c r="BM17" s="64"/>
+      <c r="BN17" s="64"/>
+      <c r="BO17" s="64"/>
+      <c r="BP17" s="64"/>
     </row>
-    <row r="18" spans="1:76" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="23" t="s">
+    <row r="18" spans="1:76" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="23">
-        <v>1</v>
-      </c>
-      <c r="D18" s="23" t="s">
+      <c r="C18" s="29">
+        <v>1</v>
+      </c>
+      <c r="D18" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="48"/>
-      <c r="I18" s="24">
+      <c r="E18" s="44"/>
+      <c r="AK18" s="31"/>
+      <c r="AL18" s="31"/>
+      <c r="AM18" s="31"/>
+      <c r="AN18" s="31"/>
+      <c r="AO18" s="31"/>
+      <c r="AP18" s="31"/>
+      <c r="AQ18" s="31"/>
+      <c r="AR18" s="31"/>
+      <c r="AS18" s="31"/>
+      <c r="AT18" s="31"/>
+      <c r="AU18" s="31"/>
+      <c r="AV18" s="31"/>
+      <c r="AW18" s="31"/>
+      <c r="AX18" s="31"/>
+      <c r="AY18" s="31"/>
+      <c r="AZ18" s="31"/>
+      <c r="BA18" s="31"/>
+      <c r="BB18" s="31"/>
+      <c r="BC18" s="31"/>
+      <c r="BD18" s="30">
         <v>0</v>
       </c>
-      <c r="V18" s="24">
-        <v>15</v>
-      </c>
-      <c r="AB18" s="24">
-        <v>30</v>
-      </c>
-      <c r="AK18" s="28"/>
-      <c r="AL18" s="28"/>
-      <c r="AM18" s="28"/>
-      <c r="AN18" s="28"/>
-      <c r="AO18" s="28"/>
-      <c r="AP18" s="28"/>
-      <c r="AQ18" s="28"/>
-      <c r="AR18" s="28"/>
-      <c r="AS18" s="28"/>
-      <c r="AT18" s="28"/>
-      <c r="AU18" s="28"/>
-      <c r="AV18" s="28"/>
-      <c r="AW18" s="28"/>
-      <c r="AX18" s="28"/>
-      <c r="AY18" s="28"/>
-      <c r="AZ18" s="28"/>
-      <c r="BA18" s="28"/>
-      <c r="BB18" s="28"/>
-      <c r="BC18" s="28"/>
-      <c r="BD18" s="24">
+      <c r="BF18" s="66"/>
+      <c r="BG18" s="66"/>
+      <c r="BH18" s="66"/>
+      <c r="BI18" s="66"/>
+      <c r="BJ18" s="66">
+        <v>100</v>
+      </c>
+      <c r="BK18" s="66"/>
+      <c r="BL18" s="66"/>
+      <c r="BM18" s="66">
+        <v>100</v>
+      </c>
+      <c r="BN18" s="66"/>
+      <c r="BO18" s="66"/>
+      <c r="BP18" s="66">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="14">
+        <v>1</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="43"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="38"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="38"/>
+      <c r="R19" s="38"/>
+      <c r="S19" s="38"/>
+      <c r="T19" s="38"/>
+      <c r="U19" s="38"/>
+      <c r="V19" s="38"/>
+      <c r="W19" s="38"/>
+      <c r="X19" s="38"/>
+      <c r="Y19" s="38"/>
+      <c r="Z19" s="38"/>
+      <c r="AA19" s="38"/>
+      <c r="AB19" s="38"/>
+      <c r="AC19" s="38"/>
+      <c r="AD19" s="38"/>
+      <c r="AE19" s="38"/>
+      <c r="AF19" s="38"/>
+      <c r="AG19" s="38"/>
+      <c r="AH19" s="38"/>
+      <c r="AI19" s="38"/>
+      <c r="AJ19" s="38"/>
+      <c r="AK19" s="38"/>
+      <c r="AL19" s="38"/>
+      <c r="AM19" s="38"/>
+      <c r="AN19" s="38"/>
+      <c r="AO19" s="38"/>
+      <c r="AP19" s="38"/>
+      <c r="AQ19" s="38"/>
+      <c r="AR19" s="38"/>
+      <c r="AS19" s="38"/>
+      <c r="AT19" s="38"/>
+      <c r="AU19" s="38"/>
+      <c r="AV19" s="38"/>
+      <c r="AW19" s="38"/>
+      <c r="AX19" s="38"/>
+      <c r="AY19" s="38"/>
+      <c r="AZ19" s="38"/>
+      <c r="BA19" s="38"/>
+      <c r="BB19" s="38"/>
+      <c r="BC19" s="38"/>
+      <c r="BD19" s="38">
+        <v>0</v>
+      </c>
+      <c r="BE19" s="38"/>
+      <c r="BF19" s="67">
+        <v>100</v>
+      </c>
+      <c r="BG19" s="67"/>
+      <c r="BH19" s="67"/>
+      <c r="BI19" s="67"/>
+      <c r="BJ19" s="67"/>
+      <c r="BK19" s="67"/>
+      <c r="BL19" s="67"/>
+      <c r="BM19" s="67">
+        <v>100</v>
+      </c>
+      <c r="BN19" s="67"/>
+      <c r="BO19" s="67"/>
+      <c r="BP19" s="67">
+        <v>100</v>
+      </c>
+      <c r="BQ19" s="38"/>
+      <c r="BR19" s="38"/>
+      <c r="BS19" s="38"/>
+      <c r="BT19" s="38"/>
+      <c r="BU19" s="38"/>
+      <c r="BV19" s="38"/>
+      <c r="BW19" s="38"/>
+      <c r="BX19" s="38"/>
+    </row>
+    <row r="20" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="14">
+        <v>1</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="43">
+        <v>0</v>
+      </c>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="38"/>
+      <c r="R20" s="38"/>
+      <c r="S20" s="38"/>
+      <c r="T20" s="38"/>
+      <c r="U20" s="38"/>
+      <c r="V20" s="38"/>
+      <c r="W20" s="38"/>
+      <c r="X20" s="38"/>
+      <c r="Y20" s="38"/>
+      <c r="Z20" s="38"/>
+      <c r="AA20" s="38"/>
+      <c r="AB20" s="38"/>
+      <c r="AC20" s="38"/>
+      <c r="AD20" s="38"/>
+      <c r="AE20" s="38"/>
+      <c r="AF20" s="38"/>
+      <c r="AG20" s="38"/>
+      <c r="AH20" s="38"/>
+      <c r="AI20" s="38"/>
+      <c r="AJ20" s="38"/>
+      <c r="AK20" s="38"/>
+      <c r="AL20" s="38"/>
+      <c r="AM20" s="38"/>
+      <c r="AN20" s="38"/>
+      <c r="AO20" s="38"/>
+      <c r="AP20" s="38"/>
+      <c r="AQ20" s="38"/>
+      <c r="AR20" s="38"/>
+      <c r="AS20" s="38"/>
+      <c r="AT20" s="38"/>
+      <c r="AU20" s="38"/>
+      <c r="AV20" s="38"/>
+      <c r="AW20" s="38"/>
+      <c r="AX20" s="38"/>
+      <c r="AY20" s="38"/>
+      <c r="AZ20" s="38"/>
+      <c r="BA20" s="38"/>
+      <c r="BB20" s="38"/>
+      <c r="BC20" s="38"/>
+      <c r="BD20" s="38">
+        <v>0</v>
+      </c>
+      <c r="BE20" s="38"/>
+      <c r="BF20" s="67"/>
+      <c r="BG20" s="67"/>
+      <c r="BH20" s="67">
+        <v>17</v>
+      </c>
+      <c r="BI20" s="67">
+        <v>70</v>
+      </c>
+      <c r="BJ20" s="67"/>
+      <c r="BK20" s="67"/>
+      <c r="BL20" s="67"/>
+      <c r="BM20" s="67">
+        <v>70</v>
+      </c>
+      <c r="BN20" s="67"/>
+      <c r="BO20" s="67"/>
+      <c r="BP20" s="67">
+        <v>70</v>
+      </c>
+      <c r="BQ20" s="38"/>
+      <c r="BR20" s="38"/>
+      <c r="BS20" s="38"/>
+      <c r="BT20" s="38"/>
+      <c r="BU20" s="38"/>
+      <c r="BV20" s="38"/>
+      <c r="BW20" s="38"/>
+      <c r="BX20" s="38"/>
+    </row>
+    <row r="21" spans="1:76" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="47">
+        <v>1</v>
+      </c>
+      <c r="D21" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="48"/>
+      <c r="BD21" s="49">
+        <v>0</v>
+      </c>
+      <c r="BF21" s="62"/>
+      <c r="BG21" s="62"/>
+      <c r="BH21" s="62"/>
+      <c r="BI21" s="62"/>
+      <c r="BJ21" s="62"/>
+      <c r="BK21" s="62"/>
+      <c r="BL21" s="62"/>
+      <c r="BM21" s="62"/>
+      <c r="BN21" s="62"/>
+      <c r="BO21" s="62"/>
+      <c r="BP21" s="62"/>
+    </row>
+    <row r="22" spans="1:76" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="47">
+        <v>1</v>
+      </c>
+      <c r="D22" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="48"/>
+      <c r="BD22" s="49">
+        <v>0</v>
+      </c>
+      <c r="BF22" s="62"/>
+      <c r="BG22" s="62"/>
+      <c r="BH22" s="62"/>
+      <c r="BI22" s="62"/>
+      <c r="BJ22" s="62"/>
+      <c r="BK22" s="62">
         <v>50</v>
       </c>
-      <c r="BF18" s="71"/>
-      <c r="BG18" s="71"/>
-      <c r="BH18" s="71"/>
-      <c r="BI18" s="71"/>
-      <c r="BJ18" s="71"/>
-      <c r="BK18" s="71"/>
-      <c r="BL18" s="71"/>
-      <c r="BM18" s="71"/>
-      <c r="BN18" s="71"/>
-      <c r="BO18" s="71"/>
-      <c r="BP18" s="71"/>
+      <c r="BL22" s="62"/>
+      <c r="BM22" s="62">
+        <v>50</v>
+      </c>
+      <c r="BN22" s="62"/>
+      <c r="BO22" s="62"/>
+      <c r="BP22" s="62">
+        <v>50</v>
+      </c>
     </row>
-    <row r="19" spans="1:76" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="23" t="s">
+    <row r="23" spans="1:76" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="23">
-        <v>1</v>
-      </c>
-      <c r="D19" s="23" t="s">
+      <c r="C23" s="51">
+        <v>1</v>
+      </c>
+      <c r="D23" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="48"/>
-      <c r="I19" s="24">
-        <v>0</v>
-      </c>
-      <c r="V19" s="24">
-        <v>55</v>
-      </c>
-      <c r="AB19" s="24">
-        <v>50</v>
-      </c>
-      <c r="AK19" s="28"/>
-      <c r="AL19" s="28"/>
-      <c r="AM19" s="28"/>
-      <c r="AN19" s="28"/>
-      <c r="AO19" s="28"/>
-      <c r="AP19" s="28"/>
-      <c r="AQ19" s="28"/>
-      <c r="AR19" s="28"/>
-      <c r="AS19" s="28"/>
-      <c r="AT19" s="28"/>
-      <c r="AU19" s="28"/>
-      <c r="AV19" s="28"/>
-      <c r="AW19" s="28"/>
-      <c r="AX19" s="28"/>
-      <c r="AY19" s="28"/>
-      <c r="AZ19" s="28"/>
-      <c r="BA19" s="28"/>
-      <c r="BB19" s="28"/>
-      <c r="BC19" s="28"/>
-      <c r="BD19" s="24">
-        <v>20</v>
-      </c>
-      <c r="BF19" s="71"/>
-      <c r="BG19" s="71"/>
-      <c r="BH19" s="71"/>
-      <c r="BI19" s="71"/>
-      <c r="BJ19" s="71"/>
-      <c r="BK19" s="71"/>
-      <c r="BL19" s="71"/>
-      <c r="BM19" s="71"/>
-      <c r="BN19" s="71"/>
-      <c r="BO19" s="71"/>
-      <c r="BP19" s="71"/>
-    </row>
-    <row r="20" spans="1:76" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="8">
-        <v>1</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="44"/>
-      <c r="I20" s="9">
-        <v>0</v>
-      </c>
-      <c r="V20" s="9">
-        <v>5</v>
-      </c>
-      <c r="AB20" s="9">
-        <v>15</v>
-      </c>
-      <c r="AK20" s="26"/>
-      <c r="AL20" s="26"/>
-      <c r="AM20" s="26"/>
-      <c r="AN20" s="26"/>
-      <c r="AO20" s="26"/>
-      <c r="AP20" s="26"/>
-      <c r="AQ20" s="26"/>
-      <c r="AR20" s="26"/>
-      <c r="AS20" s="26"/>
-      <c r="AT20" s="26"/>
-      <c r="AU20" s="26"/>
-      <c r="AV20" s="26"/>
-      <c r="AW20" s="26"/>
-      <c r="AX20" s="26"/>
-      <c r="AY20" s="26"/>
-      <c r="AZ20" s="26"/>
-      <c r="BA20" s="26"/>
-      <c r="BB20" s="26"/>
-      <c r="BC20" s="26"/>
-      <c r="BD20" s="9">
-        <v>30</v>
-      </c>
-      <c r="BF20" s="66"/>
-      <c r="BG20" s="66"/>
-      <c r="BH20" s="66"/>
-      <c r="BI20" s="66"/>
-      <c r="BJ20" s="66"/>
-      <c r="BK20" s="66"/>
-      <c r="BL20" s="66"/>
-      <c r="BM20" s="66"/>
-      <c r="BN20" s="66"/>
-      <c r="BO20" s="66"/>
-      <c r="BP20" s="66"/>
-    </row>
-    <row r="21" spans="1:76" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="8">
-        <v>1</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="44"/>
-      <c r="I21" s="9">
-        <v>0</v>
-      </c>
-      <c r="V21" s="9">
-        <v>65</v>
-      </c>
-      <c r="AB21" s="9">
-        <v>62</v>
-      </c>
-      <c r="AK21" s="26"/>
-      <c r="AL21" s="26"/>
-      <c r="AM21" s="26"/>
-      <c r="AN21" s="26"/>
-      <c r="AO21" s="26"/>
-      <c r="AP21" s="26"/>
-      <c r="AQ21" s="26"/>
-      <c r="AR21" s="26"/>
-      <c r="AS21" s="26"/>
-      <c r="AT21" s="26"/>
-      <c r="AU21" s="26"/>
-      <c r="AV21" s="26"/>
-      <c r="AW21" s="26"/>
-      <c r="AX21" s="26"/>
-      <c r="AY21" s="26"/>
-      <c r="AZ21" s="26"/>
-      <c r="BA21" s="26"/>
-      <c r="BB21" s="26"/>
-      <c r="BC21" s="26"/>
-      <c r="BD21" s="9">
-        <v>35</v>
-      </c>
-      <c r="BF21" s="66"/>
-      <c r="BG21" s="66"/>
-      <c r="BH21" s="66"/>
-      <c r="BI21" s="66"/>
-      <c r="BJ21" s="66"/>
-      <c r="BK21" s="66"/>
-      <c r="BL21" s="66"/>
-      <c r="BM21" s="66"/>
-      <c r="BN21" s="66"/>
-      <c r="BO21" s="66"/>
-      <c r="BP21" s="66"/>
-    </row>
-    <row r="22" spans="1:76" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="33">
-        <v>1</v>
-      </c>
-      <c r="D22" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="49"/>
-      <c r="AK22" s="35"/>
-      <c r="AL22" s="35"/>
-      <c r="AM22" s="35"/>
-      <c r="AN22" s="35"/>
-      <c r="AO22" s="35"/>
-      <c r="AP22" s="35"/>
-      <c r="AQ22" s="35"/>
-      <c r="AR22" s="35"/>
-      <c r="AS22" s="35"/>
-      <c r="AT22" s="35"/>
-      <c r="AU22" s="35"/>
-      <c r="AV22" s="35"/>
-      <c r="AW22" s="35"/>
-      <c r="AX22" s="35"/>
-      <c r="AY22" s="35"/>
-      <c r="AZ22" s="35"/>
-      <c r="BA22" s="35"/>
-      <c r="BB22" s="35"/>
-      <c r="BC22" s="35"/>
-      <c r="BD22" s="34">
-        <v>0</v>
-      </c>
-      <c r="BF22" s="72"/>
-      <c r="BG22" s="72"/>
-      <c r="BH22" s="72"/>
-      <c r="BI22" s="72"/>
-      <c r="BJ22" s="72">
+      <c r="E23" s="52">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="F23" s="53">
+        <v>4.84</v>
+      </c>
+      <c r="G23" s="53">
+        <v>5.44</v>
+      </c>
+      <c r="H23" s="53">
+        <v>6.11</v>
+      </c>
+      <c r="I23" s="53">
+        <v>6.86</v>
+      </c>
+      <c r="J23" s="53">
+        <v>7.7</v>
+      </c>
+      <c r="K23" s="53">
+        <v>8.68</v>
+      </c>
+      <c r="L23" s="53">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="M23" s="53">
+        <v>9.41</v>
+      </c>
+      <c r="N23" s="53">
+        <v>11.48</v>
+      </c>
+      <c r="O23" s="53">
+        <v>12.75</v>
+      </c>
+      <c r="P23" s="53">
+        <v>14.6</v>
+      </c>
+      <c r="Q23" s="53">
+        <v>16.5</v>
+      </c>
+      <c r="R23" s="53">
+        <v>18.38</v>
+      </c>
+      <c r="S23" s="53">
+        <v>19.670000000000002</v>
+      </c>
+      <c r="T23" s="53">
+        <v>20.87</v>
+      </c>
+      <c r="U23" s="53">
+        <v>22.5</v>
+      </c>
+      <c r="V23" s="53">
+        <v>25.9</v>
+      </c>
+      <c r="W23" s="53">
+        <v>28.8</v>
+      </c>
+      <c r="X23" s="53">
+        <v>30.8</v>
+      </c>
+      <c r="Y23" s="53">
+        <v>32.9</v>
+      </c>
+      <c r="Z23" s="53">
+        <v>34.6</v>
+      </c>
+      <c r="AA23" s="53">
+        <v>36.1</v>
+      </c>
+      <c r="AB23" s="53">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="AC23" s="53">
+        <v>38.9</v>
+      </c>
+      <c r="AD23" s="53">
+        <v>43.4</v>
+      </c>
+      <c r="AE23" s="53">
+        <v>46.1</v>
+      </c>
+      <c r="AF23" s="53">
+        <v>49.9</v>
+      </c>
+      <c r="AG23" s="53">
+        <v>53.1</v>
+      </c>
+      <c r="AH23" s="53">
+        <v>55.7</v>
+      </c>
+      <c r="AI23" s="53">
+        <v>58.6</v>
+      </c>
+      <c r="AJ23" s="53">
+        <v>59.1</v>
+      </c>
+      <c r="AK23" s="53">
+        <v>60.4</v>
+      </c>
+      <c r="AL23" s="53">
+        <v>62.2</v>
+      </c>
+      <c r="AM23" s="53">
+        <v>64.3</v>
+      </c>
+      <c r="AN23" s="53">
+        <v>68</v>
+      </c>
+      <c r="AO23" s="53">
+        <v>69.3</v>
+      </c>
+      <c r="AP23" s="53">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="AQ23" s="53">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="AR23" s="53">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="AS23" s="53">
+        <v>76.7</v>
+      </c>
+      <c r="AT23" s="53">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="AU23" s="53">
+        <v>80.8</v>
+      </c>
+      <c r="AV23" s="53">
+        <v>82.8</v>
+      </c>
+      <c r="AW23" s="53">
+        <v>86.7</v>
+      </c>
+      <c r="AX23" s="53">
+        <v>93.4</v>
+      </c>
+      <c r="AY23" s="53">
+        <v>96.5</v>
+      </c>
+      <c r="AZ23" s="53">
         <v>100</v>
       </c>
-      <c r="BK22" s="72"/>
-      <c r="BL22" s="72"/>
-      <c r="BM22" s="72">
-        <v>100</v>
-      </c>
-      <c r="BN22" s="72"/>
-      <c r="BO22" s="72"/>
-      <c r="BP22" s="72">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="14">
-        <v>1</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="47"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="42"/>
-      <c r="N23" s="42"/>
-      <c r="O23" s="42"/>
-      <c r="P23" s="42"/>
-      <c r="Q23" s="42"/>
-      <c r="R23" s="42"/>
-      <c r="S23" s="42"/>
-      <c r="T23" s="42"/>
-      <c r="U23" s="42"/>
-      <c r="V23" s="42"/>
-      <c r="W23" s="42"/>
-      <c r="X23" s="42"/>
-      <c r="Y23" s="42"/>
-      <c r="Z23" s="42"/>
-      <c r="AA23" s="42"/>
-      <c r="AB23" s="42"/>
-      <c r="AC23" s="42"/>
-      <c r="AD23" s="42"/>
-      <c r="AE23" s="42"/>
-      <c r="AF23" s="42"/>
-      <c r="AG23" s="42"/>
-      <c r="AH23" s="42"/>
-      <c r="AI23" s="42"/>
-      <c r="AJ23" s="42"/>
-      <c r="AK23" s="42"/>
-      <c r="AL23" s="42"/>
-      <c r="AM23" s="42"/>
-      <c r="AN23" s="42"/>
-      <c r="AO23" s="42"/>
-      <c r="AP23" s="42"/>
-      <c r="AQ23" s="42"/>
-      <c r="AR23" s="42"/>
-      <c r="AS23" s="42"/>
-      <c r="AT23" s="42"/>
-      <c r="AU23" s="42"/>
-      <c r="AV23" s="42"/>
-      <c r="AW23" s="42"/>
-      <c r="AX23" s="42"/>
-      <c r="AY23" s="42"/>
-      <c r="AZ23" s="42"/>
-      <c r="BA23" s="42"/>
-      <c r="BB23" s="42"/>
-      <c r="BC23" s="42"/>
-      <c r="BD23" s="42">
-        <v>0</v>
-      </c>
-      <c r="BE23" s="42"/>
-      <c r="BF23" s="73">
-        <v>100</v>
-      </c>
-      <c r="BG23" s="73"/>
-      <c r="BH23" s="73"/>
-      <c r="BI23" s="73"/>
-      <c r="BJ23" s="73"/>
-      <c r="BK23" s="73"/>
-      <c r="BL23" s="73"/>
-      <c r="BM23" s="73">
-        <v>100</v>
-      </c>
-      <c r="BN23" s="73"/>
-      <c r="BO23" s="73"/>
-      <c r="BP23" s="73">
-        <v>100</v>
-      </c>
-      <c r="BQ23" s="42"/>
-      <c r="BR23" s="42"/>
-      <c r="BS23" s="42"/>
-      <c r="BT23" s="42"/>
-      <c r="BU23" s="42"/>
-      <c r="BV23" s="42"/>
-      <c r="BW23" s="42"/>
-      <c r="BX23" s="42"/>
+      <c r="BA23" s="53">
+        <v>107.3</v>
+      </c>
+      <c r="BB23" s="53">
+        <v>110.9</v>
+      </c>
+      <c r="BC23" s="53">
+        <v>114.2</v>
+      </c>
+      <c r="BD23" s="53">
+        <v>114.8</v>
+      </c>
+      <c r="BE23" s="53">
+        <v>116.4</v>
+      </c>
+      <c r="BF23" s="68"/>
+      <c r="BG23" s="68"/>
+      <c r="BH23" s="68"/>
+      <c r="BI23" s="68"/>
+      <c r="BJ23" s="68"/>
+      <c r="BK23" s="68"/>
+      <c r="BL23" s="68"/>
+      <c r="BM23" s="68"/>
+      <c r="BN23" s="68"/>
+      <c r="BO23" s="68"/>
+      <c r="BP23" s="68"/>
     </row>
     <row r="24" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>3</v>
@@ -3772,546 +3864,200 @@
       <c r="D24" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="47">
+      <c r="E24" s="43">
+        <v>1</v>
+      </c>
+      <c r="F24" s="15">
+        <v>1</v>
+      </c>
+      <c r="G24" s="15">
+        <v>1</v>
+      </c>
+      <c r="H24" s="15">
+        <v>1</v>
+      </c>
+      <c r="I24" s="15">
+        <v>1</v>
+      </c>
+      <c r="J24" s="15">
+        <v>1</v>
+      </c>
+      <c r="K24" s="15">
+        <v>1</v>
+      </c>
+      <c r="L24" s="15">
+        <v>1</v>
+      </c>
+      <c r="M24" s="15">
+        <v>1</v>
+      </c>
+      <c r="N24" s="15">
+        <v>1</v>
+      </c>
+      <c r="O24" s="15">
+        <v>1</v>
+      </c>
+      <c r="P24" s="15">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="15">
+        <v>1</v>
+      </c>
+      <c r="R24" s="15">
+        <v>1</v>
+      </c>
+      <c r="S24" s="15">
+        <v>1</v>
+      </c>
+      <c r="T24" s="15">
+        <v>1</v>
+      </c>
+      <c r="U24" s="15">
+        <v>1</v>
+      </c>
+      <c r="V24" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="BA24" s="15">
+        <v>3.11</v>
+      </c>
+      <c r="BF24" s="65"/>
+      <c r="BG24" s="65"/>
+      <c r="BH24" s="65"/>
+      <c r="BI24" s="65"/>
+      <c r="BJ24" s="65"/>
+      <c r="BK24" s="65"/>
+      <c r="BL24" s="65"/>
+      <c r="BM24" s="65"/>
+      <c r="BN24" s="65"/>
+      <c r="BO24" s="65"/>
+      <c r="BP24" s="65"/>
+    </row>
+    <row r="25" spans="1:76" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="58"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="44"/>
+      <c r="BF25" s="66"/>
+      <c r="BG25" s="66"/>
+      <c r="BH25" s="66"/>
+      <c r="BI25" s="66"/>
+      <c r="BJ25" s="66"/>
+      <c r="BK25" s="66"/>
+      <c r="BL25" s="66"/>
+      <c r="BM25" s="66"/>
+      <c r="BN25" s="66"/>
+      <c r="BO25" s="66"/>
+      <c r="BP25" s="66"/>
+    </row>
+    <row r="26" spans="1:76" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="29">
+        <v>1</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="44">
+        <v>1</v>
+      </c>
+      <c r="BD26" s="30">
+        <v>1</v>
+      </c>
+      <c r="BF26" s="66"/>
+      <c r="BG26" s="66"/>
+      <c r="BH26" s="66"/>
+      <c r="BI26" s="66"/>
+      <c r="BJ26" s="66"/>
+      <c r="BK26" s="66"/>
+      <c r="BL26" s="66"/>
+      <c r="BM26" s="66"/>
+      <c r="BN26" s="66"/>
+      <c r="BO26" s="66"/>
+      <c r="BP26" s="66"/>
+    </row>
+    <row r="27" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A27" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="45">
         <v>0</v>
       </c>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="42"/>
-      <c r="O24" s="42"/>
-      <c r="P24" s="42"/>
-      <c r="Q24" s="42"/>
-      <c r="R24" s="42"/>
-      <c r="S24" s="42"/>
-      <c r="T24" s="42"/>
-      <c r="U24" s="42"/>
-      <c r="V24" s="42"/>
-      <c r="W24" s="42"/>
-      <c r="X24" s="42"/>
-      <c r="Y24" s="42"/>
-      <c r="Z24" s="42"/>
-      <c r="AA24" s="42"/>
-      <c r="AB24" s="42"/>
-      <c r="AC24" s="42"/>
-      <c r="AD24" s="42"/>
-      <c r="AE24" s="42"/>
-      <c r="AF24" s="42"/>
-      <c r="AG24" s="42"/>
-      <c r="AH24" s="42"/>
-      <c r="AI24" s="42"/>
-      <c r="AJ24" s="42"/>
-      <c r="AK24" s="42"/>
-      <c r="AL24" s="42"/>
-      <c r="AM24" s="42"/>
-      <c r="AN24" s="42"/>
-      <c r="AO24" s="42"/>
-      <c r="AP24" s="42"/>
-      <c r="AQ24" s="42"/>
-      <c r="AR24" s="42"/>
-      <c r="AS24" s="42"/>
-      <c r="AT24" s="42"/>
-      <c r="AU24" s="42"/>
-      <c r="AV24" s="42"/>
-      <c r="AW24" s="42"/>
-      <c r="AX24" s="42"/>
-      <c r="AY24" s="42"/>
-      <c r="AZ24" s="42"/>
-      <c r="BA24" s="42"/>
-      <c r="BB24" s="42"/>
-      <c r="BC24" s="42"/>
-      <c r="BD24" s="42">
+      <c r="K27" s="1">
         <v>0</v>
       </c>
-      <c r="BE24" s="42"/>
-      <c r="BF24" s="73"/>
-      <c r="BG24" s="73"/>
-      <c r="BH24" s="73">
-        <v>17</v>
-      </c>
-      <c r="BI24" s="73">
-        <v>70</v>
-      </c>
-      <c r="BJ24" s="73"/>
-      <c r="BK24" s="73"/>
-      <c r="BL24" s="73"/>
-      <c r="BM24" s="73">
-        <v>70</v>
-      </c>
-      <c r="BN24" s="73"/>
-      <c r="BO24" s="73"/>
-      <c r="BP24" s="73">
-        <v>70</v>
-      </c>
-      <c r="BQ24" s="42"/>
-      <c r="BR24" s="42"/>
-      <c r="BS24" s="42"/>
-      <c r="BT24" s="42"/>
-      <c r="BU24" s="42"/>
-      <c r="BV24" s="42"/>
-      <c r="BW24" s="42"/>
-      <c r="BX24" s="42"/>
-    </row>
-    <row r="25" spans="1:76" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="52" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="52">
-        <v>1</v>
-      </c>
-      <c r="D25" s="52" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="53"/>
-      <c r="BD25" s="54">
+      <c r="T27" s="1">
         <v>0</v>
       </c>
-      <c r="BF25" s="67"/>
-      <c r="BG25" s="67"/>
-      <c r="BH25" s="67"/>
-      <c r="BI25" s="67"/>
-      <c r="BJ25" s="67"/>
-      <c r="BK25" s="67"/>
-      <c r="BL25" s="67"/>
-      <c r="BM25" s="67"/>
-      <c r="BN25" s="67"/>
-      <c r="BO25" s="67"/>
-      <c r="BP25" s="67"/>
-    </row>
-    <row r="26" spans="1:76" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="51" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="52" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="52">
-        <v>1</v>
-      </c>
-      <c r="D26" s="52" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" s="53"/>
-      <c r="BD26" s="54">
-        <v>0</v>
-      </c>
-      <c r="BF26" s="67"/>
-      <c r="BG26" s="67"/>
-      <c r="BH26" s="67"/>
-      <c r="BI26" s="67"/>
-      <c r="BJ26" s="67"/>
-      <c r="BK26" s="67">
-        <v>50</v>
-      </c>
-      <c r="BL26" s="67"/>
-      <c r="BM26" s="67">
-        <v>50</v>
-      </c>
-      <c r="BN26" s="67"/>
-      <c r="BO26" s="67"/>
-      <c r="BP26" s="67">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:76" s="58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="56" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="56">
-        <v>1</v>
-      </c>
-      <c r="D27" s="56" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" s="57">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="F27" s="58">
-        <v>4.84</v>
-      </c>
-      <c r="G27" s="58">
-        <v>5.44</v>
-      </c>
-      <c r="H27" s="58">
-        <v>6.11</v>
-      </c>
-      <c r="I27" s="58">
-        <v>6.86</v>
-      </c>
-      <c r="J27" s="58">
+      <c r="V27" s="1">
         <v>7.7</v>
       </c>
-      <c r="K27" s="58">
-        <v>8.68</v>
-      </c>
-      <c r="L27" s="58">
-        <v>9.0399999999999991</v>
-      </c>
-      <c r="M27" s="58">
-        <v>9.41</v>
-      </c>
-      <c r="N27" s="58">
-        <v>11.48</v>
-      </c>
-      <c r="O27" s="58">
-        <v>12.75</v>
-      </c>
-      <c r="P27" s="58">
-        <v>14.6</v>
-      </c>
-      <c r="Q27" s="58">
+      <c r="AI27" s="1">
+        <v>11.1</v>
+      </c>
+      <c r="AR27" s="1">
         <v>16.5</v>
       </c>
-      <c r="R27" s="58">
-        <v>18.38</v>
-      </c>
-      <c r="S27" s="58">
-        <v>19.670000000000002</v>
-      </c>
-      <c r="T27" s="58">
-        <v>20.87</v>
-      </c>
-      <c r="U27" s="58">
-        <v>22.5</v>
-      </c>
-      <c r="V27" s="58">
-        <v>25.9</v>
-      </c>
-      <c r="W27" s="58">
-        <v>28.8</v>
-      </c>
-      <c r="X27" s="58">
-        <v>30.8</v>
-      </c>
-      <c r="Y27" s="58">
-        <v>32.9</v>
-      </c>
-      <c r="Z27" s="58">
-        <v>34.6</v>
-      </c>
-      <c r="AA27" s="58">
-        <v>36.1</v>
-      </c>
-      <c r="AB27" s="58">
-        <v>36.799999999999997</v>
-      </c>
-      <c r="AC27" s="58">
-        <v>38.9</v>
-      </c>
-      <c r="AD27" s="58">
-        <v>43.4</v>
-      </c>
-      <c r="AE27" s="58">
-        <v>46.1</v>
-      </c>
-      <c r="AF27" s="58">
-        <v>49.9</v>
-      </c>
-      <c r="AG27" s="58">
-        <v>53.1</v>
-      </c>
-      <c r="AH27" s="58">
-        <v>55.7</v>
-      </c>
-      <c r="AI27" s="58">
-        <v>58.6</v>
-      </c>
-      <c r="AJ27" s="58">
-        <v>59.1</v>
-      </c>
-      <c r="AK27" s="58">
-        <v>60.4</v>
-      </c>
-      <c r="AL27" s="58">
-        <v>62.2</v>
-      </c>
-      <c r="AM27" s="58">
-        <v>64.3</v>
-      </c>
-      <c r="AN27" s="58">
-        <v>68</v>
-      </c>
-      <c r="AO27" s="58">
-        <v>69.3</v>
-      </c>
-      <c r="AP27" s="58">
-        <v>70.099999999999994</v>
-      </c>
-      <c r="AQ27" s="58">
-        <v>73.099999999999994</v>
-      </c>
-      <c r="AR27" s="58">
-        <v>73.599999999999994</v>
-      </c>
-      <c r="AS27" s="58">
-        <v>76.7</v>
-      </c>
-      <c r="AT27" s="58">
-        <v>78.900000000000006</v>
-      </c>
-      <c r="AU27" s="58">
-        <v>80.8</v>
-      </c>
-      <c r="AV27" s="58">
-        <v>82.8</v>
-      </c>
-      <c r="AW27" s="58">
-        <v>86.7</v>
-      </c>
-      <c r="AX27" s="58">
-        <v>93.4</v>
-      </c>
-      <c r="AY27" s="58">
-        <v>96.5</v>
-      </c>
-      <c r="AZ27" s="58">
-        <v>100</v>
-      </c>
-      <c r="BA27" s="58">
-        <v>107.3</v>
-      </c>
-      <c r="BB27" s="58">
-        <v>110.9</v>
-      </c>
-      <c r="BC27" s="58">
-        <v>114.2</v>
-      </c>
-      <c r="BD27" s="58">
-        <v>114.8</v>
-      </c>
-      <c r="BE27" s="58">
-        <v>116.4</v>
-      </c>
-      <c r="BF27" s="74"/>
-      <c r="BG27" s="74"/>
-      <c r="BH27" s="74"/>
-      <c r="BI27" s="74"/>
-      <c r="BJ27" s="74"/>
-      <c r="BK27" s="74"/>
-      <c r="BL27" s="74"/>
-      <c r="BM27" s="74"/>
-      <c r="BN27" s="74"/>
-      <c r="BO27" s="74"/>
-      <c r="BP27" s="74"/>
-    </row>
-    <row r="28" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="14">
-        <v>1</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="47">
-        <v>1</v>
-      </c>
-      <c r="F28" s="15">
-        <v>1</v>
-      </c>
-      <c r="G28" s="15">
-        <v>1</v>
-      </c>
-      <c r="H28" s="15">
-        <v>1</v>
-      </c>
-      <c r="I28" s="15">
-        <v>1</v>
-      </c>
-      <c r="J28" s="15">
-        <v>1</v>
-      </c>
-      <c r="K28" s="15">
-        <v>1</v>
-      </c>
-      <c r="L28" s="15">
-        <v>1</v>
-      </c>
-      <c r="M28" s="15">
-        <v>1</v>
-      </c>
-      <c r="N28" s="15">
-        <v>1</v>
-      </c>
-      <c r="O28" s="15">
-        <v>1</v>
-      </c>
-      <c r="P28" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q28" s="15">
-        <v>1</v>
-      </c>
-      <c r="R28" s="15">
-        <v>1</v>
-      </c>
-      <c r="S28" s="15">
-        <v>1</v>
-      </c>
-      <c r="T28" s="15">
-        <v>1</v>
-      </c>
-      <c r="U28" s="15">
-        <v>1</v>
-      </c>
-      <c r="V28" s="15">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="BA28" s="15">
-        <v>3.11</v>
-      </c>
-      <c r="BF28" s="70"/>
-      <c r="BG28" s="70"/>
-      <c r="BH28" s="70"/>
-      <c r="BI28" s="70"/>
-      <c r="BJ28" s="70"/>
-      <c r="BK28" s="70"/>
-      <c r="BL28" s="70"/>
-      <c r="BM28" s="70"/>
-      <c r="BN28" s="70"/>
-      <c r="BO28" s="70"/>
-      <c r="BP28" s="70"/>
-    </row>
-    <row r="29" spans="1:76" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="63"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="49"/>
-      <c r="BF29" s="72"/>
-      <c r="BG29" s="72"/>
-      <c r="BH29" s="72"/>
-      <c r="BI29" s="72"/>
-      <c r="BJ29" s="72"/>
-      <c r="BK29" s="72"/>
-      <c r="BL29" s="72"/>
-      <c r="BM29" s="72"/>
-      <c r="BN29" s="72"/>
-      <c r="BO29" s="72"/>
-      <c r="BP29" s="72"/>
-    </row>
-    <row r="30" spans="1:76" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="63" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="33">
-        <v>1</v>
-      </c>
-      <c r="D30" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30" s="49">
-        <v>1</v>
-      </c>
-      <c r="BD30" s="34">
-        <v>1</v>
-      </c>
-      <c r="BF30" s="72"/>
-      <c r="BG30" s="72"/>
-      <c r="BH30" s="72"/>
-      <c r="BI30" s="72"/>
-      <c r="BJ30" s="72"/>
-      <c r="BK30" s="72"/>
-      <c r="BL30" s="72"/>
-      <c r="BM30" s="72"/>
-      <c r="BN30" s="72"/>
-      <c r="BO30" s="72"/>
-      <c r="BP30" s="72"/>
-    </row>
-    <row r="31" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="A31" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" s="2">
-        <v>1</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E31" s="50">
-        <v>0</v>
-      </c>
-      <c r="K31" s="1">
-        <v>0</v>
-      </c>
-      <c r="T31" s="1">
-        <v>0</v>
-      </c>
-      <c r="V31" s="1">
-        <v>7.7</v>
-      </c>
-      <c r="AI31" s="1">
-        <v>11.1</v>
-      </c>
-      <c r="AR31" s="1">
-        <v>16.5</v>
-      </c>
-      <c r="AT31" s="1">
+      <c r="AT27" s="1">
         <v>14.5</v>
       </c>
-      <c r="AY31" s="1">
+      <c r="AY27" s="1">
         <v>16.100000000000001</v>
       </c>
-      <c r="BA31" s="1">
+      <c r="BA27" s="1">
         <v>15.6</v>
       </c>
-      <c r="BC31" s="1">
+      <c r="BC27" s="1">
         <v>15.6</v>
       </c>
-      <c r="BE31" s="1">
+      <c r="BE27" s="1">
         <v>15.6</v>
       </c>
-      <c r="BF31" s="75"/>
-      <c r="BG31" s="75"/>
-      <c r="BH31" s="75"/>
-      <c r="BI31" s="75"/>
-      <c r="BJ31" s="75"/>
-      <c r="BK31" s="75"/>
-      <c r="BL31" s="75"/>
-      <c r="BM31" s="75"/>
-      <c r="BN31" s="75"/>
-      <c r="BO31" s="75"/>
-      <c r="BP31" s="75"/>
+      <c r="BF27" s="69"/>
+      <c r="BG27" s="69"/>
+      <c r="BH27" s="69"/>
+      <c r="BI27" s="69"/>
+      <c r="BJ27" s="69"/>
+      <c r="BK27" s="69"/>
+      <c r="BL27" s="69"/>
+      <c r="BM27" s="69"/>
+      <c r="BN27" s="69"/>
+      <c r="BO27" s="69"/>
+      <c r="BP27" s="69"/>
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="5">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF22:BG22 F5:BG8">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF18:BG18 F5:BG8">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:D1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F12:BG21 F22:BE22 F2:BG4">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F12:BG17 F18:BE18 F2:BG4">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C31:C1048576 C2:C28">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C27:C1048576 C2:C24">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Leave blank" sqref="B29:D30"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Leave blank" sqref="B25:D26"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4322,13 +4068,13 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B8 B12:B22</xm:sqref>
+          <xm:sqref>B2:B8 B12:B18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time-variant?" prompt="If no, the most recent value will be selected.">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D31:D1048576 D2:D28</xm:sqref>
+          <xm:sqref>D27:D1048576 D2:D24</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Enable selection of whether to consider IPT in model
As for other non-compulsory interventions, skip over IPT if not being
implemented.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="57">
   <si>
     <t>parameter</t>
   </si>
@@ -175,12 +175,6 @@
   </si>
   <si>
     <t>program_perc_novel_ipt</t>
-  </si>
-  <si>
-    <t>program_perc_novel_ipt_age0to5</t>
-  </si>
-  <si>
-    <t>program_perc_novel_ipt_age5to15</t>
   </si>
   <si>
     <t>program_perc_novel_vaccination</t>
@@ -2373,13 +2367,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BX27"/>
+  <dimension ref="A1:BX25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2617,7 +2611,7 @@
         <v>27</v>
       </c>
       <c r="BQ1" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:69" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2690,7 +2684,7 @@
     </row>
     <row r="3" spans="1:69" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>4</v>
@@ -2965,7 +2959,7 @@
     </row>
     <row r="8" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>4</v>
@@ -3030,1034 +3024,928 @@
       <c r="BO9" s="62"/>
       <c r="BP9" s="62"/>
     </row>
-    <row r="10" spans="1:69" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="47" t="s">
+    <row r="10" spans="1:69" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="47">
+      <c r="C10" s="10">
         <v>1</v>
       </c>
-      <c r="D10" s="47" t="s">
+      <c r="D10" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="48">
+      <c r="E10" s="41"/>
+      <c r="F10" s="11">
+        <v>70</v>
+      </c>
+      <c r="J10" s="11">
+        <v>80</v>
+      </c>
+      <c r="AD10" s="11">
+        <v>82</v>
+      </c>
+      <c r="AQ10" s="11">
+        <v>84</v>
+      </c>
+      <c r="BC10" s="11">
+        <v>85</v>
+      </c>
+      <c r="BF10" s="63"/>
+      <c r="BG10" s="63"/>
+      <c r="BH10" s="63"/>
+      <c r="BI10" s="63"/>
+      <c r="BJ10" s="63"/>
+      <c r="BK10" s="63"/>
+      <c r="BL10" s="63"/>
+      <c r="BM10" s="63"/>
+      <c r="BN10" s="63"/>
+      <c r="BO10" s="63"/>
+      <c r="BP10" s="63"/>
+    </row>
+    <row r="11" spans="1:69" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="12">
+        <v>1</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="42"/>
+      <c r="H11" s="13">
+        <v>30</v>
+      </c>
+      <c r="K11" s="13">
+        <v>40</v>
+      </c>
+      <c r="AF11" s="13">
+        <v>40</v>
+      </c>
+      <c r="BF11" s="64"/>
+      <c r="BG11" s="64"/>
+      <c r="BH11" s="64"/>
+      <c r="BI11" s="64"/>
+      <c r="BJ11" s="64"/>
+      <c r="BK11" s="64"/>
+      <c r="BL11" s="64"/>
+      <c r="BM11" s="64"/>
+      <c r="BN11" s="64"/>
+      <c r="BO11" s="64"/>
+      <c r="BP11" s="64"/>
+    </row>
+    <row r="12" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="14">
+        <v>1</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="43"/>
+      <c r="V12" s="15">
+        <v>30</v>
+      </c>
+      <c r="AF12" s="15">
+        <v>40</v>
+      </c>
+      <c r="AP12" s="15">
+        <v>50</v>
+      </c>
+      <c r="BF12" s="65"/>
+      <c r="BG12" s="65"/>
+      <c r="BH12" s="65"/>
+      <c r="BI12" s="65"/>
+      <c r="BJ12" s="65"/>
+      <c r="BK12" s="65"/>
+      <c r="BL12" s="65"/>
+      <c r="BM12" s="65"/>
+      <c r="BN12" s="65"/>
+      <c r="BO12" s="65"/>
+      <c r="BP12" s="65"/>
+    </row>
+    <row r="13" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="14">
+        <v>1</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="43"/>
+      <c r="I13" s="15">
+        <v>7</v>
+      </c>
+      <c r="AK13" s="15">
+        <v>50</v>
+      </c>
+      <c r="AP13" s="15">
+        <v>70</v>
+      </c>
+      <c r="BF13" s="65"/>
+      <c r="BG13" s="65"/>
+      <c r="BH13" s="65"/>
+      <c r="BI13" s="65"/>
+      <c r="BJ13" s="65"/>
+      <c r="BK13" s="65"/>
+      <c r="BL13" s="65"/>
+      <c r="BM13" s="65"/>
+      <c r="BN13" s="65"/>
+      <c r="BO13" s="65"/>
+      <c r="BP13" s="65"/>
+    </row>
+    <row r="14" spans="1:69" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="12">
+        <v>1</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="42"/>
+      <c r="I14" s="13">
         <v>0</v>
       </c>
-      <c r="BD10" s="49">
+      <c r="V14" s="13">
+        <v>40</v>
+      </c>
+      <c r="AB14" s="13">
+        <v>65</v>
+      </c>
+      <c r="AK14" s="24"/>
+      <c r="AL14" s="24"/>
+      <c r="AM14" s="24"/>
+      <c r="AN14" s="24"/>
+      <c r="AO14" s="24"/>
+      <c r="AP14" s="24"/>
+      <c r="AQ14" s="24"/>
+      <c r="AR14" s="24"/>
+      <c r="AS14" s="24"/>
+      <c r="AT14" s="24"/>
+      <c r="AU14" s="24"/>
+      <c r="AV14" s="24"/>
+      <c r="AW14" s="24"/>
+      <c r="AX14" s="24"/>
+      <c r="AY14" s="24"/>
+      <c r="AZ14" s="24"/>
+      <c r="BA14" s="24"/>
+      <c r="BB14" s="24">
+        <v>93</v>
+      </c>
+      <c r="BC14" s="24">
+        <v>85</v>
+      </c>
+      <c r="BF14" s="64"/>
+      <c r="BG14" s="64">
+        <v>96</v>
+      </c>
+      <c r="BH14" s="64"/>
+      <c r="BI14" s="64"/>
+      <c r="BJ14" s="64"/>
+      <c r="BK14" s="64"/>
+      <c r="BL14" s="64"/>
+      <c r="BM14" s="64"/>
+      <c r="BN14" s="64"/>
+      <c r="BO14" s="64"/>
+      <c r="BP14" s="64"/>
+    </row>
+    <row r="15" spans="1:69" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="12">
+        <v>3</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="42"/>
+      <c r="I15" s="13">
         <v>0</v>
       </c>
-      <c r="BF10" s="62"/>
-      <c r="BG10" s="62"/>
-      <c r="BH10" s="62"/>
-      <c r="BI10" s="62"/>
-      <c r="BJ10" s="62"/>
-      <c r="BK10" s="62"/>
-      <c r="BL10" s="62"/>
-      <c r="BM10" s="62"/>
-      <c r="BN10" s="62"/>
-      <c r="BO10" s="62"/>
-      <c r="BP10" s="62"/>
+      <c r="V15" s="13">
+        <v>10</v>
+      </c>
+      <c r="AB15" s="13">
+        <v>8</v>
+      </c>
+      <c r="AK15" s="24"/>
+      <c r="AL15" s="24"/>
+      <c r="AM15" s="24"/>
+      <c r="AN15" s="24"/>
+      <c r="AO15" s="24"/>
+      <c r="AP15" s="24"/>
+      <c r="AQ15" s="24"/>
+      <c r="AR15" s="24"/>
+      <c r="AS15" s="24"/>
+      <c r="AT15" s="24"/>
+      <c r="AU15" s="24"/>
+      <c r="AV15" s="24"/>
+      <c r="AW15" s="24"/>
+      <c r="AX15" s="24"/>
+      <c r="AY15" s="24"/>
+      <c r="AZ15" s="24"/>
+      <c r="BA15" s="24"/>
+      <c r="BB15" s="24"/>
+      <c r="BC15" s="24"/>
+      <c r="BD15" s="13">
+        <v>5</v>
+      </c>
+      <c r="BF15" s="64"/>
+      <c r="BG15" s="64">
+        <v>1.3</v>
+      </c>
+      <c r="BH15" s="64"/>
+      <c r="BI15" s="64"/>
+      <c r="BJ15" s="64"/>
+      <c r="BK15" s="64"/>
+      <c r="BL15" s="64"/>
+      <c r="BM15" s="64"/>
+      <c r="BN15" s="64"/>
+      <c r="BO15" s="64"/>
+      <c r="BP15" s="64"/>
     </row>
-    <row r="11" spans="1:69" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="46" t="s">
+    <row r="16" spans="1:69" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="29">
+        <v>1</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="44"/>
+      <c r="AK16" s="31"/>
+      <c r="AL16" s="31"/>
+      <c r="AM16" s="31"/>
+      <c r="AN16" s="31"/>
+      <c r="AO16" s="31"/>
+      <c r="AP16" s="31"/>
+      <c r="AQ16" s="31"/>
+      <c r="AR16" s="31"/>
+      <c r="AS16" s="31"/>
+      <c r="AT16" s="31"/>
+      <c r="AU16" s="31"/>
+      <c r="AV16" s="31"/>
+      <c r="AW16" s="31"/>
+      <c r="AX16" s="31"/>
+      <c r="AY16" s="31"/>
+      <c r="AZ16" s="31"/>
+      <c r="BA16" s="31"/>
+      <c r="BB16" s="31"/>
+      <c r="BC16" s="31"/>
+      <c r="BD16" s="30">
+        <v>0</v>
+      </c>
+      <c r="BF16" s="66"/>
+      <c r="BG16" s="66"/>
+      <c r="BH16" s="66"/>
+      <c r="BI16" s="66"/>
+      <c r="BJ16" s="66">
+        <v>100</v>
+      </c>
+      <c r="BK16" s="66"/>
+      <c r="BL16" s="66"/>
+      <c r="BM16" s="66">
+        <v>100</v>
+      </c>
+      <c r="BN16" s="66"/>
+      <c r="BO16" s="66"/>
+      <c r="BP16" s="66">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="14">
+        <v>1</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="43"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="38"/>
+      <c r="S17" s="38"/>
+      <c r="T17" s="38"/>
+      <c r="U17" s="38"/>
+      <c r="V17" s="38"/>
+      <c r="W17" s="38"/>
+      <c r="X17" s="38"/>
+      <c r="Y17" s="38"/>
+      <c r="Z17" s="38"/>
+      <c r="AA17" s="38"/>
+      <c r="AB17" s="38"/>
+      <c r="AC17" s="38"/>
+      <c r="AD17" s="38"/>
+      <c r="AE17" s="38"/>
+      <c r="AF17" s="38"/>
+      <c r="AG17" s="38"/>
+      <c r="AH17" s="38"/>
+      <c r="AI17" s="38"/>
+      <c r="AJ17" s="38"/>
+      <c r="AK17" s="38"/>
+      <c r="AL17" s="38"/>
+      <c r="AM17" s="38"/>
+      <c r="AN17" s="38"/>
+      <c r="AO17" s="38"/>
+      <c r="AP17" s="38"/>
+      <c r="AQ17" s="38"/>
+      <c r="AR17" s="38"/>
+      <c r="AS17" s="38"/>
+      <c r="AT17" s="38"/>
+      <c r="AU17" s="38"/>
+      <c r="AV17" s="38"/>
+      <c r="AW17" s="38"/>
+      <c r="AX17" s="38"/>
+      <c r="AY17" s="38"/>
+      <c r="AZ17" s="38"/>
+      <c r="BA17" s="38"/>
+      <c r="BB17" s="38"/>
+      <c r="BC17" s="38"/>
+      <c r="BD17" s="38">
+        <v>0</v>
+      </c>
+      <c r="BE17" s="38"/>
+      <c r="BF17" s="67">
+        <v>100</v>
+      </c>
+      <c r="BG17" s="67"/>
+      <c r="BH17" s="67"/>
+      <c r="BI17" s="67"/>
+      <c r="BJ17" s="67"/>
+      <c r="BK17" s="67"/>
+      <c r="BL17" s="67"/>
+      <c r="BM17" s="67">
+        <v>100</v>
+      </c>
+      <c r="BN17" s="67"/>
+      <c r="BO17" s="67"/>
+      <c r="BP17" s="67">
+        <v>100</v>
+      </c>
+      <c r="BQ17" s="38"/>
+      <c r="BR17" s="38"/>
+      <c r="BS17" s="38"/>
+      <c r="BT17" s="38"/>
+      <c r="BU17" s="38"/>
+      <c r="BV17" s="38"/>
+      <c r="BW17" s="38"/>
+      <c r="BX17" s="38"/>
+    </row>
+    <row r="18" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="14">
+        <v>1</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="43">
+        <v>0</v>
+      </c>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="38"/>
+      <c r="R18" s="38"/>
+      <c r="S18" s="38"/>
+      <c r="T18" s="38"/>
+      <c r="U18" s="38"/>
+      <c r="V18" s="38"/>
+      <c r="W18" s="38"/>
+      <c r="X18" s="38"/>
+      <c r="Y18" s="38"/>
+      <c r="Z18" s="38"/>
+      <c r="AA18" s="38"/>
+      <c r="AB18" s="38"/>
+      <c r="AC18" s="38"/>
+      <c r="AD18" s="38"/>
+      <c r="AE18" s="38"/>
+      <c r="AF18" s="38"/>
+      <c r="AG18" s="38"/>
+      <c r="AH18" s="38"/>
+      <c r="AI18" s="38"/>
+      <c r="AJ18" s="38"/>
+      <c r="AK18" s="38"/>
+      <c r="AL18" s="38"/>
+      <c r="AM18" s="38"/>
+      <c r="AN18" s="38"/>
+      <c r="AO18" s="38"/>
+      <c r="AP18" s="38"/>
+      <c r="AQ18" s="38"/>
+      <c r="AR18" s="38"/>
+      <c r="AS18" s="38"/>
+      <c r="AT18" s="38"/>
+      <c r="AU18" s="38"/>
+      <c r="AV18" s="38"/>
+      <c r="AW18" s="38"/>
+      <c r="AX18" s="38"/>
+      <c r="AY18" s="38"/>
+      <c r="AZ18" s="38"/>
+      <c r="BA18" s="38"/>
+      <c r="BB18" s="38"/>
+      <c r="BC18" s="38"/>
+      <c r="BD18" s="38">
+        <v>0</v>
+      </c>
+      <c r="BE18" s="38"/>
+      <c r="BF18" s="67"/>
+      <c r="BG18" s="67"/>
+      <c r="BH18" s="67">
+        <v>17</v>
+      </c>
+      <c r="BI18" s="67">
+        <v>70</v>
+      </c>
+      <c r="BJ18" s="67"/>
+      <c r="BK18" s="67"/>
+      <c r="BL18" s="67"/>
+      <c r="BM18" s="67">
+        <v>70</v>
+      </c>
+      <c r="BN18" s="67"/>
+      <c r="BO18" s="67"/>
+      <c r="BP18" s="67">
+        <v>70</v>
+      </c>
+      <c r="BQ18" s="38"/>
+      <c r="BR18" s="38"/>
+      <c r="BS18" s="38"/>
+      <c r="BT18" s="38"/>
+      <c r="BU18" s="38"/>
+      <c r="BV18" s="38"/>
+      <c r="BW18" s="38"/>
+      <c r="BX18" s="38"/>
+    </row>
+    <row r="19" spans="1:76" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="47">
+        <v>1</v>
+      </c>
+      <c r="D19" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="48"/>
+      <c r="BD19" s="49">
+        <v>0</v>
+      </c>
+      <c r="BF19" s="62"/>
+      <c r="BG19" s="62"/>
+      <c r="BH19" s="62"/>
+      <c r="BI19" s="62"/>
+      <c r="BJ19" s="62"/>
+      <c r="BK19" s="62"/>
+      <c r="BL19" s="62"/>
+      <c r="BM19" s="62"/>
+      <c r="BN19" s="62"/>
+      <c r="BO19" s="62"/>
+      <c r="BP19" s="62"/>
+    </row>
+    <row r="20" spans="1:76" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="47">
+        <v>1</v>
+      </c>
+      <c r="D20" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="48"/>
+      <c r="BD20" s="49">
+        <v>0</v>
+      </c>
+      <c r="BF20" s="62"/>
+      <c r="BG20" s="62"/>
+      <c r="BH20" s="62"/>
+      <c r="BI20" s="62"/>
+      <c r="BJ20" s="62"/>
+      <c r="BK20" s="62">
+        <v>50</v>
+      </c>
+      <c r="BL20" s="62"/>
+      <c r="BM20" s="62">
+        <v>50</v>
+      </c>
+      <c r="BN20" s="62"/>
+      <c r="BO20" s="62"/>
+      <c r="BP20" s="62">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:76" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="51">
+        <v>1</v>
+      </c>
+      <c r="D21" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="52">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="F21" s="53">
+        <v>4.84</v>
+      </c>
+      <c r="G21" s="53">
+        <v>5.44</v>
+      </c>
+      <c r="H21" s="53">
+        <v>6.11</v>
+      </c>
+      <c r="I21" s="53">
+        <v>6.86</v>
+      </c>
+      <c r="J21" s="53">
+        <v>7.7</v>
+      </c>
+      <c r="K21" s="53">
+        <v>8.68</v>
+      </c>
+      <c r="L21" s="53">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="M21" s="53">
+        <v>9.41</v>
+      </c>
+      <c r="N21" s="53">
+        <v>11.48</v>
+      </c>
+      <c r="O21" s="53">
+        <v>12.75</v>
+      </c>
+      <c r="P21" s="53">
+        <v>14.6</v>
+      </c>
+      <c r="Q21" s="53">
+        <v>16.5</v>
+      </c>
+      <c r="R21" s="53">
+        <v>18.38</v>
+      </c>
+      <c r="S21" s="53">
+        <v>19.670000000000002</v>
+      </c>
+      <c r="T21" s="53">
+        <v>20.87</v>
+      </c>
+      <c r="U21" s="53">
+        <v>22.5</v>
+      </c>
+      <c r="V21" s="53">
+        <v>25.9</v>
+      </c>
+      <c r="W21" s="53">
+        <v>28.8</v>
+      </c>
+      <c r="X21" s="53">
+        <v>30.8</v>
+      </c>
+      <c r="Y21" s="53">
+        <v>32.9</v>
+      </c>
+      <c r="Z21" s="53">
+        <v>34.6</v>
+      </c>
+      <c r="AA21" s="53">
+        <v>36.1</v>
+      </c>
+      <c r="AB21" s="53">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="AC21" s="53">
+        <v>38.9</v>
+      </c>
+      <c r="AD21" s="53">
+        <v>43.4</v>
+      </c>
+      <c r="AE21" s="53">
+        <v>46.1</v>
+      </c>
+      <c r="AF21" s="53">
+        <v>49.9</v>
+      </c>
+      <c r="AG21" s="53">
+        <v>53.1</v>
+      </c>
+      <c r="AH21" s="53">
+        <v>55.7</v>
+      </c>
+      <c r="AI21" s="53">
+        <v>58.6</v>
+      </c>
+      <c r="AJ21" s="53">
+        <v>59.1</v>
+      </c>
+      <c r="AK21" s="53">
+        <v>60.4</v>
+      </c>
+      <c r="AL21" s="53">
+        <v>62.2</v>
+      </c>
+      <c r="AM21" s="53">
+        <v>64.3</v>
+      </c>
+      <c r="AN21" s="53">
+        <v>68</v>
+      </c>
+      <c r="AO21" s="53">
+        <v>69.3</v>
+      </c>
+      <c r="AP21" s="53">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="AQ21" s="53">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="AR21" s="53">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="AS21" s="53">
+        <v>76.7</v>
+      </c>
+      <c r="AT21" s="53">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="AU21" s="53">
+        <v>80.8</v>
+      </c>
+      <c r="AV21" s="53">
+        <v>82.8</v>
+      </c>
+      <c r="AW21" s="53">
+        <v>86.7</v>
+      </c>
+      <c r="AX21" s="53">
+        <v>93.4</v>
+      </c>
+      <c r="AY21" s="53">
+        <v>96.5</v>
+      </c>
+      <c r="AZ21" s="53">
+        <v>100</v>
+      </c>
+      <c r="BA21" s="53">
+        <v>107.3</v>
+      </c>
+      <c r="BB21" s="53">
+        <v>110.9</v>
+      </c>
+      <c r="BC21" s="53">
+        <v>114.2</v>
+      </c>
+      <c r="BD21" s="53">
+        <v>114.8</v>
+      </c>
+      <c r="BE21" s="53">
+        <v>116.4</v>
+      </c>
+      <c r="BF21" s="68"/>
+      <c r="BG21" s="68"/>
+      <c r="BH21" s="68"/>
+      <c r="BI21" s="68"/>
+      <c r="BJ21" s="68"/>
+      <c r="BK21" s="68"/>
+      <c r="BL21" s="68"/>
+      <c r="BM21" s="68"/>
+      <c r="BN21" s="68"/>
+      <c r="BO21" s="68"/>
+      <c r="BP21" s="68"/>
+    </row>
+    <row r="22" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="14">
+        <v>1</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="43">
+        <v>1</v>
+      </c>
+      <c r="K22" s="15">
+        <v>1</v>
+      </c>
+      <c r="U22" s="15">
+        <v>1</v>
+      </c>
+      <c r="V22" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="BA22" s="15">
+        <v>3.11</v>
+      </c>
+      <c r="BF22" s="65"/>
+      <c r="BG22" s="65"/>
+      <c r="BH22" s="65"/>
+      <c r="BI22" s="65"/>
+      <c r="BJ22" s="65"/>
+      <c r="BK22" s="65"/>
+      <c r="BL22" s="65"/>
+      <c r="BM22" s="65"/>
+      <c r="BN22" s="65"/>
+      <c r="BO22" s="65"/>
+      <c r="BP22" s="65"/>
+    </row>
+    <row r="23" spans="1:76" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="58"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="44"/>
+      <c r="BF23" s="66"/>
+      <c r="BG23" s="66"/>
+      <c r="BH23" s="66"/>
+      <c r="BI23" s="66"/>
+      <c r="BJ23" s="66"/>
+      <c r="BK23" s="66"/>
+      <c r="BL23" s="66"/>
+      <c r="BM23" s="66"/>
+      <c r="BN23" s="66"/>
+      <c r="BO23" s="66"/>
+      <c r="BP23" s="66"/>
+    </row>
+    <row r="24" spans="1:76" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B24" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="47">
+      <c r="C24" s="29">
         <v>1</v>
       </c>
-      <c r="D11" s="47" t="s">
+      <c r="D24" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="48">
+      <c r="E24" s="44"/>
+      <c r="BD24" s="30">
+        <v>1</v>
+      </c>
+      <c r="BF24" s="66"/>
+      <c r="BG24" s="66"/>
+      <c r="BH24" s="66"/>
+      <c r="BI24" s="66"/>
+      <c r="BJ24" s="66"/>
+      <c r="BK24" s="66"/>
+      <c r="BL24" s="66"/>
+      <c r="BM24" s="66"/>
+      <c r="BN24" s="66"/>
+      <c r="BO24" s="66"/>
+      <c r="BP24" s="66"/>
+    </row>
+    <row r="25" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A25" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="45">
         <v>0</v>
       </c>
-      <c r="BD11" s="49">
+      <c r="K25" s="1">
         <v>0</v>
       </c>
-      <c r="BF11" s="62"/>
-      <c r="BG11" s="62"/>
-      <c r="BH11" s="62"/>
-      <c r="BI11" s="62"/>
-      <c r="BJ11" s="62"/>
-      <c r="BK11" s="62"/>
-      <c r="BL11" s="62"/>
-      <c r="BM11" s="62"/>
-      <c r="BN11" s="62"/>
-      <c r="BO11" s="62"/>
-      <c r="BP11" s="62"/>
-    </row>
-    <row r="12" spans="1:69" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="10">
-        <v>1</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="41"/>
-      <c r="F12" s="11">
-        <v>70</v>
-      </c>
-      <c r="J12" s="11">
-        <v>80</v>
-      </c>
-      <c r="AD12" s="11">
-        <v>82</v>
-      </c>
-      <c r="AQ12" s="11">
-        <v>84</v>
-      </c>
-      <c r="BC12" s="11">
-        <v>85</v>
-      </c>
-      <c r="BF12" s="63"/>
-      <c r="BG12" s="63"/>
-      <c r="BH12" s="63"/>
-      <c r="BI12" s="63"/>
-      <c r="BJ12" s="63"/>
-      <c r="BK12" s="63"/>
-      <c r="BL12" s="63"/>
-      <c r="BM12" s="63"/>
-      <c r="BN12" s="63"/>
-      <c r="BO12" s="63"/>
-      <c r="BP12" s="63"/>
-    </row>
-    <row r="13" spans="1:69" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="12">
-        <v>1</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="42"/>
-      <c r="H13" s="13">
-        <v>30</v>
-      </c>
-      <c r="K13" s="13">
-        <v>40</v>
-      </c>
-      <c r="AF13" s="13">
-        <v>40</v>
-      </c>
-      <c r="BF13" s="64"/>
-      <c r="BG13" s="64"/>
-      <c r="BH13" s="64"/>
-      <c r="BI13" s="64"/>
-      <c r="BJ13" s="64"/>
-      <c r="BK13" s="64"/>
-      <c r="BL13" s="64"/>
-      <c r="BM13" s="64"/>
-      <c r="BN13" s="64"/>
-      <c r="BO13" s="64"/>
-      <c r="BP13" s="64"/>
-    </row>
-    <row r="14" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="14">
-        <v>1</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="43"/>
-      <c r="V14" s="15">
-        <v>30</v>
-      </c>
-      <c r="AF14" s="15">
-        <v>40</v>
-      </c>
-      <c r="AP14" s="15">
-        <v>50</v>
-      </c>
-      <c r="BF14" s="65"/>
-      <c r="BG14" s="65"/>
-      <c r="BH14" s="65"/>
-      <c r="BI14" s="65"/>
-      <c r="BJ14" s="65"/>
-      <c r="BK14" s="65"/>
-      <c r="BL14" s="65"/>
-      <c r="BM14" s="65"/>
-      <c r="BN14" s="65"/>
-      <c r="BO14" s="65"/>
-      <c r="BP14" s="65"/>
-    </row>
-    <row r="15" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="14">
-        <v>1</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="43"/>
-      <c r="I15" s="15">
-        <v>7</v>
-      </c>
-      <c r="AK15" s="15">
-        <v>50</v>
-      </c>
-      <c r="AP15" s="15">
-        <v>70</v>
-      </c>
-      <c r="BF15" s="65"/>
-      <c r="BG15" s="65"/>
-      <c r="BH15" s="65"/>
-      <c r="BI15" s="65"/>
-      <c r="BJ15" s="65"/>
-      <c r="BK15" s="65"/>
-      <c r="BL15" s="65"/>
-      <c r="BM15" s="65"/>
-      <c r="BN15" s="65"/>
-      <c r="BO15" s="65"/>
-      <c r="BP15" s="65"/>
-    </row>
-    <row r="16" spans="1:69" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="12">
-        <v>1</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="42"/>
-      <c r="I16" s="13">
+      <c r="T25" s="1">
         <v>0</v>
       </c>
-      <c r="V16" s="13">
-        <v>40</v>
-      </c>
-      <c r="AB16" s="13">
-        <v>65</v>
-      </c>
-      <c r="AK16" s="24"/>
-      <c r="AL16" s="24"/>
-      <c r="AM16" s="24"/>
-      <c r="AN16" s="24"/>
-      <c r="AO16" s="24"/>
-      <c r="AP16" s="24"/>
-      <c r="AQ16" s="24"/>
-      <c r="AR16" s="24"/>
-      <c r="AS16" s="24"/>
-      <c r="AT16" s="24"/>
-      <c r="AU16" s="24"/>
-      <c r="AV16" s="24"/>
-      <c r="AW16" s="24"/>
-      <c r="AX16" s="24"/>
-      <c r="AY16" s="24"/>
-      <c r="AZ16" s="24"/>
-      <c r="BA16" s="24"/>
-      <c r="BB16" s="24">
-        <v>93</v>
-      </c>
-      <c r="BC16" s="24">
-        <v>85</v>
-      </c>
-      <c r="BF16" s="64"/>
-      <c r="BG16" s="64">
-        <v>96</v>
-      </c>
-      <c r="BH16" s="64"/>
-      <c r="BI16" s="64"/>
-      <c r="BJ16" s="64"/>
-      <c r="BK16" s="64"/>
-      <c r="BL16" s="64"/>
-      <c r="BM16" s="64"/>
-      <c r="BN16" s="64"/>
-      <c r="BO16" s="64"/>
-      <c r="BP16" s="64"/>
-    </row>
-    <row r="17" spans="1:76" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="12">
-        <v>3</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="42"/>
-      <c r="I17" s="13">
-        <v>0</v>
-      </c>
-      <c r="V17" s="13">
-        <v>10</v>
-      </c>
-      <c r="AB17" s="13">
-        <v>8</v>
-      </c>
-      <c r="AK17" s="24"/>
-      <c r="AL17" s="24"/>
-      <c r="AM17" s="24"/>
-      <c r="AN17" s="24"/>
-      <c r="AO17" s="24"/>
-      <c r="AP17" s="24"/>
-      <c r="AQ17" s="24"/>
-      <c r="AR17" s="24"/>
-      <c r="AS17" s="24"/>
-      <c r="AT17" s="24"/>
-      <c r="AU17" s="24"/>
-      <c r="AV17" s="24"/>
-      <c r="AW17" s="24"/>
-      <c r="AX17" s="24"/>
-      <c r="AY17" s="24"/>
-      <c r="AZ17" s="24"/>
-      <c r="BA17" s="24"/>
-      <c r="BB17" s="24"/>
-      <c r="BC17" s="24"/>
-      <c r="BD17" s="13">
-        <v>5</v>
-      </c>
-      <c r="BF17" s="64"/>
-      <c r="BG17" s="64">
-        <v>1.3</v>
-      </c>
-      <c r="BH17" s="64"/>
-      <c r="BI17" s="64"/>
-      <c r="BJ17" s="64"/>
-      <c r="BK17" s="64"/>
-      <c r="BL17" s="64"/>
-      <c r="BM17" s="64"/>
-      <c r="BN17" s="64"/>
-      <c r="BO17" s="64"/>
-      <c r="BP17" s="64"/>
-    </row>
-    <row r="18" spans="1:76" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="29">
-        <v>1</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="44"/>
-      <c r="AK18" s="31"/>
-      <c r="AL18" s="31"/>
-      <c r="AM18" s="31"/>
-      <c r="AN18" s="31"/>
-      <c r="AO18" s="31"/>
-      <c r="AP18" s="31"/>
-      <c r="AQ18" s="31"/>
-      <c r="AR18" s="31"/>
-      <c r="AS18" s="31"/>
-      <c r="AT18" s="31"/>
-      <c r="AU18" s="31"/>
-      <c r="AV18" s="31"/>
-      <c r="AW18" s="31"/>
-      <c r="AX18" s="31"/>
-      <c r="AY18" s="31"/>
-      <c r="AZ18" s="31"/>
-      <c r="BA18" s="31"/>
-      <c r="BB18" s="31"/>
-      <c r="BC18" s="31"/>
-      <c r="BD18" s="30">
-        <v>0</v>
-      </c>
-      <c r="BF18" s="66"/>
-      <c r="BG18" s="66"/>
-      <c r="BH18" s="66"/>
-      <c r="BI18" s="66"/>
-      <c r="BJ18" s="66">
-        <v>100</v>
-      </c>
-      <c r="BK18" s="66"/>
-      <c r="BL18" s="66"/>
-      <c r="BM18" s="66">
-        <v>100</v>
-      </c>
-      <c r="BN18" s="66"/>
-      <c r="BO18" s="66"/>
-      <c r="BP18" s="66">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="14">
-        <v>1</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="43"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="38"/>
-      <c r="O19" s="38"/>
-      <c r="P19" s="38"/>
-      <c r="Q19" s="38"/>
-      <c r="R19" s="38"/>
-      <c r="S19" s="38"/>
-      <c r="T19" s="38"/>
-      <c r="U19" s="38"/>
-      <c r="V19" s="38"/>
-      <c r="W19" s="38"/>
-      <c r="X19" s="38"/>
-      <c r="Y19" s="38"/>
-      <c r="Z19" s="38"/>
-      <c r="AA19" s="38"/>
-      <c r="AB19" s="38"/>
-      <c r="AC19" s="38"/>
-      <c r="AD19" s="38"/>
-      <c r="AE19" s="38"/>
-      <c r="AF19" s="38"/>
-      <c r="AG19" s="38"/>
-      <c r="AH19" s="38"/>
-      <c r="AI19" s="38"/>
-      <c r="AJ19" s="38"/>
-      <c r="AK19" s="38"/>
-      <c r="AL19" s="38"/>
-      <c r="AM19" s="38"/>
-      <c r="AN19" s="38"/>
-      <c r="AO19" s="38"/>
-      <c r="AP19" s="38"/>
-      <c r="AQ19" s="38"/>
-      <c r="AR19" s="38"/>
-      <c r="AS19" s="38"/>
-      <c r="AT19" s="38"/>
-      <c r="AU19" s="38"/>
-      <c r="AV19" s="38"/>
-      <c r="AW19" s="38"/>
-      <c r="AX19" s="38"/>
-      <c r="AY19" s="38"/>
-      <c r="AZ19" s="38"/>
-      <c r="BA19" s="38"/>
-      <c r="BB19" s="38"/>
-      <c r="BC19" s="38"/>
-      <c r="BD19" s="38">
-        <v>0</v>
-      </c>
-      <c r="BE19" s="38"/>
-      <c r="BF19" s="67">
-        <v>100</v>
-      </c>
-      <c r="BG19" s="67"/>
-      <c r="BH19" s="67"/>
-      <c r="BI19" s="67"/>
-      <c r="BJ19" s="67"/>
-      <c r="BK19" s="67"/>
-      <c r="BL19" s="67"/>
-      <c r="BM19" s="67">
-        <v>100</v>
-      </c>
-      <c r="BN19" s="67"/>
-      <c r="BO19" s="67"/>
-      <c r="BP19" s="67">
-        <v>100</v>
-      </c>
-      <c r="BQ19" s="38"/>
-      <c r="BR19" s="38"/>
-      <c r="BS19" s="38"/>
-      <c r="BT19" s="38"/>
-      <c r="BU19" s="38"/>
-      <c r="BV19" s="38"/>
-      <c r="BW19" s="38"/>
-      <c r="BX19" s="38"/>
-    </row>
-    <row r="20" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="14">
-        <v>1</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="43">
-        <v>0</v>
-      </c>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38"/>
-      <c r="P20" s="38"/>
-      <c r="Q20" s="38"/>
-      <c r="R20" s="38"/>
-      <c r="S20" s="38"/>
-      <c r="T20" s="38"/>
-      <c r="U20" s="38"/>
-      <c r="V20" s="38"/>
-      <c r="W20" s="38"/>
-      <c r="X20" s="38"/>
-      <c r="Y20" s="38"/>
-      <c r="Z20" s="38"/>
-      <c r="AA20" s="38"/>
-      <c r="AB20" s="38"/>
-      <c r="AC20" s="38"/>
-      <c r="AD20" s="38"/>
-      <c r="AE20" s="38"/>
-      <c r="AF20" s="38"/>
-      <c r="AG20" s="38"/>
-      <c r="AH20" s="38"/>
-      <c r="AI20" s="38"/>
-      <c r="AJ20" s="38"/>
-      <c r="AK20" s="38"/>
-      <c r="AL20" s="38"/>
-      <c r="AM20" s="38"/>
-      <c r="AN20" s="38"/>
-      <c r="AO20" s="38"/>
-      <c r="AP20" s="38"/>
-      <c r="AQ20" s="38"/>
-      <c r="AR20" s="38"/>
-      <c r="AS20" s="38"/>
-      <c r="AT20" s="38"/>
-      <c r="AU20" s="38"/>
-      <c r="AV20" s="38"/>
-      <c r="AW20" s="38"/>
-      <c r="AX20" s="38"/>
-      <c r="AY20" s="38"/>
-      <c r="AZ20" s="38"/>
-      <c r="BA20" s="38"/>
-      <c r="BB20" s="38"/>
-      <c r="BC20" s="38"/>
-      <c r="BD20" s="38">
-        <v>0</v>
-      </c>
-      <c r="BE20" s="38"/>
-      <c r="BF20" s="67"/>
-      <c r="BG20" s="67"/>
-      <c r="BH20" s="67">
-        <v>17</v>
-      </c>
-      <c r="BI20" s="67">
-        <v>70</v>
-      </c>
-      <c r="BJ20" s="67"/>
-      <c r="BK20" s="67"/>
-      <c r="BL20" s="67"/>
-      <c r="BM20" s="67">
-        <v>70</v>
-      </c>
-      <c r="BN20" s="67"/>
-      <c r="BO20" s="67"/>
-      <c r="BP20" s="67">
-        <v>70</v>
-      </c>
-      <c r="BQ20" s="38"/>
-      <c r="BR20" s="38"/>
-      <c r="BS20" s="38"/>
-      <c r="BT20" s="38"/>
-      <c r="BU20" s="38"/>
-      <c r="BV20" s="38"/>
-      <c r="BW20" s="38"/>
-      <c r="BX20" s="38"/>
-    </row>
-    <row r="21" spans="1:76" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="47">
-        <v>1</v>
-      </c>
-      <c r="D21" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="48"/>
-      <c r="BD21" s="49">
-        <v>0</v>
-      </c>
-      <c r="BF21" s="62"/>
-      <c r="BG21" s="62"/>
-      <c r="BH21" s="62"/>
-      <c r="BI21" s="62"/>
-      <c r="BJ21" s="62"/>
-      <c r="BK21" s="62"/>
-      <c r="BL21" s="62"/>
-      <c r="BM21" s="62"/>
-      <c r="BN21" s="62"/>
-      <c r="BO21" s="62"/>
-      <c r="BP21" s="62"/>
-    </row>
-    <row r="22" spans="1:76" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="47">
-        <v>1</v>
-      </c>
-      <c r="D22" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="48"/>
-      <c r="BD22" s="49">
-        <v>0</v>
-      </c>
-      <c r="BF22" s="62"/>
-      <c r="BG22" s="62"/>
-      <c r="BH22" s="62"/>
-      <c r="BI22" s="62"/>
-      <c r="BJ22" s="62"/>
-      <c r="BK22" s="62">
-        <v>50</v>
-      </c>
-      <c r="BL22" s="62"/>
-      <c r="BM22" s="62">
-        <v>50</v>
-      </c>
-      <c r="BN22" s="62"/>
-      <c r="BO22" s="62"/>
-      <c r="BP22" s="62">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:76" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="51" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="51">
-        <v>1</v>
-      </c>
-      <c r="D23" s="51" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="52">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="F23" s="53">
-        <v>4.84</v>
-      </c>
-      <c r="G23" s="53">
-        <v>5.44</v>
-      </c>
-      <c r="H23" s="53">
-        <v>6.11</v>
-      </c>
-      <c r="I23" s="53">
-        <v>6.86</v>
-      </c>
-      <c r="J23" s="53">
+      <c r="V25" s="1">
         <v>7.7</v>
       </c>
-      <c r="K23" s="53">
-        <v>8.68</v>
-      </c>
-      <c r="L23" s="53">
-        <v>9.0399999999999991</v>
-      </c>
-      <c r="M23" s="53">
-        <v>9.41</v>
-      </c>
-      <c r="N23" s="53">
-        <v>11.48</v>
-      </c>
-      <c r="O23" s="53">
-        <v>12.75</v>
-      </c>
-      <c r="P23" s="53">
-        <v>14.6</v>
-      </c>
-      <c r="Q23" s="53">
+      <c r="AI25" s="1">
+        <v>11.1</v>
+      </c>
+      <c r="AR25" s="1">
         <v>16.5</v>
       </c>
-      <c r="R23" s="53">
-        <v>18.38</v>
-      </c>
-      <c r="S23" s="53">
-        <v>19.670000000000002</v>
-      </c>
-      <c r="T23" s="53">
-        <v>20.87</v>
-      </c>
-      <c r="U23" s="53">
-        <v>22.5</v>
-      </c>
-      <c r="V23" s="53">
-        <v>25.9</v>
-      </c>
-      <c r="W23" s="53">
-        <v>28.8</v>
-      </c>
-      <c r="X23" s="53">
-        <v>30.8</v>
-      </c>
-      <c r="Y23" s="53">
-        <v>32.9</v>
-      </c>
-      <c r="Z23" s="53">
-        <v>34.6</v>
-      </c>
-      <c r="AA23" s="53">
-        <v>36.1</v>
-      </c>
-      <c r="AB23" s="53">
-        <v>36.799999999999997</v>
-      </c>
-      <c r="AC23" s="53">
-        <v>38.9</v>
-      </c>
-      <c r="AD23" s="53">
-        <v>43.4</v>
-      </c>
-      <c r="AE23" s="53">
-        <v>46.1</v>
-      </c>
-      <c r="AF23" s="53">
-        <v>49.9</v>
-      </c>
-      <c r="AG23" s="53">
-        <v>53.1</v>
-      </c>
-      <c r="AH23" s="53">
-        <v>55.7</v>
-      </c>
-      <c r="AI23" s="53">
-        <v>58.6</v>
-      </c>
-      <c r="AJ23" s="53">
-        <v>59.1</v>
-      </c>
-      <c r="AK23" s="53">
-        <v>60.4</v>
-      </c>
-      <c r="AL23" s="53">
-        <v>62.2</v>
-      </c>
-      <c r="AM23" s="53">
-        <v>64.3</v>
-      </c>
-      <c r="AN23" s="53">
-        <v>68</v>
-      </c>
-      <c r="AO23" s="53">
-        <v>69.3</v>
-      </c>
-      <c r="AP23" s="53">
-        <v>70.099999999999994</v>
-      </c>
-      <c r="AQ23" s="53">
-        <v>73.099999999999994</v>
-      </c>
-      <c r="AR23" s="53">
-        <v>73.599999999999994</v>
-      </c>
-      <c r="AS23" s="53">
-        <v>76.7</v>
-      </c>
-      <c r="AT23" s="53">
-        <v>78.900000000000006</v>
-      </c>
-      <c r="AU23" s="53">
-        <v>80.8</v>
-      </c>
-      <c r="AV23" s="53">
-        <v>82.8</v>
-      </c>
-      <c r="AW23" s="53">
-        <v>86.7</v>
-      </c>
-      <c r="AX23" s="53">
-        <v>93.4</v>
-      </c>
-      <c r="AY23" s="53">
-        <v>96.5</v>
-      </c>
-      <c r="AZ23" s="53">
-        <v>100</v>
-      </c>
-      <c r="BA23" s="53">
-        <v>107.3</v>
-      </c>
-      <c r="BB23" s="53">
-        <v>110.9</v>
-      </c>
-      <c r="BC23" s="53">
-        <v>114.2</v>
-      </c>
-      <c r="BD23" s="53">
-        <v>114.8</v>
-      </c>
-      <c r="BE23" s="53">
-        <v>116.4</v>
-      </c>
-      <c r="BF23" s="68"/>
-      <c r="BG23" s="68"/>
-      <c r="BH23" s="68"/>
-      <c r="BI23" s="68"/>
-      <c r="BJ23" s="68"/>
-      <c r="BK23" s="68"/>
-      <c r="BL23" s="68"/>
-      <c r="BM23" s="68"/>
-      <c r="BN23" s="68"/>
-      <c r="BO23" s="68"/>
-      <c r="BP23" s="68"/>
-    </row>
-    <row r="24" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="14">
-        <v>1</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="43">
-        <v>1</v>
-      </c>
-      <c r="F24" s="15">
-        <v>1</v>
-      </c>
-      <c r="G24" s="15">
-        <v>1</v>
-      </c>
-      <c r="H24" s="15">
-        <v>1</v>
-      </c>
-      <c r="I24" s="15">
-        <v>1</v>
-      </c>
-      <c r="J24" s="15">
-        <v>1</v>
-      </c>
-      <c r="K24" s="15">
-        <v>1</v>
-      </c>
-      <c r="L24" s="15">
-        <v>1</v>
-      </c>
-      <c r="M24" s="15">
-        <v>1</v>
-      </c>
-      <c r="N24" s="15">
-        <v>1</v>
-      </c>
-      <c r="O24" s="15">
-        <v>1</v>
-      </c>
-      <c r="P24" s="15">
-        <v>1</v>
-      </c>
-      <c r="Q24" s="15">
-        <v>1</v>
-      </c>
-      <c r="R24" s="15">
-        <v>1</v>
-      </c>
-      <c r="S24" s="15">
-        <v>1</v>
-      </c>
-      <c r="T24" s="15">
-        <v>1</v>
-      </c>
-      <c r="U24" s="15">
-        <v>1</v>
-      </c>
-      <c r="V24" s="15">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="BA24" s="15">
-        <v>3.11</v>
-      </c>
-      <c r="BF24" s="65"/>
-      <c r="BG24" s="65"/>
-      <c r="BH24" s="65"/>
-      <c r="BI24" s="65"/>
-      <c r="BJ24" s="65"/>
-      <c r="BK24" s="65"/>
-      <c r="BL24" s="65"/>
-      <c r="BM24" s="65"/>
-      <c r="BN24" s="65"/>
-      <c r="BO24" s="65"/>
-      <c r="BP24" s="65"/>
-    </row>
-    <row r="25" spans="1:76" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="58"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="44"/>
-      <c r="BF25" s="66"/>
-      <c r="BG25" s="66"/>
-      <c r="BH25" s="66"/>
-      <c r="BI25" s="66"/>
-      <c r="BJ25" s="66"/>
-      <c r="BK25" s="66"/>
-      <c r="BL25" s="66"/>
-      <c r="BM25" s="66"/>
-      <c r="BN25" s="66"/>
-      <c r="BO25" s="66"/>
-      <c r="BP25" s="66"/>
-    </row>
-    <row r="26" spans="1:76" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="58" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="29">
-        <v>1</v>
-      </c>
-      <c r="D26" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" s="44">
-        <v>1</v>
-      </c>
-      <c r="BD26" s="30">
-        <v>1</v>
-      </c>
-      <c r="BF26" s="66"/>
-      <c r="BG26" s="66"/>
-      <c r="BH26" s="66"/>
-      <c r="BI26" s="66"/>
-      <c r="BJ26" s="66"/>
-      <c r="BK26" s="66"/>
-      <c r="BL26" s="66"/>
-      <c r="BM26" s="66"/>
-      <c r="BN26" s="66"/>
-      <c r="BO26" s="66"/>
-      <c r="BP26" s="66"/>
-    </row>
-    <row r="27" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="2">
-        <v>1</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" s="45">
-        <v>0</v>
-      </c>
-      <c r="K27" s="1">
-        <v>0</v>
-      </c>
-      <c r="T27" s="1">
-        <v>0</v>
-      </c>
-      <c r="V27" s="1">
-        <v>7.7</v>
-      </c>
-      <c r="AI27" s="1">
-        <v>11.1</v>
-      </c>
-      <c r="AR27" s="1">
-        <v>16.5</v>
-      </c>
-      <c r="AT27" s="1">
+      <c r="AT25" s="1">
         <v>14.5</v>
       </c>
-      <c r="AY27" s="1">
+      <c r="AY25" s="1">
         <v>16.100000000000001</v>
       </c>
-      <c r="BA27" s="1">
+      <c r="BA25" s="1">
         <v>15.6</v>
       </c>
-      <c r="BC27" s="1">
+      <c r="BC25" s="1">
         <v>15.6</v>
       </c>
-      <c r="BE27" s="1">
+      <c r="BE25" s="1">
         <v>15.6</v>
       </c>
-      <c r="BF27" s="69"/>
-      <c r="BG27" s="69"/>
-      <c r="BH27" s="69"/>
-      <c r="BI27" s="69"/>
-      <c r="BJ27" s="69"/>
-      <c r="BK27" s="69"/>
-      <c r="BL27" s="69"/>
-      <c r="BM27" s="69"/>
-      <c r="BN27" s="69"/>
-      <c r="BO27" s="69"/>
-      <c r="BP27" s="69"/>
+      <c r="BF25" s="69"/>
+      <c r="BG25" s="69"/>
+      <c r="BH25" s="69"/>
+      <c r="BI25" s="69"/>
+      <c r="BJ25" s="69"/>
+      <c r="BK25" s="69"/>
+      <c r="BL25" s="69"/>
+      <c r="BM25" s="69"/>
+      <c r="BN25" s="69"/>
+      <c r="BO25" s="69"/>
+      <c r="BP25" s="69"/>
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="5">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF18:BG18 F5:BG8">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF16:BG16 F5:BG8">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:D1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F12:BG17 F18:BE18 F2:BG4">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10:BG15 F16:BE16 F2:BG4">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C27:C1048576 C2:C24">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C25:C1048576 C2:C22">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Leave blank" sqref="B25:D26"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Leave blank" sqref="B23:D24"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4068,13 +3956,13 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B8 B12:B18</xm:sqref>
+          <xm:sqref>B2:B8 B10:B16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time-variant?" prompt="If no, the most recent value will be selected.">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D27:D1048576 D2:D24</xm:sqref>
+          <xm:sqref>D25:D1048576 D2:D22</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Remove unnecessary vaccination row for Fiji
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
   <si>
     <t>parameter</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>with_diabetes</t>
-  </si>
-  <si>
-    <t>program_perc_vaccination</t>
   </si>
   <si>
     <t>program_perc_detect</t>
@@ -296,7 +293,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,12 +314,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1156,7 +1147,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1165,69 +1156,71 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1236,16 +1229,13 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2229,43 +2219,43 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.5703125" style="26" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="33" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="25"/>
-    <col min="6" max="6" width="13.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="25"/>
+    <col min="1" max="1" width="51.5703125" style="25" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="32" customWidth="1"/>
+    <col min="3" max="5" width="9.140625" style="24"/>
+    <col min="6" max="6" width="13.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="26" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="54">
+      <c r="B2" s="53">
         <v>7.55</v>
       </c>
-      <c r="F2" s="54">
+      <c r="F2" s="53">
         <v>7.55</v>
       </c>
-      <c r="G2" s="54">
+      <c r="G2" s="53">
         <v>7.85</v>
       </c>
       <c r="H2">
@@ -2273,16 +2263,16 @@
       </c>
     </row>
     <row r="3" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="55">
+      <c r="B3" s="54">
         <v>0.22</v>
       </c>
-      <c r="F3" s="55">
+      <c r="F3" s="54">
         <v>0.22</v>
       </c>
-      <c r="G3" s="55">
+      <c r="G3" s="54">
         <v>0.22</v>
       </c>
       <c r="H3">
@@ -2290,16 +2280,16 @@
       </c>
     </row>
     <row r="4" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="56">
+      <c r="B4" s="55">
         <v>1865</v>
       </c>
-      <c r="F4" s="56">
+      <c r="F4" s="55">
         <v>1865</v>
       </c>
-      <c r="G4" s="56">
+      <c r="G4" s="55">
         <v>1865</v>
       </c>
       <c r="H4">
@@ -2307,16 +2297,16 @@
       </c>
     </row>
     <row r="5" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="57">
+      <c r="B5" s="56">
         <v>190000</v>
       </c>
-      <c r="F5" s="57">
+      <c r="F5" s="56">
         <v>190000</v>
       </c>
-      <c r="G5" s="57">
+      <c r="G5" s="56">
         <v>190000</v>
       </c>
       <c r="H5">
@@ -2324,16 +2314,16 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="33">
+      <c r="A6" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="32">
         <v>5</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="24">
         <v>15</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="24">
         <v>25</v>
       </c>
     </row>
@@ -2367,7 +2357,7 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BX25"/>
+  <dimension ref="A1:BX24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -2381,7 +2371,7 @@
     <col min="1" max="1" width="56" style="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11" style="45" customWidth="1"/>
+    <col min="5" max="5" width="11" style="44" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.42578125" style="1" customWidth="1"/>
     <col min="8" max="9" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -2405,7 +2395,7 @@
     <col min="69" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:76" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -2611,15 +2601,15 @@
         <v>27</v>
       </c>
       <c r="BQ1" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:69" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:76" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="6">
         <v>1</v>
@@ -2627,115 +2617,149 @@
       <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="39"/>
-      <c r="H2" s="7">
+      <c r="E2" s="38"/>
+      <c r="V2" s="58"/>
+      <c r="W2" s="58"/>
+      <c r="X2" s="58"/>
+      <c r="Y2" s="58"/>
+      <c r="Z2" s="58"/>
+      <c r="AA2" s="58"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="58"/>
+      <c r="AD2" s="58"/>
+      <c r="AE2" s="58"/>
+      <c r="AF2" s="58"/>
+      <c r="AG2" s="58"/>
+      <c r="AH2" s="58"/>
+      <c r="AI2" s="58"/>
+      <c r="AJ2" s="58"/>
+      <c r="AK2" s="58"/>
+      <c r="AL2" s="58"/>
+      <c r="AM2" s="58"/>
+      <c r="AN2" s="58"/>
+      <c r="AO2" s="58"/>
+      <c r="AP2" s="58"/>
+      <c r="AQ2" s="58"/>
+      <c r="AR2" s="58"/>
+      <c r="AS2" s="58"/>
+      <c r="AT2" s="58"/>
+      <c r="AU2" s="58"/>
+      <c r="AV2" s="58"/>
+      <c r="AW2" s="58"/>
+      <c r="AX2" s="58"/>
+      <c r="AY2" s="58"/>
+      <c r="AZ2" s="58"/>
+      <c r="BA2" s="58"/>
+      <c r="BB2" s="58"/>
+      <c r="BC2" s="58"/>
+      <c r="BD2" s="58">
         <v>0</v>
       </c>
-      <c r="J2" s="7">
-        <v>25</v>
-      </c>
-      <c r="V2" s="22"/>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="22"/>
-      <c r="AB2" s="22"/>
-      <c r="AC2" s="22"/>
-      <c r="AD2" s="22"/>
-      <c r="AE2" s="22"/>
-      <c r="AF2" s="22"/>
-      <c r="AG2" s="22"/>
-      <c r="AH2" s="22"/>
-      <c r="AI2" s="22"/>
-      <c r="AJ2" s="22"/>
-      <c r="AK2" s="22"/>
-      <c r="AL2" s="22"/>
-      <c r="AM2" s="22"/>
-      <c r="AN2" s="22"/>
-      <c r="AO2" s="22"/>
-      <c r="AP2" s="22"/>
-      <c r="AQ2" s="22"/>
-      <c r="AR2" s="22"/>
-      <c r="AS2" s="22"/>
-      <c r="AT2" s="22"/>
-      <c r="AU2" s="22"/>
-      <c r="AV2" s="22"/>
-      <c r="AW2" s="22"/>
-      <c r="AX2" s="22"/>
-      <c r="AY2" s="22"/>
-      <c r="AZ2" s="22"/>
-      <c r="BA2" s="22"/>
-      <c r="BB2" s="22"/>
-      <c r="BC2" s="22"/>
-      <c r="BD2" s="22"/>
-      <c r="BE2" s="22"/>
-      <c r="BF2" s="60"/>
-      <c r="BG2" s="60"/>
-      <c r="BH2" s="60"/>
-      <c r="BI2" s="60"/>
-      <c r="BJ2" s="60"/>
-      <c r="BK2" s="60"/>
-      <c r="BL2" s="60"/>
-      <c r="BM2" s="60"/>
-      <c r="BN2" s="60"/>
-      <c r="BO2" s="60"/>
-      <c r="BP2" s="60"/>
+      <c r="BE2" s="58"/>
+      <c r="BF2" s="59"/>
+      <c r="BG2" s="59"/>
+      <c r="BH2" s="59"/>
+      <c r="BI2" s="59"/>
+      <c r="BJ2" s="59"/>
+      <c r="BK2" s="59"/>
+      <c r="BL2" s="59"/>
+      <c r="BM2" s="59"/>
+      <c r="BN2" s="59"/>
+      <c r="BO2" s="59">
+        <v>90</v>
+      </c>
+      <c r="BP2" s="59"/>
     </row>
-    <row r="3" spans="1:69" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="6">
-        <v>1</v>
-      </c>
-      <c r="D3" s="6" t="s">
+    <row r="3" spans="1:76" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="39">
+      <c r="C3" s="8">
+        <v>5</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="39"/>
+      <c r="F3" s="9">
         <v>0</v>
       </c>
-      <c r="V3" s="59"/>
-      <c r="W3" s="59"/>
-      <c r="X3" s="59"/>
-      <c r="Y3" s="59"/>
-      <c r="Z3" s="59"/>
-      <c r="AA3" s="59"/>
-      <c r="AB3" s="59"/>
-      <c r="AC3" s="59"/>
-      <c r="AD3" s="59"/>
-      <c r="AE3" s="59"/>
-      <c r="AF3" s="59"/>
-      <c r="AG3" s="59"/>
-      <c r="AH3" s="59"/>
-      <c r="AI3" s="59"/>
-      <c r="AJ3" s="59"/>
-      <c r="AK3" s="59"/>
-      <c r="AL3" s="59"/>
-      <c r="AM3" s="59"/>
-      <c r="AN3" s="59"/>
-      <c r="AO3" s="59"/>
-      <c r="AP3" s="59"/>
-      <c r="AQ3" s="59"/>
-      <c r="AR3" s="59"/>
-      <c r="AS3" s="59"/>
-      <c r="AT3" s="59"/>
-      <c r="AU3" s="59"/>
-      <c r="AV3" s="59"/>
-      <c r="AW3" s="59"/>
-      <c r="AX3" s="59"/>
-      <c r="AY3" s="59"/>
-      <c r="AZ3" s="59"/>
-      <c r="BA3" s="59"/>
-      <c r="BB3" s="59"/>
-      <c r="BC3" s="59"/>
-      <c r="BD3" s="59">
-        <v>0</v>
-      </c>
-      <c r="BE3" s="59"/>
+      <c r="K3" s="9">
+        <v>10</v>
+      </c>
+      <c r="AF3" s="22">
+        <v>40</v>
+      </c>
+      <c r="AG3" s="22">
+        <v>40</v>
+      </c>
+      <c r="AH3" s="22">
+        <v>40</v>
+      </c>
+      <c r="AI3" s="22">
+        <v>40</v>
+      </c>
+      <c r="AJ3" s="22">
+        <v>40</v>
+      </c>
+      <c r="AK3" s="22">
+        <v>40</v>
+      </c>
+      <c r="AL3" s="22">
+        <v>40</v>
+      </c>
+      <c r="AM3" s="22">
+        <v>40</v>
+      </c>
+      <c r="AN3" s="22">
+        <v>40</v>
+      </c>
+      <c r="AO3" s="22">
+        <v>40</v>
+      </c>
+      <c r="AP3" s="22">
+        <v>40</v>
+      </c>
+      <c r="AQ3" s="22">
+        <v>40</v>
+      </c>
+      <c r="AR3" s="22">
+        <v>40</v>
+      </c>
+      <c r="AS3" s="22">
+        <v>40</v>
+      </c>
+      <c r="AT3" s="22">
+        <v>40</v>
+      </c>
+      <c r="AU3" s="22">
+        <v>40</v>
+      </c>
+      <c r="AV3" s="22">
+        <v>10</v>
+      </c>
+      <c r="AW3" s="22">
+        <v>10</v>
+      </c>
+      <c r="AX3" s="22">
+        <v>10</v>
+      </c>
+      <c r="AY3" s="22"/>
+      <c r="AZ3" s="22">
+        <v>30</v>
+      </c>
+      <c r="BA3" s="22">
+        <v>30</v>
+      </c>
+      <c r="BB3" s="22"/>
+      <c r="BC3" s="22"/>
+      <c r="BD3" s="22">
+        <v>55</v>
+      </c>
+      <c r="BE3" s="22"/>
       <c r="BF3" s="60"/>
       <c r="BG3" s="60"/>
       <c r="BH3" s="60"/>
@@ -2745,12 +2769,10 @@
       <c r="BL3" s="60"/>
       <c r="BM3" s="60"/>
       <c r="BN3" s="60"/>
-      <c r="BO3" s="60">
-        <v>90</v>
-      </c>
+      <c r="BO3" s="60"/>
       <c r="BP3" s="60"/>
     </row>
-    <row r="4" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:76" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>33</v>
       </c>
@@ -2758,101 +2780,28 @@
         <v>3</v>
       </c>
       <c r="C4" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="40"/>
-      <c r="F4" s="9">
+      <c r="E4" s="39"/>
+      <c r="BD4" s="9">
         <v>0</v>
       </c>
-      <c r="K4" s="9">
-        <v>10</v>
-      </c>
-      <c r="AF4" s="23">
-        <v>40</v>
-      </c>
-      <c r="AG4" s="23">
-        <v>40</v>
-      </c>
-      <c r="AH4" s="23">
-        <v>40</v>
-      </c>
-      <c r="AI4" s="23">
-        <v>40</v>
-      </c>
-      <c r="AJ4" s="23">
-        <v>40</v>
-      </c>
-      <c r="AK4" s="23">
-        <v>40</v>
-      </c>
-      <c r="AL4" s="23">
-        <v>40</v>
-      </c>
-      <c r="AM4" s="23">
-        <v>40</v>
-      </c>
-      <c r="AN4" s="23">
-        <v>40</v>
-      </c>
-      <c r="AO4" s="23">
-        <v>40</v>
-      </c>
-      <c r="AP4" s="23">
-        <v>40</v>
-      </c>
-      <c r="AQ4" s="23">
-        <v>40</v>
-      </c>
-      <c r="AR4" s="23">
-        <v>40</v>
-      </c>
-      <c r="AS4" s="23">
-        <v>40</v>
-      </c>
-      <c r="AT4" s="23">
-        <v>40</v>
-      </c>
-      <c r="AU4" s="23">
-        <v>40</v>
-      </c>
-      <c r="AV4" s="23">
-        <v>10</v>
-      </c>
-      <c r="AW4" s="23">
-        <v>10</v>
-      </c>
-      <c r="AX4" s="23">
-        <v>10</v>
-      </c>
-      <c r="AY4" s="23"/>
-      <c r="AZ4" s="23">
-        <v>30</v>
-      </c>
-      <c r="BA4" s="23">
-        <v>30</v>
-      </c>
-      <c r="BB4" s="23"/>
-      <c r="BC4" s="23"/>
-      <c r="BD4" s="23">
-        <v>55</v>
-      </c>
-      <c r="BE4" s="23"/>
-      <c r="BF4" s="61"/>
-      <c r="BG4" s="61"/>
-      <c r="BH4" s="61"/>
-      <c r="BI4" s="61"/>
-      <c r="BJ4" s="61"/>
-      <c r="BK4" s="61"/>
-      <c r="BL4" s="61"/>
-      <c r="BM4" s="61"/>
-      <c r="BN4" s="61"/>
-      <c r="BO4" s="61"/>
-      <c r="BP4" s="61"/>
+      <c r="BF4" s="60"/>
+      <c r="BG4" s="60"/>
+      <c r="BH4" s="60"/>
+      <c r="BI4" s="60"/>
+      <c r="BJ4" s="60"/>
+      <c r="BK4" s="60"/>
+      <c r="BL4" s="60"/>
+      <c r="BM4" s="60"/>
+      <c r="BN4" s="60"/>
+      <c r="BO4" s="60"/>
+      <c r="BP4" s="60"/>
     </row>
-    <row r="5" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:76" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>34</v>
       </c>
@@ -2865,23 +2814,35 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="40"/>
+      <c r="E5" s="39"/>
+      <c r="BA5" s="9">
+        <v>0</v>
+      </c>
+      <c r="BB5" s="9">
+        <v>7</v>
+      </c>
       <c r="BD5" s="9">
-        <v>0</v>
-      </c>
-      <c r="BF5" s="61"/>
-      <c r="BG5" s="61"/>
-      <c r="BH5" s="61"/>
-      <c r="BI5" s="61"/>
-      <c r="BJ5" s="61"/>
-      <c r="BK5" s="61"/>
-      <c r="BL5" s="61"/>
-      <c r="BM5" s="61"/>
-      <c r="BN5" s="61"/>
-      <c r="BO5" s="61"/>
-      <c r="BP5" s="61"/>
+        <v>23.6</v>
+      </c>
+      <c r="BF5" s="60"/>
+      <c r="BG5" s="60"/>
+      <c r="BH5" s="60"/>
+      <c r="BI5" s="60"/>
+      <c r="BJ5" s="60"/>
+      <c r="BK5" s="60"/>
+      <c r="BL5" s="60">
+        <v>80</v>
+      </c>
+      <c r="BM5" s="60">
+        <v>80</v>
+      </c>
+      <c r="BN5" s="60"/>
+      <c r="BO5" s="60"/>
+      <c r="BP5" s="60">
+        <v>80</v>
+      </c>
     </row>
-    <row r="6" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:76" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>35</v>
       </c>
@@ -2894,40 +2855,34 @@
       <c r="D6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="40"/>
-      <c r="BA6" s="9">
+      <c r="E6" s="39"/>
+      <c r="BD6" s="9">
         <v>0</v>
       </c>
-      <c r="BB6" s="9">
-        <v>7</v>
-      </c>
-      <c r="BD6" s="9">
-        <v>23.6</v>
-      </c>
-      <c r="BF6" s="61"/>
-      <c r="BG6" s="61"/>
-      <c r="BH6" s="61"/>
-      <c r="BI6" s="61"/>
-      <c r="BJ6" s="61"/>
-      <c r="BK6" s="61"/>
-      <c r="BL6" s="61">
+      <c r="BF6" s="60"/>
+      <c r="BG6" s="60"/>
+      <c r="BH6" s="60"/>
+      <c r="BI6" s="60"/>
+      <c r="BJ6" s="60"/>
+      <c r="BK6" s="60"/>
+      <c r="BL6" s="60">
         <v>80</v>
       </c>
-      <c r="BM6" s="61">
+      <c r="BM6" s="60">
         <v>80</v>
       </c>
-      <c r="BN6" s="61"/>
-      <c r="BO6" s="61"/>
-      <c r="BP6" s="61">
+      <c r="BN6" s="60"/>
+      <c r="BO6" s="60"/>
+      <c r="BP6" s="60">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:76" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="8">
         <v>1</v>
@@ -2935,43 +2890,42 @@
       <c r="D7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="40"/>
+      <c r="E7" s="39"/>
       <c r="BD7" s="9">
         <v>0</v>
       </c>
-      <c r="BF7" s="61"/>
-      <c r="BG7" s="61"/>
-      <c r="BH7" s="61"/>
-      <c r="BI7" s="61"/>
-      <c r="BJ7" s="61"/>
-      <c r="BK7" s="61"/>
-      <c r="BL7" s="61">
-        <v>80</v>
-      </c>
-      <c r="BM7" s="61">
-        <v>80</v>
-      </c>
-      <c r="BN7" s="61"/>
-      <c r="BO7" s="61"/>
-      <c r="BP7" s="61">
-        <v>80</v>
+      <c r="BF7" s="60"/>
+      <c r="BG7" s="60"/>
+      <c r="BH7" s="60"/>
+      <c r="BI7" s="60"/>
+      <c r="BJ7" s="60"/>
+      <c r="BK7" s="60"/>
+      <c r="BL7" s="60"/>
+      <c r="BM7" s="60"/>
+      <c r="BN7" s="60"/>
+      <c r="BO7" s="60"/>
+      <c r="BP7" s="9">
+        <v>10</v>
+      </c>
+      <c r="BQ7" s="9">
+        <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:69" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="8" t="s">
+    <row r="8" spans="1:76" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="46">
         <v>1</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="40"/>
-      <c r="BD8" s="9">
+      <c r="E8" s="47"/>
+      <c r="BD8" s="48">
         <v>0</v>
       </c>
       <c r="BF8" s="61"/>
@@ -2982,33 +2936,40 @@
       <c r="BK8" s="61"/>
       <c r="BL8" s="61"/>
       <c r="BM8" s="61"/>
-      <c r="BN8" s="61"/>
+      <c r="BN8" s="61">
+        <v>10</v>
+      </c>
       <c r="BO8" s="61"/>
-      <c r="BP8" s="9">
-        <v>10</v>
-      </c>
-      <c r="BQ8" s="9">
-        <v>50</v>
-      </c>
+      <c r="BP8" s="61"/>
     </row>
-    <row r="9" spans="1:69" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="47" t="s">
+    <row r="9" spans="1:76" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="47">
+      <c r="C9" s="10">
         <v>1</v>
       </c>
-      <c r="D9" s="47" t="s">
+      <c r="D9" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="48">
-        <v>0</v>
-      </c>
-      <c r="BD9" s="49">
-        <v>0</v>
+      <c r="E9" s="40"/>
+      <c r="F9" s="11">
+        <v>70</v>
+      </c>
+      <c r="J9" s="11">
+        <v>80</v>
+      </c>
+      <c r="AD9" s="11">
+        <v>82</v>
+      </c>
+      <c r="AQ9" s="11">
+        <v>84</v>
+      </c>
+      <c r="BC9" s="11">
+        <v>85</v>
       </c>
       <c r="BF9" s="62"/>
       <c r="BG9" s="62"/>
@@ -3018,40 +2979,32 @@
       <c r="BK9" s="62"/>
       <c r="BL9" s="62"/>
       <c r="BM9" s="62"/>
-      <c r="BN9" s="62">
-        <v>10</v>
-      </c>
+      <c r="BN9" s="62"/>
       <c r="BO9" s="62"/>
       <c r="BP9" s="62"/>
     </row>
-    <row r="10" spans="1:69" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+    <row r="10" spans="1:76" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="12">
         <v>1</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E10" s="41"/>
-      <c r="F10" s="11">
-        <v>70</v>
-      </c>
-      <c r="J10" s="11">
-        <v>80</v>
-      </c>
-      <c r="AD10" s="11">
-        <v>82</v>
-      </c>
-      <c r="AQ10" s="11">
-        <v>84</v>
-      </c>
-      <c r="BC10" s="11">
-        <v>85</v>
+      <c r="H10" s="13">
+        <v>30</v>
+      </c>
+      <c r="K10" s="13">
+        <v>40</v>
+      </c>
+      <c r="AF10" s="13">
+        <v>40</v>
       </c>
       <c r="BF10" s="63"/>
       <c r="BG10" s="63"/>
@@ -3065,28 +3018,28 @@
       <c r="BO10" s="63"/>
       <c r="BP10" s="63"/>
     </row>
-    <row r="11" spans="1:69" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+    <row r="11" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="14">
         <v>1</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="42"/>
-      <c r="H11" s="13">
+      <c r="V11" s="15">
         <v>30</v>
       </c>
-      <c r="K11" s="13">
+      <c r="AF11" s="15">
         <v>40</v>
       </c>
-      <c r="AF11" s="13">
-        <v>40</v>
+      <c r="AP11" s="15">
+        <v>50</v>
       </c>
       <c r="BF11" s="64"/>
       <c r="BG11" s="64"/>
@@ -3100,7 +3053,7 @@
       <c r="BO11" s="64"/>
       <c r="BP11" s="64"/>
     </row>
-    <row r="12" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>39</v>
       </c>
@@ -3113,64 +3066,89 @@
       <c r="D12" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="43"/>
-      <c r="V12" s="15">
-        <v>30</v>
-      </c>
-      <c r="AF12" s="15">
+      <c r="E12" s="42"/>
+      <c r="I12" s="15">
+        <v>7</v>
+      </c>
+      <c r="AK12" s="15">
+        <v>50</v>
+      </c>
+      <c r="AP12" s="15">
+        <v>70</v>
+      </c>
+      <c r="BF12" s="64"/>
+      <c r="BG12" s="64"/>
+      <c r="BH12" s="64"/>
+      <c r="BI12" s="64"/>
+      <c r="BJ12" s="64"/>
+      <c r="BK12" s="64"/>
+      <c r="BL12" s="64"/>
+      <c r="BM12" s="64"/>
+      <c r="BN12" s="64"/>
+      <c r="BO12" s="64"/>
+      <c r="BP12" s="64"/>
+    </row>
+    <row r="13" spans="1:76" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="12">
+        <v>1</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="41"/>
+      <c r="I13" s="13">
+        <v>0</v>
+      </c>
+      <c r="V13" s="13">
         <v>40</v>
       </c>
-      <c r="AP12" s="15">
-        <v>50</v>
-      </c>
-      <c r="BF12" s="65"/>
-      <c r="BG12" s="65"/>
-      <c r="BH12" s="65"/>
-      <c r="BI12" s="65"/>
-      <c r="BJ12" s="65"/>
-      <c r="BK12" s="65"/>
-      <c r="BL12" s="65"/>
-      <c r="BM12" s="65"/>
-      <c r="BN12" s="65"/>
-      <c r="BO12" s="65"/>
-      <c r="BP12" s="65"/>
+      <c r="AB13" s="13">
+        <v>65</v>
+      </c>
+      <c r="AK13" s="23"/>
+      <c r="AL13" s="23"/>
+      <c r="AM13" s="23"/>
+      <c r="AN13" s="23"/>
+      <c r="AO13" s="23"/>
+      <c r="AP13" s="23"/>
+      <c r="AQ13" s="23"/>
+      <c r="AR13" s="23"/>
+      <c r="AS13" s="23"/>
+      <c r="AT13" s="23"/>
+      <c r="AU13" s="23"/>
+      <c r="AV13" s="23"/>
+      <c r="AW13" s="23"/>
+      <c r="AX13" s="23"/>
+      <c r="AY13" s="23"/>
+      <c r="AZ13" s="23"/>
+      <c r="BA13" s="23"/>
+      <c r="BB13" s="23">
+        <v>93</v>
+      </c>
+      <c r="BC13" s="23">
+        <v>85</v>
+      </c>
+      <c r="BF13" s="63"/>
+      <c r="BG13" s="63">
+        <v>96</v>
+      </c>
+      <c r="BH13" s="63"/>
+      <c r="BI13" s="63"/>
+      <c r="BJ13" s="63"/>
+      <c r="BK13" s="63"/>
+      <c r="BL13" s="63"/>
+      <c r="BM13" s="63"/>
+      <c r="BN13" s="63"/>
+      <c r="BO13" s="63"/>
+      <c r="BP13" s="63"/>
     </row>
-    <row r="13" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="14">
-        <v>1</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="43"/>
-      <c r="I13" s="15">
-        <v>7</v>
-      </c>
-      <c r="AK13" s="15">
-        <v>50</v>
-      </c>
-      <c r="AP13" s="15">
-        <v>70</v>
-      </c>
-      <c r="BF13" s="65"/>
-      <c r="BG13" s="65"/>
-      <c r="BH13" s="65"/>
-      <c r="BI13" s="65"/>
-      <c r="BJ13" s="65"/>
-      <c r="BK13" s="65"/>
-      <c r="BL13" s="65"/>
-      <c r="BM13" s="65"/>
-      <c r="BN13" s="65"/>
-      <c r="BO13" s="65"/>
-      <c r="BP13" s="65"/>
-    </row>
-    <row r="14" spans="1:69" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:76" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>45</v>
       </c>
@@ -3178,160 +3156,186 @@
         <v>3</v>
       </c>
       <c r="C14" s="12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="42"/>
+      <c r="E14" s="41"/>
       <c r="I14" s="13">
         <v>0</v>
       </c>
       <c r="V14" s="13">
+        <v>10</v>
+      </c>
+      <c r="AB14" s="13">
+        <v>8</v>
+      </c>
+      <c r="AK14" s="23"/>
+      <c r="AL14" s="23"/>
+      <c r="AM14" s="23"/>
+      <c r="AN14" s="23"/>
+      <c r="AO14" s="23"/>
+      <c r="AP14" s="23"/>
+      <c r="AQ14" s="23"/>
+      <c r="AR14" s="23"/>
+      <c r="AS14" s="23"/>
+      <c r="AT14" s="23"/>
+      <c r="AU14" s="23"/>
+      <c r="AV14" s="23"/>
+      <c r="AW14" s="23"/>
+      <c r="AX14" s="23"/>
+      <c r="AY14" s="23"/>
+      <c r="AZ14" s="23"/>
+      <c r="BA14" s="23"/>
+      <c r="BB14" s="23"/>
+      <c r="BC14" s="23"/>
+      <c r="BD14" s="13">
+        <v>5</v>
+      </c>
+      <c r="BF14" s="63"/>
+      <c r="BG14" s="63">
+        <v>1.3</v>
+      </c>
+      <c r="BH14" s="63"/>
+      <c r="BI14" s="63"/>
+      <c r="BJ14" s="63"/>
+      <c r="BK14" s="63"/>
+      <c r="BL14" s="63"/>
+      <c r="BM14" s="63"/>
+      <c r="BN14" s="63"/>
+      <c r="BO14" s="63"/>
+      <c r="BP14" s="63"/>
+    </row>
+    <row r="15" spans="1:76" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="AB14" s="13">
-        <v>65</v>
-      </c>
-      <c r="AK14" s="24"/>
-      <c r="AL14" s="24"/>
-      <c r="AM14" s="24"/>
-      <c r="AN14" s="24"/>
-      <c r="AO14" s="24"/>
-      <c r="AP14" s="24"/>
-      <c r="AQ14" s="24"/>
-      <c r="AR14" s="24"/>
-      <c r="AS14" s="24"/>
-      <c r="AT14" s="24"/>
-      <c r="AU14" s="24"/>
-      <c r="AV14" s="24"/>
-      <c r="AW14" s="24"/>
-      <c r="AX14" s="24"/>
-      <c r="AY14" s="24"/>
-      <c r="AZ14" s="24"/>
-      <c r="BA14" s="24"/>
-      <c r="BB14" s="24">
-        <v>93</v>
-      </c>
-      <c r="BC14" s="24">
-        <v>85</v>
-      </c>
-      <c r="BF14" s="64"/>
-      <c r="BG14" s="64">
-        <v>96</v>
-      </c>
-      <c r="BH14" s="64"/>
-      <c r="BI14" s="64"/>
-      <c r="BJ14" s="64"/>
-      <c r="BK14" s="64"/>
-      <c r="BL14" s="64"/>
-      <c r="BM14" s="64"/>
-      <c r="BN14" s="64"/>
-      <c r="BO14" s="64"/>
-      <c r="BP14" s="64"/>
+      <c r="B15" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="28">
+        <v>1</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="43"/>
+      <c r="AK15" s="30"/>
+      <c r="AL15" s="30"/>
+      <c r="AM15" s="30"/>
+      <c r="AN15" s="30"/>
+      <c r="AO15" s="30"/>
+      <c r="AP15" s="30"/>
+      <c r="AQ15" s="30"/>
+      <c r="AR15" s="30"/>
+      <c r="AS15" s="30"/>
+      <c r="AT15" s="30"/>
+      <c r="AU15" s="30"/>
+      <c r="AV15" s="30"/>
+      <c r="AW15" s="30"/>
+      <c r="AX15" s="30"/>
+      <c r="AY15" s="30"/>
+      <c r="AZ15" s="30"/>
+      <c r="BA15" s="30"/>
+      <c r="BB15" s="30"/>
+      <c r="BC15" s="30"/>
+      <c r="BD15" s="29">
+        <v>0</v>
+      </c>
+      <c r="BF15" s="65"/>
+      <c r="BG15" s="65"/>
+      <c r="BH15" s="65"/>
+      <c r="BI15" s="65"/>
+      <c r="BJ15" s="65">
+        <v>100</v>
+      </c>
+      <c r="BK15" s="65"/>
+      <c r="BL15" s="65"/>
+      <c r="BM15" s="65">
+        <v>100</v>
+      </c>
+      <c r="BN15" s="65"/>
+      <c r="BO15" s="65"/>
+      <c r="BP15" s="65">
+        <v>100</v>
+      </c>
     </row>
-    <row r="15" spans="1:69" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="12" t="s">
+    <row r="16" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C16" s="14">
+        <v>1</v>
+      </c>
+      <c r="D16" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="42"/>
-      <c r="I15" s="13">
+      <c r="E16" s="42"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="37"/>
+      <c r="R16" s="37"/>
+      <c r="S16" s="37"/>
+      <c r="T16" s="37"/>
+      <c r="U16" s="37"/>
+      <c r="V16" s="37"/>
+      <c r="W16" s="37"/>
+      <c r="X16" s="37"/>
+      <c r="Y16" s="37"/>
+      <c r="Z16" s="37"/>
+      <c r="AA16" s="37"/>
+      <c r="AB16" s="37"/>
+      <c r="AC16" s="37"/>
+      <c r="AD16" s="37"/>
+      <c r="AE16" s="37"/>
+      <c r="AF16" s="37"/>
+      <c r="AG16" s="37"/>
+      <c r="AH16" s="37"/>
+      <c r="AI16" s="37"/>
+      <c r="AJ16" s="37"/>
+      <c r="AK16" s="37"/>
+      <c r="AL16" s="37"/>
+      <c r="AM16" s="37"/>
+      <c r="AN16" s="37"/>
+      <c r="AO16" s="37"/>
+      <c r="AP16" s="37"/>
+      <c r="AQ16" s="37"/>
+      <c r="AR16" s="37"/>
+      <c r="AS16" s="37"/>
+      <c r="AT16" s="37"/>
+      <c r="AU16" s="37"/>
+      <c r="AV16" s="37"/>
+      <c r="AW16" s="37"/>
+      <c r="AX16" s="37"/>
+      <c r="AY16" s="37"/>
+      <c r="AZ16" s="37"/>
+      <c r="BA16" s="37"/>
+      <c r="BB16" s="37"/>
+      <c r="BC16" s="37"/>
+      <c r="BD16" s="37">
         <v>0</v>
       </c>
-      <c r="V15" s="13">
-        <v>10</v>
-      </c>
-      <c r="AB15" s="13">
-        <v>8</v>
-      </c>
-      <c r="AK15" s="24"/>
-      <c r="AL15" s="24"/>
-      <c r="AM15" s="24"/>
-      <c r="AN15" s="24"/>
-      <c r="AO15" s="24"/>
-      <c r="AP15" s="24"/>
-      <c r="AQ15" s="24"/>
-      <c r="AR15" s="24"/>
-      <c r="AS15" s="24"/>
-      <c r="AT15" s="24"/>
-      <c r="AU15" s="24"/>
-      <c r="AV15" s="24"/>
-      <c r="AW15" s="24"/>
-      <c r="AX15" s="24"/>
-      <c r="AY15" s="24"/>
-      <c r="AZ15" s="24"/>
-      <c r="BA15" s="24"/>
-      <c r="BB15" s="24"/>
-      <c r="BC15" s="24"/>
-      <c r="BD15" s="13">
-        <v>5</v>
-      </c>
-      <c r="BF15" s="64"/>
-      <c r="BG15" s="64">
-        <v>1.3</v>
-      </c>
-      <c r="BH15" s="64"/>
-      <c r="BI15" s="64"/>
-      <c r="BJ15" s="64"/>
-      <c r="BK15" s="64"/>
-      <c r="BL15" s="64"/>
-      <c r="BM15" s="64"/>
-      <c r="BN15" s="64"/>
-      <c r="BO15" s="64"/>
-      <c r="BP15" s="64"/>
-    </row>
-    <row r="16" spans="1:69" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="29">
-        <v>1</v>
-      </c>
-      <c r="D16" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="44"/>
-      <c r="AK16" s="31"/>
-      <c r="AL16" s="31"/>
-      <c r="AM16" s="31"/>
-      <c r="AN16" s="31"/>
-      <c r="AO16" s="31"/>
-      <c r="AP16" s="31"/>
-      <c r="AQ16" s="31"/>
-      <c r="AR16" s="31"/>
-      <c r="AS16" s="31"/>
-      <c r="AT16" s="31"/>
-      <c r="AU16" s="31"/>
-      <c r="AV16" s="31"/>
-      <c r="AW16" s="31"/>
-      <c r="AX16" s="31"/>
-      <c r="AY16" s="31"/>
-      <c r="AZ16" s="31"/>
-      <c r="BA16" s="31"/>
-      <c r="BB16" s="31"/>
-      <c r="BC16" s="31"/>
-      <c r="BD16" s="30">
-        <v>0</v>
-      </c>
-      <c r="BF16" s="66"/>
+      <c r="BE16" s="37"/>
+      <c r="BF16" s="66">
+        <v>100</v>
+      </c>
       <c r="BG16" s="66"/>
       <c r="BH16" s="66"/>
       <c r="BI16" s="66"/>
-      <c r="BJ16" s="66">
-        <v>100</v>
-      </c>
+      <c r="BJ16" s="66"/>
       <c r="BK16" s="66"/>
       <c r="BL16" s="66"/>
       <c r="BM16" s="66">
@@ -3342,10 +3346,18 @@
       <c r="BP16" s="66">
         <v>100</v>
       </c>
+      <c r="BQ16" s="37"/>
+      <c r="BR16" s="37"/>
+      <c r="BS16" s="37"/>
+      <c r="BT16" s="37"/>
+      <c r="BU16" s="37"/>
+      <c r="BV16" s="37"/>
+      <c r="BW16" s="37"/>
+      <c r="BX16" s="37"/>
     </row>
     <row r="17" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>3</v>
@@ -3356,461 +3368,385 @@
       <c r="D17" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="43"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
-      <c r="L17" s="38"/>
-      <c r="M17" s="38"/>
-      <c r="N17" s="38"/>
-      <c r="O17" s="38"/>
-      <c r="P17" s="38"/>
-      <c r="Q17" s="38"/>
-      <c r="R17" s="38"/>
-      <c r="S17" s="38"/>
-      <c r="T17" s="38"/>
-      <c r="U17" s="38"/>
-      <c r="V17" s="38"/>
-      <c r="W17" s="38"/>
-      <c r="X17" s="38"/>
-      <c r="Y17" s="38"/>
-      <c r="Z17" s="38"/>
-      <c r="AA17" s="38"/>
-      <c r="AB17" s="38"/>
-      <c r="AC17" s="38"/>
-      <c r="AD17" s="38"/>
-      <c r="AE17" s="38"/>
-      <c r="AF17" s="38"/>
-      <c r="AG17" s="38"/>
-      <c r="AH17" s="38"/>
-      <c r="AI17" s="38"/>
-      <c r="AJ17" s="38"/>
-      <c r="AK17" s="38"/>
-      <c r="AL17" s="38"/>
-      <c r="AM17" s="38"/>
-      <c r="AN17" s="38"/>
-      <c r="AO17" s="38"/>
-      <c r="AP17" s="38"/>
-      <c r="AQ17" s="38"/>
-      <c r="AR17" s="38"/>
-      <c r="AS17" s="38"/>
-      <c r="AT17" s="38"/>
-      <c r="AU17" s="38"/>
-      <c r="AV17" s="38"/>
-      <c r="AW17" s="38"/>
-      <c r="AX17" s="38"/>
-      <c r="AY17" s="38"/>
-      <c r="AZ17" s="38"/>
-      <c r="BA17" s="38"/>
-      <c r="BB17" s="38"/>
-      <c r="BC17" s="38"/>
-      <c r="BD17" s="38">
+      <c r="E17" s="42"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="37"/>
+      <c r="S17" s="37"/>
+      <c r="T17" s="37"/>
+      <c r="U17" s="37"/>
+      <c r="V17" s="37"/>
+      <c r="W17" s="37"/>
+      <c r="X17" s="37"/>
+      <c r="Y17" s="37"/>
+      <c r="Z17" s="37"/>
+      <c r="AA17" s="37"/>
+      <c r="AB17" s="37"/>
+      <c r="AC17" s="37"/>
+      <c r="AD17" s="37"/>
+      <c r="AE17" s="37"/>
+      <c r="AF17" s="37"/>
+      <c r="AG17" s="37"/>
+      <c r="AH17" s="37"/>
+      <c r="AI17" s="37"/>
+      <c r="AJ17" s="37"/>
+      <c r="AK17" s="37"/>
+      <c r="AL17" s="37"/>
+      <c r="AM17" s="37"/>
+      <c r="AN17" s="37"/>
+      <c r="AO17" s="37"/>
+      <c r="AP17" s="37"/>
+      <c r="AQ17" s="37"/>
+      <c r="AR17" s="37"/>
+      <c r="AS17" s="37"/>
+      <c r="AT17" s="37"/>
+      <c r="AU17" s="37"/>
+      <c r="AV17" s="37"/>
+      <c r="AW17" s="37"/>
+      <c r="AX17" s="37"/>
+      <c r="AY17" s="37"/>
+      <c r="AZ17" s="37"/>
+      <c r="BA17" s="37"/>
+      <c r="BB17" s="37"/>
+      <c r="BC17" s="37"/>
+      <c r="BD17" s="37">
         <v>0</v>
       </c>
-      <c r="BE17" s="38"/>
-      <c r="BF17" s="67">
+      <c r="BE17" s="37"/>
+      <c r="BF17" s="66"/>
+      <c r="BG17" s="66"/>
+      <c r="BH17" s="66">
+        <v>17</v>
+      </c>
+      <c r="BI17" s="66">
+        <v>70</v>
+      </c>
+      <c r="BJ17" s="66"/>
+      <c r="BK17" s="66"/>
+      <c r="BL17" s="66"/>
+      <c r="BM17" s="66">
+        <v>70</v>
+      </c>
+      <c r="BN17" s="66"/>
+      <c r="BO17" s="66"/>
+      <c r="BP17" s="66">
+        <v>70</v>
+      </c>
+      <c r="BQ17" s="37"/>
+      <c r="BR17" s="37"/>
+      <c r="BS17" s="37"/>
+      <c r="BT17" s="37"/>
+      <c r="BU17" s="37"/>
+      <c r="BV17" s="37"/>
+      <c r="BW17" s="37"/>
+      <c r="BX17" s="37"/>
+    </row>
+    <row r="18" spans="1:76" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="46">
+        <v>1</v>
+      </c>
+      <c r="D18" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="47"/>
+      <c r="BD18" s="48">
+        <v>0</v>
+      </c>
+      <c r="BF18" s="61"/>
+      <c r="BG18" s="61"/>
+      <c r="BH18" s="61"/>
+      <c r="BI18" s="61"/>
+      <c r="BJ18" s="61"/>
+      <c r="BK18" s="61"/>
+      <c r="BL18" s="61"/>
+      <c r="BM18" s="61"/>
+      <c r="BN18" s="61"/>
+      <c r="BO18" s="61"/>
+      <c r="BP18" s="61"/>
+    </row>
+    <row r="19" spans="1:76" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="46">
+        <v>1</v>
+      </c>
+      <c r="D19" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="47"/>
+      <c r="BD19" s="48">
+        <v>0</v>
+      </c>
+      <c r="BF19" s="61"/>
+      <c r="BG19" s="61"/>
+      <c r="BH19" s="61"/>
+      <c r="BI19" s="61"/>
+      <c r="BJ19" s="61"/>
+      <c r="BK19" s="61">
+        <v>50</v>
+      </c>
+      <c r="BL19" s="61"/>
+      <c r="BM19" s="61">
+        <v>50</v>
+      </c>
+      <c r="BN19" s="61"/>
+      <c r="BO19" s="61"/>
+      <c r="BP19" s="61">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:76" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="50">
+        <v>1</v>
+      </c>
+      <c r="D20" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="51">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="F20" s="52">
+        <v>4.84</v>
+      </c>
+      <c r="G20" s="52">
+        <v>5.44</v>
+      </c>
+      <c r="H20" s="52">
+        <v>6.11</v>
+      </c>
+      <c r="I20" s="52">
+        <v>6.86</v>
+      </c>
+      <c r="J20" s="52">
+        <v>7.7</v>
+      </c>
+      <c r="K20" s="52">
+        <v>8.68</v>
+      </c>
+      <c r="L20" s="52">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="M20" s="52">
+        <v>9.41</v>
+      </c>
+      <c r="N20" s="52">
+        <v>11.48</v>
+      </c>
+      <c r="O20" s="52">
+        <v>12.75</v>
+      </c>
+      <c r="P20" s="52">
+        <v>14.6</v>
+      </c>
+      <c r="Q20" s="52">
+        <v>16.5</v>
+      </c>
+      <c r="R20" s="52">
+        <v>18.38</v>
+      </c>
+      <c r="S20" s="52">
+        <v>19.670000000000002</v>
+      </c>
+      <c r="T20" s="52">
+        <v>20.87</v>
+      </c>
+      <c r="U20" s="52">
+        <v>22.5</v>
+      </c>
+      <c r="V20" s="52">
+        <v>25.9</v>
+      </c>
+      <c r="W20" s="52">
+        <v>28.8</v>
+      </c>
+      <c r="X20" s="52">
+        <v>30.8</v>
+      </c>
+      <c r="Y20" s="52">
+        <v>32.9</v>
+      </c>
+      <c r="Z20" s="52">
+        <v>34.6</v>
+      </c>
+      <c r="AA20" s="52">
+        <v>36.1</v>
+      </c>
+      <c r="AB20" s="52">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="AC20" s="52">
+        <v>38.9</v>
+      </c>
+      <c r="AD20" s="52">
+        <v>43.4</v>
+      </c>
+      <c r="AE20" s="52">
+        <v>46.1</v>
+      </c>
+      <c r="AF20" s="52">
+        <v>49.9</v>
+      </c>
+      <c r="AG20" s="52">
+        <v>53.1</v>
+      </c>
+      <c r="AH20" s="52">
+        <v>55.7</v>
+      </c>
+      <c r="AI20" s="52">
+        <v>58.6</v>
+      </c>
+      <c r="AJ20" s="52">
+        <v>59.1</v>
+      </c>
+      <c r="AK20" s="52">
+        <v>60.4</v>
+      </c>
+      <c r="AL20" s="52">
+        <v>62.2</v>
+      </c>
+      <c r="AM20" s="52">
+        <v>64.3</v>
+      </c>
+      <c r="AN20" s="52">
+        <v>68</v>
+      </c>
+      <c r="AO20" s="52">
+        <v>69.3</v>
+      </c>
+      <c r="AP20" s="52">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="AQ20" s="52">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="AR20" s="52">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="AS20" s="52">
+        <v>76.7</v>
+      </c>
+      <c r="AT20" s="52">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="AU20" s="52">
+        <v>80.8</v>
+      </c>
+      <c r="AV20" s="52">
+        <v>82.8</v>
+      </c>
+      <c r="AW20" s="52">
+        <v>86.7</v>
+      </c>
+      <c r="AX20" s="52">
+        <v>93.4</v>
+      </c>
+      <c r="AY20" s="52">
+        <v>96.5</v>
+      </c>
+      <c r="AZ20" s="52">
         <v>100</v>
       </c>
-      <c r="BG17" s="67"/>
-      <c r="BH17" s="67"/>
-      <c r="BI17" s="67"/>
-      <c r="BJ17" s="67"/>
-      <c r="BK17" s="67"/>
-      <c r="BL17" s="67"/>
-      <c r="BM17" s="67">
-        <v>100</v>
-      </c>
-      <c r="BN17" s="67"/>
-      <c r="BO17" s="67"/>
-      <c r="BP17" s="67">
-        <v>100</v>
-      </c>
-      <c r="BQ17" s="38"/>
-      <c r="BR17" s="38"/>
-      <c r="BS17" s="38"/>
-      <c r="BT17" s="38"/>
-      <c r="BU17" s="38"/>
-      <c r="BV17" s="38"/>
-      <c r="BW17" s="38"/>
-      <c r="BX17" s="38"/>
+      <c r="BA20" s="52">
+        <v>107.3</v>
+      </c>
+      <c r="BB20" s="52">
+        <v>110.9</v>
+      </c>
+      <c r="BC20" s="52">
+        <v>114.2</v>
+      </c>
+      <c r="BD20" s="52">
+        <v>114.8</v>
+      </c>
+      <c r="BE20" s="52">
+        <v>116.4</v>
+      </c>
+      <c r="BF20" s="67"/>
+      <c r="BG20" s="67"/>
+      <c r="BH20" s="67"/>
+      <c r="BI20" s="67"/>
+      <c r="BJ20" s="67"/>
+      <c r="BK20" s="67"/>
+      <c r="BL20" s="67"/>
+      <c r="BM20" s="67"/>
+      <c r="BN20" s="67"/>
+      <c r="BO20" s="67"/>
+      <c r="BP20" s="67"/>
     </row>
-    <row r="18" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="14" t="s">
+    <row r="21" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C21" s="14">
         <v>1</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D21" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="43">
-        <v>0</v>
-      </c>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
-      <c r="L18" s="38"/>
-      <c r="M18" s="38"/>
-      <c r="N18" s="38"/>
-      <c r="O18" s="38"/>
-      <c r="P18" s="38"/>
-      <c r="Q18" s="38"/>
-      <c r="R18" s="38"/>
-      <c r="S18" s="38"/>
-      <c r="T18" s="38"/>
-      <c r="U18" s="38"/>
-      <c r="V18" s="38"/>
-      <c r="W18" s="38"/>
-      <c r="X18" s="38"/>
-      <c r="Y18" s="38"/>
-      <c r="Z18" s="38"/>
-      <c r="AA18" s="38"/>
-      <c r="AB18" s="38"/>
-      <c r="AC18" s="38"/>
-      <c r="AD18" s="38"/>
-      <c r="AE18" s="38"/>
-      <c r="AF18" s="38"/>
-      <c r="AG18" s="38"/>
-      <c r="AH18" s="38"/>
-      <c r="AI18" s="38"/>
-      <c r="AJ18" s="38"/>
-      <c r="AK18" s="38"/>
-      <c r="AL18" s="38"/>
-      <c r="AM18" s="38"/>
-      <c r="AN18" s="38"/>
-      <c r="AO18" s="38"/>
-      <c r="AP18" s="38"/>
-      <c r="AQ18" s="38"/>
-      <c r="AR18" s="38"/>
-      <c r="AS18" s="38"/>
-      <c r="AT18" s="38"/>
-      <c r="AU18" s="38"/>
-      <c r="AV18" s="38"/>
-      <c r="AW18" s="38"/>
-      <c r="AX18" s="38"/>
-      <c r="AY18" s="38"/>
-      <c r="AZ18" s="38"/>
-      <c r="BA18" s="38"/>
-      <c r="BB18" s="38"/>
-      <c r="BC18" s="38"/>
-      <c r="BD18" s="38">
-        <v>0</v>
-      </c>
-      <c r="BE18" s="38"/>
-      <c r="BF18" s="67"/>
-      <c r="BG18" s="67"/>
-      <c r="BH18" s="67">
-        <v>17</v>
-      </c>
-      <c r="BI18" s="67">
-        <v>70</v>
-      </c>
-      <c r="BJ18" s="67"/>
-      <c r="BK18" s="67"/>
-      <c r="BL18" s="67"/>
-      <c r="BM18" s="67">
-        <v>70</v>
-      </c>
-      <c r="BN18" s="67"/>
-      <c r="BO18" s="67"/>
-      <c r="BP18" s="67">
-        <v>70</v>
-      </c>
-      <c r="BQ18" s="38"/>
-      <c r="BR18" s="38"/>
-      <c r="BS18" s="38"/>
-      <c r="BT18" s="38"/>
-      <c r="BU18" s="38"/>
-      <c r="BV18" s="38"/>
-      <c r="BW18" s="38"/>
-      <c r="BX18" s="38"/>
+      <c r="E21" s="42">
+        <v>1</v>
+      </c>
+      <c r="K21" s="15">
+        <v>1</v>
+      </c>
+      <c r="U21" s="15">
+        <v>1</v>
+      </c>
+      <c r="V21" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="BA21" s="15">
+        <v>3.11</v>
+      </c>
+      <c r="BF21" s="64"/>
+      <c r="BG21" s="64"/>
+      <c r="BH21" s="64"/>
+      <c r="BI21" s="64"/>
+      <c r="BJ21" s="64"/>
+      <c r="BK21" s="64"/>
+      <c r="BL21" s="64"/>
+      <c r="BM21" s="64"/>
+      <c r="BN21" s="64"/>
+      <c r="BO21" s="64"/>
+      <c r="BP21" s="64"/>
     </row>
-    <row r="19" spans="1:76" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="47">
-        <v>1</v>
-      </c>
-      <c r="D19" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="48"/>
-      <c r="BD19" s="49">
-        <v>0</v>
-      </c>
-      <c r="BF19" s="62"/>
-      <c r="BG19" s="62"/>
-      <c r="BH19" s="62"/>
-      <c r="BI19" s="62"/>
-      <c r="BJ19" s="62"/>
-      <c r="BK19" s="62"/>
-      <c r="BL19" s="62"/>
-      <c r="BM19" s="62"/>
-      <c r="BN19" s="62"/>
-      <c r="BO19" s="62"/>
-      <c r="BP19" s="62"/>
-    </row>
-    <row r="20" spans="1:76" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="47">
-        <v>1</v>
-      </c>
-      <c r="D20" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="48"/>
-      <c r="BD20" s="49">
-        <v>0</v>
-      </c>
-      <c r="BF20" s="62"/>
-      <c r="BG20" s="62"/>
-      <c r="BH20" s="62"/>
-      <c r="BI20" s="62"/>
-      <c r="BJ20" s="62"/>
-      <c r="BK20" s="62">
-        <v>50</v>
-      </c>
-      <c r="BL20" s="62"/>
-      <c r="BM20" s="62">
-        <v>50</v>
-      </c>
-      <c r="BN20" s="62"/>
-      <c r="BO20" s="62"/>
-      <c r="BP20" s="62">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:76" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="51" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="51">
-        <v>1</v>
-      </c>
-      <c r="D21" s="51" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="52">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="F21" s="53">
-        <v>4.84</v>
-      </c>
-      <c r="G21" s="53">
-        <v>5.44</v>
-      </c>
-      <c r="H21" s="53">
-        <v>6.11</v>
-      </c>
-      <c r="I21" s="53">
-        <v>6.86</v>
-      </c>
-      <c r="J21" s="53">
-        <v>7.7</v>
-      </c>
-      <c r="K21" s="53">
-        <v>8.68</v>
-      </c>
-      <c r="L21" s="53">
-        <v>9.0399999999999991</v>
-      </c>
-      <c r="M21" s="53">
-        <v>9.41</v>
-      </c>
-      <c r="N21" s="53">
-        <v>11.48</v>
-      </c>
-      <c r="O21" s="53">
-        <v>12.75</v>
-      </c>
-      <c r="P21" s="53">
-        <v>14.6</v>
-      </c>
-      <c r="Q21" s="53">
-        <v>16.5</v>
-      </c>
-      <c r="R21" s="53">
-        <v>18.38</v>
-      </c>
-      <c r="S21" s="53">
-        <v>19.670000000000002</v>
-      </c>
-      <c r="T21" s="53">
-        <v>20.87</v>
-      </c>
-      <c r="U21" s="53">
-        <v>22.5</v>
-      </c>
-      <c r="V21" s="53">
-        <v>25.9</v>
-      </c>
-      <c r="W21" s="53">
-        <v>28.8</v>
-      </c>
-      <c r="X21" s="53">
-        <v>30.8</v>
-      </c>
-      <c r="Y21" s="53">
-        <v>32.9</v>
-      </c>
-      <c r="Z21" s="53">
-        <v>34.6</v>
-      </c>
-      <c r="AA21" s="53">
-        <v>36.1</v>
-      </c>
-      <c r="AB21" s="53">
-        <v>36.799999999999997</v>
-      </c>
-      <c r="AC21" s="53">
-        <v>38.9</v>
-      </c>
-      <c r="AD21" s="53">
-        <v>43.4</v>
-      </c>
-      <c r="AE21" s="53">
-        <v>46.1</v>
-      </c>
-      <c r="AF21" s="53">
-        <v>49.9</v>
-      </c>
-      <c r="AG21" s="53">
-        <v>53.1</v>
-      </c>
-      <c r="AH21" s="53">
-        <v>55.7</v>
-      </c>
-      <c r="AI21" s="53">
-        <v>58.6</v>
-      </c>
-      <c r="AJ21" s="53">
-        <v>59.1</v>
-      </c>
-      <c r="AK21" s="53">
-        <v>60.4</v>
-      </c>
-      <c r="AL21" s="53">
-        <v>62.2</v>
-      </c>
-      <c r="AM21" s="53">
-        <v>64.3</v>
-      </c>
-      <c r="AN21" s="53">
-        <v>68</v>
-      </c>
-      <c r="AO21" s="53">
-        <v>69.3</v>
-      </c>
-      <c r="AP21" s="53">
-        <v>70.099999999999994</v>
-      </c>
-      <c r="AQ21" s="53">
-        <v>73.099999999999994</v>
-      </c>
-      <c r="AR21" s="53">
-        <v>73.599999999999994</v>
-      </c>
-      <c r="AS21" s="53">
-        <v>76.7</v>
-      </c>
-      <c r="AT21" s="53">
-        <v>78.900000000000006</v>
-      </c>
-      <c r="AU21" s="53">
-        <v>80.8</v>
-      </c>
-      <c r="AV21" s="53">
-        <v>82.8</v>
-      </c>
-      <c r="AW21" s="53">
-        <v>86.7</v>
-      </c>
-      <c r="AX21" s="53">
-        <v>93.4</v>
-      </c>
-      <c r="AY21" s="53">
-        <v>96.5</v>
-      </c>
-      <c r="AZ21" s="53">
-        <v>100</v>
-      </c>
-      <c r="BA21" s="53">
-        <v>107.3</v>
-      </c>
-      <c r="BB21" s="53">
-        <v>110.9</v>
-      </c>
-      <c r="BC21" s="53">
-        <v>114.2</v>
-      </c>
-      <c r="BD21" s="53">
-        <v>114.8</v>
-      </c>
-      <c r="BE21" s="53">
-        <v>116.4</v>
-      </c>
-      <c r="BF21" s="68"/>
-      <c r="BG21" s="68"/>
-      <c r="BH21" s="68"/>
-      <c r="BI21" s="68"/>
-      <c r="BJ21" s="68"/>
-      <c r="BK21" s="68"/>
-      <c r="BL21" s="68"/>
-      <c r="BM21" s="68"/>
-      <c r="BN21" s="68"/>
-      <c r="BO21" s="68"/>
-      <c r="BP21" s="68"/>
-    </row>
-    <row r="22" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
+    <row r="22" spans="1:76" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="14">
-        <v>1</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="43">
-        <v>1</v>
-      </c>
-      <c r="K22" s="15">
-        <v>1</v>
-      </c>
-      <c r="U22" s="15">
-        <v>1</v>
-      </c>
-      <c r="V22" s="15">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="BA22" s="15">
-        <v>3.11</v>
-      </c>
+      <c r="B22" s="57"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="43"/>
       <c r="BF22" s="65"/>
       <c r="BG22" s="65"/>
       <c r="BH22" s="65"/>
@@ -3823,129 +3759,106 @@
       <c r="BO22" s="65"/>
       <c r="BP22" s="65"/>
     </row>
-    <row r="23" spans="1:76" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="58"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="44"/>
-      <c r="BF23" s="66"/>
-      <c r="BG23" s="66"/>
-      <c r="BH23" s="66"/>
-      <c r="BI23" s="66"/>
-      <c r="BJ23" s="66"/>
-      <c r="BK23" s="66"/>
-      <c r="BL23" s="66"/>
-      <c r="BM23" s="66"/>
-      <c r="BN23" s="66"/>
-      <c r="BO23" s="66"/>
-      <c r="BP23" s="66"/>
+    <row r="23" spans="1:76" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="28">
+        <v>1</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="43"/>
+      <c r="BD23" s="29">
+        <v>1</v>
+      </c>
+      <c r="BF23" s="65"/>
+      <c r="BG23" s="65"/>
+      <c r="BH23" s="65"/>
+      <c r="BI23" s="65"/>
+      <c r="BJ23" s="65"/>
+      <c r="BK23" s="65"/>
+      <c r="BL23" s="65"/>
+      <c r="BM23" s="65"/>
+      <c r="BN23" s="65"/>
+      <c r="BO23" s="65"/>
+      <c r="BP23" s="65"/>
     </row>
-    <row r="24" spans="1:76" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="58" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="29">
+    <row r="24" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="2">
         <v>1</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="D24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="44"/>
-      <c r="BD24" s="30">
-        <v>1</v>
-      </c>
-      <c r="BF24" s="66"/>
-      <c r="BG24" s="66"/>
-      <c r="BH24" s="66"/>
-      <c r="BI24" s="66"/>
-      <c r="BJ24" s="66"/>
-      <c r="BK24" s="66"/>
-      <c r="BL24" s="66"/>
-      <c r="BM24" s="66"/>
-      <c r="BN24" s="66"/>
-      <c r="BO24" s="66"/>
-      <c r="BP24" s="66"/>
-    </row>
-    <row r="25" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="2">
-        <v>1</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="45">
+      <c r="E24" s="44">
         <v>0</v>
       </c>
-      <c r="K25" s="1">
+      <c r="T24" s="1">
         <v>0</v>
       </c>
-      <c r="T25" s="1">
-        <v>0</v>
-      </c>
-      <c r="V25" s="1">
+      <c r="V24" s="1">
         <v>7.7</v>
       </c>
-      <c r="AI25" s="1">
+      <c r="AI24" s="1">
         <v>11.1</v>
       </c>
-      <c r="AR25" s="1">
+      <c r="AR24" s="1">
         <v>16.5</v>
       </c>
-      <c r="AT25" s="1">
+      <c r="AT24" s="1">
         <v>14.5</v>
       </c>
-      <c r="AY25" s="1">
+      <c r="AY24" s="1">
         <v>16.100000000000001</v>
       </c>
-      <c r="BA25" s="1">
+      <c r="BA24" s="1">
         <v>15.6</v>
       </c>
-      <c r="BC25" s="1">
+      <c r="BC24" s="1">
         <v>15.6</v>
       </c>
-      <c r="BE25" s="1">
+      <c r="BE24" s="1">
         <v>15.6</v>
       </c>
-      <c r="BF25" s="69"/>
-      <c r="BG25" s="69"/>
-      <c r="BH25" s="69"/>
-      <c r="BI25" s="69"/>
-      <c r="BJ25" s="69"/>
-      <c r="BK25" s="69"/>
-      <c r="BL25" s="69"/>
-      <c r="BM25" s="69"/>
-      <c r="BN25" s="69"/>
-      <c r="BO25" s="69"/>
-      <c r="BP25" s="69"/>
+      <c r="BF24" s="68"/>
+      <c r="BG24" s="68"/>
+      <c r="BH24" s="68"/>
+      <c r="BI24" s="68"/>
+      <c r="BJ24" s="68"/>
+      <c r="BK24" s="68"/>
+      <c r="BL24" s="68"/>
+      <c r="BM24" s="68"/>
+      <c r="BN24" s="68"/>
+      <c r="BO24" s="68"/>
+      <c r="BP24" s="68"/>
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="5">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF16:BG16 F5:BG8">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF15:BG15 F4:BG7">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:D1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10:BG15 F16:BE16 F2:BG4">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:BG14 F15:BE15 F2:BG3">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C25:C1048576 C2:C22">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C24:C1048576 C2:C21">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Leave blank" sqref="B23:D24"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Leave blank" sqref="B22:D23"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3956,13 +3869,13 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B8 B10:B16</xm:sqref>
+          <xm:sqref>B9:B15 B2:B7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time-variant?" prompt="If no, the most recent value will be selected.">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D25:D1048576 D2:D22</xm:sqref>
+          <xm:sqref>D24:D1048576 D2:D21</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Final round of spreadsheet rationalisation
Remove unnecessary time variants (which are now optional) from Fiji
sheets.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
   <si>
     <t>parameter</t>
   </si>
@@ -117,9 +117,6 @@
     <t>program_perc_detect</t>
   </si>
   <si>
-    <t>program_perc_ipt</t>
-  </si>
-  <si>
     <t>program_perc_ipt_age0to5</t>
   </si>
   <si>
@@ -129,22 +126,13 @@
     <t>program_perc_algorithm_sensitivity</t>
   </si>
   <si>
-    <t>program_perc_lowquality</t>
-  </si>
-  <si>
     <t>program_perc_firstline_dst</t>
   </si>
   <si>
-    <t>program_perc_secondline_dst</t>
-  </si>
-  <si>
     <t>program_perc_xpert</t>
   </si>
   <si>
     <t>program_perc_treatment_support</t>
-  </si>
-  <si>
-    <t>program_perc_smearacf</t>
   </si>
   <si>
     <t>program_perc_xpertacf</t>
@@ -2315,7 +2303,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B6" s="32">
         <v>5</v>
@@ -2357,13 +2345,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BX24"/>
+  <dimension ref="A1:BX20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomRight" activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2601,12 +2589,12 @@
         <v>27</v>
       </c>
       <c r="BQ1" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:76" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>4</v>
@@ -2786,8 +2774,14 @@
         <v>3</v>
       </c>
       <c r="E4" s="39"/>
+      <c r="BA4" s="9">
+        <v>0</v>
+      </c>
+      <c r="BB4" s="9">
+        <v>7</v>
+      </c>
       <c r="BD4" s="9">
-        <v>0</v>
+        <v>23.6</v>
       </c>
       <c r="BF4" s="60"/>
       <c r="BG4" s="60"/>
@@ -2795,11 +2789,17 @@
       <c r="BI4" s="60"/>
       <c r="BJ4" s="60"/>
       <c r="BK4" s="60"/>
-      <c r="BL4" s="60"/>
-      <c r="BM4" s="60"/>
+      <c r="BL4" s="60">
+        <v>80</v>
+      </c>
+      <c r="BM4" s="60">
+        <v>80</v>
+      </c>
       <c r="BN4" s="60"/>
       <c r="BO4" s="60"/>
-      <c r="BP4" s="60"/>
+      <c r="BP4" s="60">
+        <v>80</v>
+      </c>
     </row>
     <row r="5" spans="1:76" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -2815,14 +2815,8 @@
         <v>3</v>
       </c>
       <c r="E5" s="39"/>
-      <c r="BA5" s="9">
+      <c r="BD5" s="9">
         <v>0</v>
-      </c>
-      <c r="BB5" s="9">
-        <v>7</v>
-      </c>
-      <c r="BD5" s="9">
-        <v>23.6</v>
       </c>
       <c r="BF5" s="60"/>
       <c r="BG5" s="60"/>
@@ -2844,10 +2838,10 @@
     </row>
     <row r="6" spans="1:76" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="8">
         <v>1</v>
@@ -2865,130 +2859,130 @@
       <c r="BI6" s="60"/>
       <c r="BJ6" s="60"/>
       <c r="BK6" s="60"/>
-      <c r="BL6" s="60">
-        <v>80</v>
-      </c>
-      <c r="BM6" s="60">
-        <v>80</v>
-      </c>
+      <c r="BL6" s="60"/>
+      <c r="BM6" s="60"/>
       <c r="BN6" s="60"/>
       <c r="BO6" s="60"/>
-      <c r="BP6" s="60">
+      <c r="BP6" s="9">
+        <v>10</v>
+      </c>
+      <c r="BQ6" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:76" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="46">
+        <v>1</v>
+      </c>
+      <c r="D7" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="47"/>
+      <c r="BD7" s="48">
+        <v>0</v>
+      </c>
+      <c r="BF7" s="61"/>
+      <c r="BG7" s="61"/>
+      <c r="BH7" s="61"/>
+      <c r="BI7" s="61"/>
+      <c r="BJ7" s="61"/>
+      <c r="BK7" s="61"/>
+      <c r="BL7" s="61"/>
+      <c r="BM7" s="61"/>
+      <c r="BN7" s="61">
+        <v>10</v>
+      </c>
+      <c r="BO7" s="61"/>
+      <c r="BP7" s="61"/>
+    </row>
+    <row r="8" spans="1:76" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="10">
+        <v>1</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="40"/>
+      <c r="F8" s="11">
+        <v>70</v>
+      </c>
+      <c r="J8" s="11">
         <v>80</v>
       </c>
+      <c r="AD8" s="11">
+        <v>82</v>
+      </c>
+      <c r="AQ8" s="11">
+        <v>84</v>
+      </c>
+      <c r="BC8" s="11">
+        <v>85</v>
+      </c>
+      <c r="BF8" s="62"/>
+      <c r="BG8" s="62"/>
+      <c r="BH8" s="62"/>
+      <c r="BI8" s="62"/>
+      <c r="BJ8" s="62"/>
+      <c r="BK8" s="62"/>
+      <c r="BL8" s="62"/>
+      <c r="BM8" s="62"/>
+      <c r="BN8" s="62"/>
+      <c r="BO8" s="62"/>
+      <c r="BP8" s="62"/>
     </row>
-    <row r="7" spans="1:76" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="8" t="s">
+    <row r="9" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C9" s="14">
         <v>1</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D9" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="39"/>
-      <c r="BD7" s="9">
-        <v>0</v>
-      </c>
-      <c r="BF7" s="60"/>
-      <c r="BG7" s="60"/>
-      <c r="BH7" s="60"/>
-      <c r="BI7" s="60"/>
-      <c r="BJ7" s="60"/>
-      <c r="BK7" s="60"/>
-      <c r="BL7" s="60"/>
-      <c r="BM7" s="60"/>
-      <c r="BN7" s="60"/>
-      <c r="BO7" s="60"/>
-      <c r="BP7" s="9">
-        <v>10</v>
-      </c>
-      <c r="BQ7" s="9">
+      <c r="E9" s="42"/>
+      <c r="V9" s="15">
+        <v>30</v>
+      </c>
+      <c r="AF9" s="15">
+        <v>40</v>
+      </c>
+      <c r="AP9" s="15">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:76" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="46">
-        <v>1</v>
-      </c>
-      <c r="D8" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="47"/>
-      <c r="BD8" s="48">
-        <v>0</v>
-      </c>
-      <c r="BF8" s="61"/>
-      <c r="BG8" s="61"/>
-      <c r="BH8" s="61"/>
-      <c r="BI8" s="61"/>
-      <c r="BJ8" s="61"/>
-      <c r="BK8" s="61"/>
-      <c r="BL8" s="61"/>
-      <c r="BM8" s="61"/>
-      <c r="BN8" s="61">
-        <v>10</v>
-      </c>
-      <c r="BO8" s="61"/>
-      <c r="BP8" s="61"/>
-    </row>
-    <row r="9" spans="1:76" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="10">
-        <v>1</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="40"/>
-      <c r="F9" s="11">
-        <v>70</v>
-      </c>
-      <c r="J9" s="11">
-        <v>80</v>
-      </c>
-      <c r="AD9" s="11">
-        <v>82</v>
-      </c>
-      <c r="AQ9" s="11">
-        <v>84</v>
-      </c>
-      <c r="BC9" s="11">
-        <v>85</v>
-      </c>
-      <c r="BF9" s="62"/>
-      <c r="BG9" s="62"/>
-      <c r="BH9" s="62"/>
-      <c r="BI9" s="62"/>
-      <c r="BJ9" s="62"/>
-      <c r="BK9" s="62"/>
-      <c r="BL9" s="62"/>
-      <c r="BM9" s="62"/>
-      <c r="BN9" s="62"/>
-      <c r="BO9" s="62"/>
-      <c r="BP9" s="62"/>
+      <c r="BF9" s="64"/>
+      <c r="BG9" s="64"/>
+      <c r="BH9" s="64"/>
+      <c r="BI9" s="64"/>
+      <c r="BJ9" s="64"/>
+      <c r="BK9" s="64"/>
+      <c r="BL9" s="64"/>
+      <c r="BM9" s="64"/>
+      <c r="BN9" s="64"/>
+      <c r="BO9" s="64"/>
+      <c r="BP9" s="64"/>
     </row>
     <row r="10" spans="1:76" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" s="12">
         <v>1</v>
@@ -2997,17 +2991,42 @@
         <v>3</v>
       </c>
       <c r="E10" s="41"/>
-      <c r="H10" s="13">
-        <v>30</v>
-      </c>
-      <c r="K10" s="13">
+      <c r="I10" s="13">
+        <v>0</v>
+      </c>
+      <c r="V10" s="13">
         <v>40</v>
       </c>
-      <c r="AF10" s="13">
-        <v>40</v>
+      <c r="AB10" s="13">
+        <v>65</v>
+      </c>
+      <c r="AK10" s="23"/>
+      <c r="AL10" s="23"/>
+      <c r="AM10" s="23"/>
+      <c r="AN10" s="23"/>
+      <c r="AO10" s="23"/>
+      <c r="AP10" s="23"/>
+      <c r="AQ10" s="23"/>
+      <c r="AR10" s="23"/>
+      <c r="AS10" s="23"/>
+      <c r="AT10" s="23"/>
+      <c r="AU10" s="23"/>
+      <c r="AV10" s="23"/>
+      <c r="AW10" s="23"/>
+      <c r="AX10" s="23"/>
+      <c r="AY10" s="23"/>
+      <c r="AZ10" s="23"/>
+      <c r="BA10" s="23"/>
+      <c r="BB10" s="23">
+        <v>93</v>
+      </c>
+      <c r="BC10" s="23">
+        <v>85</v>
       </c>
       <c r="BF10" s="63"/>
-      <c r="BG10" s="63"/>
+      <c r="BG10" s="63">
+        <v>96</v>
+      </c>
       <c r="BH10" s="63"/>
       <c r="BI10" s="63"/>
       <c r="BJ10" s="63"/>
@@ -3018,346 +3037,531 @@
       <c r="BO10" s="63"/>
       <c r="BP10" s="63"/>
     </row>
-    <row r="11" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+    <row r="11" spans="1:76" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="12">
+        <v>3</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="41"/>
+      <c r="I11" s="13">
+        <v>0</v>
+      </c>
+      <c r="V11" s="13">
+        <v>10</v>
+      </c>
+      <c r="AB11" s="13">
+        <v>8</v>
+      </c>
+      <c r="AK11" s="23"/>
+      <c r="AL11" s="23"/>
+      <c r="AM11" s="23"/>
+      <c r="AN11" s="23"/>
+      <c r="AO11" s="23"/>
+      <c r="AP11" s="23"/>
+      <c r="AQ11" s="23"/>
+      <c r="AR11" s="23"/>
+      <c r="AS11" s="23"/>
+      <c r="AT11" s="23"/>
+      <c r="AU11" s="23"/>
+      <c r="AV11" s="23"/>
+      <c r="AW11" s="23"/>
+      <c r="AX11" s="23"/>
+      <c r="AY11" s="23"/>
+      <c r="AZ11" s="23"/>
+      <c r="BA11" s="23"/>
+      <c r="BB11" s="23"/>
+      <c r="BC11" s="23"/>
+      <c r="BD11" s="13">
+        <v>5</v>
+      </c>
+      <c r="BF11" s="63"/>
+      <c r="BG11" s="63">
+        <v>1.3</v>
+      </c>
+      <c r="BH11" s="63"/>
+      <c r="BI11" s="63"/>
+      <c r="BJ11" s="63"/>
+      <c r="BK11" s="63"/>
+      <c r="BL11" s="63"/>
+      <c r="BM11" s="63"/>
+      <c r="BN11" s="63"/>
+      <c r="BO11" s="63"/>
+      <c r="BP11" s="63"/>
+    </row>
+    <row r="12" spans="1:76" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="28">
+        <v>1</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="43"/>
+      <c r="AK12" s="30"/>
+      <c r="AL12" s="30"/>
+      <c r="AM12" s="30"/>
+      <c r="AN12" s="30"/>
+      <c r="AO12" s="30"/>
+      <c r="AP12" s="30"/>
+      <c r="AQ12" s="30"/>
+      <c r="AR12" s="30"/>
+      <c r="AS12" s="30"/>
+      <c r="AT12" s="30"/>
+      <c r="AU12" s="30"/>
+      <c r="AV12" s="30"/>
+      <c r="AW12" s="30"/>
+      <c r="AX12" s="30"/>
+      <c r="AY12" s="30"/>
+      <c r="AZ12" s="30"/>
+      <c r="BA12" s="30"/>
+      <c r="BB12" s="30"/>
+      <c r="BC12" s="30"/>
+      <c r="BD12" s="29">
+        <v>0</v>
+      </c>
+      <c r="BF12" s="65"/>
+      <c r="BG12" s="65"/>
+      <c r="BH12" s="65"/>
+      <c r="BI12" s="65"/>
+      <c r="BJ12" s="65">
+        <v>100</v>
+      </c>
+      <c r="BK12" s="65"/>
+      <c r="BL12" s="65"/>
+      <c r="BM12" s="65">
+        <v>100</v>
+      </c>
+      <c r="BN12" s="65"/>
+      <c r="BO12" s="65"/>
+      <c r="BP12" s="65">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="14">
+      <c r="B13" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="14">
         <v>1</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D13" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="V11" s="15">
-        <v>30</v>
-      </c>
-      <c r="AF11" s="15">
-        <v>40</v>
-      </c>
-      <c r="AP11" s="15">
+      <c r="E13" s="42"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="37"/>
+      <c r="S13" s="37"/>
+      <c r="T13" s="37"/>
+      <c r="U13" s="37"/>
+      <c r="V13" s="37"/>
+      <c r="W13" s="37"/>
+      <c r="X13" s="37"/>
+      <c r="Y13" s="37"/>
+      <c r="Z13" s="37"/>
+      <c r="AA13" s="37"/>
+      <c r="AB13" s="37"/>
+      <c r="AC13" s="37"/>
+      <c r="AD13" s="37"/>
+      <c r="AE13" s="37"/>
+      <c r="AF13" s="37"/>
+      <c r="AG13" s="37"/>
+      <c r="AH13" s="37"/>
+      <c r="AI13" s="37"/>
+      <c r="AJ13" s="37"/>
+      <c r="AK13" s="37"/>
+      <c r="AL13" s="37"/>
+      <c r="AM13" s="37"/>
+      <c r="AN13" s="37"/>
+      <c r="AO13" s="37"/>
+      <c r="AP13" s="37"/>
+      <c r="AQ13" s="37"/>
+      <c r="AR13" s="37"/>
+      <c r="AS13" s="37"/>
+      <c r="AT13" s="37"/>
+      <c r="AU13" s="37"/>
+      <c r="AV13" s="37"/>
+      <c r="AW13" s="37"/>
+      <c r="AX13" s="37"/>
+      <c r="AY13" s="37"/>
+      <c r="AZ13" s="37"/>
+      <c r="BA13" s="37"/>
+      <c r="BB13" s="37"/>
+      <c r="BC13" s="37"/>
+      <c r="BD13" s="37">
+        <v>0</v>
+      </c>
+      <c r="BE13" s="37"/>
+      <c r="BF13" s="66">
+        <v>100</v>
+      </c>
+      <c r="BG13" s="66"/>
+      <c r="BH13" s="66"/>
+      <c r="BI13" s="66"/>
+      <c r="BJ13" s="66"/>
+      <c r="BK13" s="66"/>
+      <c r="BL13" s="66"/>
+      <c r="BM13" s="66">
+        <v>100</v>
+      </c>
+      <c r="BN13" s="66"/>
+      <c r="BO13" s="66"/>
+      <c r="BP13" s="66">
+        <v>100</v>
+      </c>
+      <c r="BQ13" s="37"/>
+      <c r="BR13" s="37"/>
+      <c r="BS13" s="37"/>
+      <c r="BT13" s="37"/>
+      <c r="BU13" s="37"/>
+      <c r="BV13" s="37"/>
+      <c r="BW13" s="37"/>
+      <c r="BX13" s="37"/>
+    </row>
+    <row r="14" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="42"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="37"/>
+      <c r="S14" s="37"/>
+      <c r="T14" s="37"/>
+      <c r="U14" s="37"/>
+      <c r="V14" s="37"/>
+      <c r="W14" s="37"/>
+      <c r="X14" s="37"/>
+      <c r="Y14" s="37"/>
+      <c r="Z14" s="37"/>
+      <c r="AA14" s="37"/>
+      <c r="AB14" s="37"/>
+      <c r="AC14" s="37"/>
+      <c r="AD14" s="37"/>
+      <c r="AE14" s="37"/>
+      <c r="AF14" s="37"/>
+      <c r="AG14" s="37"/>
+      <c r="AH14" s="37"/>
+      <c r="AI14" s="37"/>
+      <c r="AJ14" s="37"/>
+      <c r="AK14" s="37"/>
+      <c r="AL14" s="37"/>
+      <c r="AM14" s="37"/>
+      <c r="AN14" s="37"/>
+      <c r="AO14" s="37"/>
+      <c r="AP14" s="37"/>
+      <c r="AQ14" s="37"/>
+      <c r="AR14" s="37"/>
+      <c r="AS14" s="37"/>
+      <c r="AT14" s="37"/>
+      <c r="AU14" s="37"/>
+      <c r="AV14" s="37"/>
+      <c r="AW14" s="37"/>
+      <c r="AX14" s="37"/>
+      <c r="AY14" s="37"/>
+      <c r="AZ14" s="37"/>
+      <c r="BA14" s="37"/>
+      <c r="BB14" s="37"/>
+      <c r="BC14" s="37"/>
+      <c r="BD14" s="37">
+        <v>0</v>
+      </c>
+      <c r="BE14" s="37"/>
+      <c r="BF14" s="66"/>
+      <c r="BG14" s="66"/>
+      <c r="BH14" s="66">
+        <v>17</v>
+      </c>
+      <c r="BI14" s="66">
+        <v>70</v>
+      </c>
+      <c r="BJ14" s="66"/>
+      <c r="BK14" s="66"/>
+      <c r="BL14" s="66"/>
+      <c r="BM14" s="66">
+        <v>70</v>
+      </c>
+      <c r="BN14" s="66"/>
+      <c r="BO14" s="66"/>
+      <c r="BP14" s="66">
+        <v>70</v>
+      </c>
+      <c r="BQ14" s="37"/>
+      <c r="BR14" s="37"/>
+      <c r="BS14" s="37"/>
+      <c r="BT14" s="37"/>
+      <c r="BU14" s="37"/>
+      <c r="BV14" s="37"/>
+      <c r="BW14" s="37"/>
+      <c r="BX14" s="37"/>
+    </row>
+    <row r="15" spans="1:76" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="46">
+        <v>1</v>
+      </c>
+      <c r="D15" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="47"/>
+      <c r="BD15" s="48">
+        <v>0</v>
+      </c>
+      <c r="BF15" s="61"/>
+      <c r="BG15" s="61"/>
+      <c r="BH15" s="61"/>
+      <c r="BI15" s="61"/>
+      <c r="BJ15" s="61"/>
+      <c r="BK15" s="61">
         <v>50</v>
       </c>
-      <c r="BF11" s="64"/>
-      <c r="BG11" s="64"/>
-      <c r="BH11" s="64"/>
-      <c r="BI11" s="64"/>
-      <c r="BJ11" s="64"/>
-      <c r="BK11" s="64"/>
-      <c r="BL11" s="64"/>
-      <c r="BM11" s="64"/>
-      <c r="BN11" s="64"/>
-      <c r="BO11" s="64"/>
-      <c r="BP11" s="64"/>
+      <c r="BL15" s="61"/>
+      <c r="BM15" s="61">
+        <v>50</v>
+      </c>
+      <c r="BN15" s="61"/>
+      <c r="BO15" s="61"/>
+      <c r="BP15" s="61">
+        <v>50</v>
+      </c>
     </row>
-    <row r="12" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="14">
+    <row r="16" spans="1:76" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="50">
         <v>1</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D16" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="42"/>
-      <c r="I12" s="15">
-        <v>7</v>
-      </c>
-      <c r="AK12" s="15">
-        <v>50</v>
-      </c>
-      <c r="AP12" s="15">
-        <v>70</v>
-      </c>
-      <c r="BF12" s="64"/>
-      <c r="BG12" s="64"/>
-      <c r="BH12" s="64"/>
-      <c r="BI12" s="64"/>
-      <c r="BJ12" s="64"/>
-      <c r="BK12" s="64"/>
-      <c r="BL12" s="64"/>
-      <c r="BM12" s="64"/>
-      <c r="BN12" s="64"/>
-      <c r="BO12" s="64"/>
-      <c r="BP12" s="64"/>
+      <c r="E16" s="51">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="F16" s="52">
+        <v>4.84</v>
+      </c>
+      <c r="G16" s="52">
+        <v>5.44</v>
+      </c>
+      <c r="H16" s="52">
+        <v>6.11</v>
+      </c>
+      <c r="I16" s="52">
+        <v>6.86</v>
+      </c>
+      <c r="J16" s="52">
+        <v>7.7</v>
+      </c>
+      <c r="K16" s="52">
+        <v>8.68</v>
+      </c>
+      <c r="L16" s="52">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="M16" s="52">
+        <v>9.41</v>
+      </c>
+      <c r="N16" s="52">
+        <v>11.48</v>
+      </c>
+      <c r="O16" s="52">
+        <v>12.75</v>
+      </c>
+      <c r="P16" s="52">
+        <v>14.6</v>
+      </c>
+      <c r="Q16" s="52">
+        <v>16.5</v>
+      </c>
+      <c r="R16" s="52">
+        <v>18.38</v>
+      </c>
+      <c r="S16" s="52">
+        <v>19.670000000000002</v>
+      </c>
+      <c r="T16" s="52">
+        <v>20.87</v>
+      </c>
+      <c r="U16" s="52">
+        <v>22.5</v>
+      </c>
+      <c r="V16" s="52">
+        <v>25.9</v>
+      </c>
+      <c r="W16" s="52">
+        <v>28.8</v>
+      </c>
+      <c r="X16" s="52">
+        <v>30.8</v>
+      </c>
+      <c r="Y16" s="52">
+        <v>32.9</v>
+      </c>
+      <c r="Z16" s="52">
+        <v>34.6</v>
+      </c>
+      <c r="AA16" s="52">
+        <v>36.1</v>
+      </c>
+      <c r="AB16" s="52">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="AC16" s="52">
+        <v>38.9</v>
+      </c>
+      <c r="AD16" s="52">
+        <v>43.4</v>
+      </c>
+      <c r="AE16" s="52">
+        <v>46.1</v>
+      </c>
+      <c r="AF16" s="52">
+        <v>49.9</v>
+      </c>
+      <c r="AG16" s="52">
+        <v>53.1</v>
+      </c>
+      <c r="AH16" s="52">
+        <v>55.7</v>
+      </c>
+      <c r="AI16" s="52">
+        <v>58.6</v>
+      </c>
+      <c r="AJ16" s="52">
+        <v>59.1</v>
+      </c>
+      <c r="AK16" s="52">
+        <v>60.4</v>
+      </c>
+      <c r="AL16" s="52">
+        <v>62.2</v>
+      </c>
+      <c r="AM16" s="52">
+        <v>64.3</v>
+      </c>
+      <c r="AN16" s="52">
+        <v>68</v>
+      </c>
+      <c r="AO16" s="52">
+        <v>69.3</v>
+      </c>
+      <c r="AP16" s="52">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="AQ16" s="52">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="AR16" s="52">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="AS16" s="52">
+        <v>76.7</v>
+      </c>
+      <c r="AT16" s="52">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="AU16" s="52">
+        <v>80.8</v>
+      </c>
+      <c r="AV16" s="52">
+        <v>82.8</v>
+      </c>
+      <c r="AW16" s="52">
+        <v>86.7</v>
+      </c>
+      <c r="AX16" s="52">
+        <v>93.4</v>
+      </c>
+      <c r="AY16" s="52">
+        <v>96.5</v>
+      </c>
+      <c r="AZ16" s="52">
+        <v>100</v>
+      </c>
+      <c r="BA16" s="52">
+        <v>107.3</v>
+      </c>
+      <c r="BB16" s="52">
+        <v>110.9</v>
+      </c>
+      <c r="BC16" s="52">
+        <v>114.2</v>
+      </c>
+      <c r="BD16" s="52">
+        <v>114.8</v>
+      </c>
+      <c r="BE16" s="52">
+        <v>116.4</v>
+      </c>
+      <c r="BF16" s="67"/>
+      <c r="BG16" s="67"/>
+      <c r="BH16" s="67"/>
+      <c r="BI16" s="67"/>
+      <c r="BJ16" s="67"/>
+      <c r="BK16" s="67"/>
+      <c r="BL16" s="67"/>
+      <c r="BM16" s="67"/>
+      <c r="BN16" s="67"/>
+      <c r="BO16" s="67"/>
+      <c r="BP16" s="67"/>
     </row>
-    <row r="13" spans="1:76" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="12">
-        <v>1</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="41"/>
-      <c r="I13" s="13">
-        <v>0</v>
-      </c>
-      <c r="V13" s="13">
-        <v>40</v>
-      </c>
-      <c r="AB13" s="13">
-        <v>65</v>
-      </c>
-      <c r="AK13" s="23"/>
-      <c r="AL13" s="23"/>
-      <c r="AM13" s="23"/>
-      <c r="AN13" s="23"/>
-      <c r="AO13" s="23"/>
-      <c r="AP13" s="23"/>
-      <c r="AQ13" s="23"/>
-      <c r="AR13" s="23"/>
-      <c r="AS13" s="23"/>
-      <c r="AT13" s="23"/>
-      <c r="AU13" s="23"/>
-      <c r="AV13" s="23"/>
-      <c r="AW13" s="23"/>
-      <c r="AX13" s="23"/>
-      <c r="AY13" s="23"/>
-      <c r="AZ13" s="23"/>
-      <c r="BA13" s="23"/>
-      <c r="BB13" s="23">
-        <v>93</v>
-      </c>
-      <c r="BC13" s="23">
-        <v>85</v>
-      </c>
-      <c r="BF13" s="63"/>
-      <c r="BG13" s="63">
-        <v>96</v>
-      </c>
-      <c r="BH13" s="63"/>
-      <c r="BI13" s="63"/>
-      <c r="BJ13" s="63"/>
-      <c r="BK13" s="63"/>
-      <c r="BL13" s="63"/>
-      <c r="BM13" s="63"/>
-      <c r="BN13" s="63"/>
-      <c r="BO13" s="63"/>
-      <c r="BP13" s="63"/>
-    </row>
-    <row r="14" spans="1:76" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="12">
-        <v>3</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="41"/>
-      <c r="I14" s="13">
-        <v>0</v>
-      </c>
-      <c r="V14" s="13">
-        <v>10</v>
-      </c>
-      <c r="AB14" s="13">
-        <v>8</v>
-      </c>
-      <c r="AK14" s="23"/>
-      <c r="AL14" s="23"/>
-      <c r="AM14" s="23"/>
-      <c r="AN14" s="23"/>
-      <c r="AO14" s="23"/>
-      <c r="AP14" s="23"/>
-      <c r="AQ14" s="23"/>
-      <c r="AR14" s="23"/>
-      <c r="AS14" s="23"/>
-      <c r="AT14" s="23"/>
-      <c r="AU14" s="23"/>
-      <c r="AV14" s="23"/>
-      <c r="AW14" s="23"/>
-      <c r="AX14" s="23"/>
-      <c r="AY14" s="23"/>
-      <c r="AZ14" s="23"/>
-      <c r="BA14" s="23"/>
-      <c r="BB14" s="23"/>
-      <c r="BC14" s="23"/>
-      <c r="BD14" s="13">
-        <v>5</v>
-      </c>
-      <c r="BF14" s="63"/>
-      <c r="BG14" s="63">
-        <v>1.3</v>
-      </c>
-      <c r="BH14" s="63"/>
-      <c r="BI14" s="63"/>
-      <c r="BJ14" s="63"/>
-      <c r="BK14" s="63"/>
-      <c r="BL14" s="63"/>
-      <c r="BM14" s="63"/>
-      <c r="BN14" s="63"/>
-      <c r="BO14" s="63"/>
-      <c r="BP14" s="63"/>
-    </row>
-    <row r="15" spans="1:76" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="28">
-        <v>1</v>
-      </c>
-      <c r="D15" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="43"/>
-      <c r="AK15" s="30"/>
-      <c r="AL15" s="30"/>
-      <c r="AM15" s="30"/>
-      <c r="AN15" s="30"/>
-      <c r="AO15" s="30"/>
-      <c r="AP15" s="30"/>
-      <c r="AQ15" s="30"/>
-      <c r="AR15" s="30"/>
-      <c r="AS15" s="30"/>
-      <c r="AT15" s="30"/>
-      <c r="AU15" s="30"/>
-      <c r="AV15" s="30"/>
-      <c r="AW15" s="30"/>
-      <c r="AX15" s="30"/>
-      <c r="AY15" s="30"/>
-      <c r="AZ15" s="30"/>
-      <c r="BA15" s="30"/>
-      <c r="BB15" s="30"/>
-      <c r="BC15" s="30"/>
-      <c r="BD15" s="29">
-        <v>0</v>
-      </c>
-      <c r="BF15" s="65"/>
-      <c r="BG15" s="65"/>
-      <c r="BH15" s="65"/>
-      <c r="BI15" s="65"/>
-      <c r="BJ15" s="65">
-        <v>100</v>
-      </c>
-      <c r="BK15" s="65"/>
-      <c r="BL15" s="65"/>
-      <c r="BM15" s="65">
-        <v>100</v>
-      </c>
-      <c r="BN15" s="65"/>
-      <c r="BO15" s="65"/>
-      <c r="BP15" s="65">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="14">
-        <v>1</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="42"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="37"/>
-      <c r="M16" s="37"/>
-      <c r="N16" s="37"/>
-      <c r="O16" s="37"/>
-      <c r="P16" s="37"/>
-      <c r="Q16" s="37"/>
-      <c r="R16" s="37"/>
-      <c r="S16" s="37"/>
-      <c r="T16" s="37"/>
-      <c r="U16" s="37"/>
-      <c r="V16" s="37"/>
-      <c r="W16" s="37"/>
-      <c r="X16" s="37"/>
-      <c r="Y16" s="37"/>
-      <c r="Z16" s="37"/>
-      <c r="AA16" s="37"/>
-      <c r="AB16" s="37"/>
-      <c r="AC16" s="37"/>
-      <c r="AD16" s="37"/>
-      <c r="AE16" s="37"/>
-      <c r="AF16" s="37"/>
-      <c r="AG16" s="37"/>
-      <c r="AH16" s="37"/>
-      <c r="AI16" s="37"/>
-      <c r="AJ16" s="37"/>
-      <c r="AK16" s="37"/>
-      <c r="AL16" s="37"/>
-      <c r="AM16" s="37"/>
-      <c r="AN16" s="37"/>
-      <c r="AO16" s="37"/>
-      <c r="AP16" s="37"/>
-      <c r="AQ16" s="37"/>
-      <c r="AR16" s="37"/>
-      <c r="AS16" s="37"/>
-      <c r="AT16" s="37"/>
-      <c r="AU16" s="37"/>
-      <c r="AV16" s="37"/>
-      <c r="AW16" s="37"/>
-      <c r="AX16" s="37"/>
-      <c r="AY16" s="37"/>
-      <c r="AZ16" s="37"/>
-      <c r="BA16" s="37"/>
-      <c r="BB16" s="37"/>
-      <c r="BC16" s="37"/>
-      <c r="BD16" s="37">
-        <v>0</v>
-      </c>
-      <c r="BE16" s="37"/>
-      <c r="BF16" s="66">
-        <v>100</v>
-      </c>
-      <c r="BG16" s="66"/>
-      <c r="BH16" s="66"/>
-      <c r="BI16" s="66"/>
-      <c r="BJ16" s="66"/>
-      <c r="BK16" s="66"/>
-      <c r="BL16" s="66"/>
-      <c r="BM16" s="66">
-        <v>100</v>
-      </c>
-      <c r="BN16" s="66"/>
-      <c r="BO16" s="66"/>
-      <c r="BP16" s="66">
-        <v>100</v>
-      </c>
-      <c r="BQ16" s="37"/>
-      <c r="BR16" s="37"/>
-      <c r="BS16" s="37"/>
-      <c r="BT16" s="37"/>
-      <c r="BU16" s="37"/>
-      <c r="BV16" s="37"/>
-      <c r="BW16" s="37"/>
-      <c r="BX16" s="37"/>
-    </row>
-    <row r="17" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>3</v>
@@ -3368,497 +3572,153 @@
       <c r="D17" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="42"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="37"/>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="37"/>
-      <c r="R17" s="37"/>
-      <c r="S17" s="37"/>
-      <c r="T17" s="37"/>
-      <c r="U17" s="37"/>
-      <c r="V17" s="37"/>
-      <c r="W17" s="37"/>
-      <c r="X17" s="37"/>
-      <c r="Y17" s="37"/>
-      <c r="Z17" s="37"/>
-      <c r="AA17" s="37"/>
-      <c r="AB17" s="37"/>
-      <c r="AC17" s="37"/>
-      <c r="AD17" s="37"/>
-      <c r="AE17" s="37"/>
-      <c r="AF17" s="37"/>
-      <c r="AG17" s="37"/>
-      <c r="AH17" s="37"/>
-      <c r="AI17" s="37"/>
-      <c r="AJ17" s="37"/>
-      <c r="AK17" s="37"/>
-      <c r="AL17" s="37"/>
-      <c r="AM17" s="37"/>
-      <c r="AN17" s="37"/>
-      <c r="AO17" s="37"/>
-      <c r="AP17" s="37"/>
-      <c r="AQ17" s="37"/>
-      <c r="AR17" s="37"/>
-      <c r="AS17" s="37"/>
-      <c r="AT17" s="37"/>
-      <c r="AU17" s="37"/>
-      <c r="AV17" s="37"/>
-      <c r="AW17" s="37"/>
-      <c r="AX17" s="37"/>
-      <c r="AY17" s="37"/>
-      <c r="AZ17" s="37"/>
-      <c r="BA17" s="37"/>
-      <c r="BB17" s="37"/>
-      <c r="BC17" s="37"/>
-      <c r="BD17" s="37">
+      <c r="E17" s="42">
+        <v>1</v>
+      </c>
+      <c r="K17" s="15">
+        <v>1</v>
+      </c>
+      <c r="U17" s="15">
+        <v>1</v>
+      </c>
+      <c r="V17" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="BA17" s="15">
+        <v>3.11</v>
+      </c>
+      <c r="BF17" s="64"/>
+      <c r="BG17" s="64"/>
+      <c r="BH17" s="64"/>
+      <c r="BI17" s="64"/>
+      <c r="BJ17" s="64"/>
+      <c r="BK17" s="64"/>
+      <c r="BL17" s="64"/>
+      <c r="BM17" s="64"/>
+      <c r="BN17" s="64"/>
+      <c r="BO17" s="64"/>
+      <c r="BP17" s="64"/>
+    </row>
+    <row r="18" spans="1:68" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="57"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="43"/>
+      <c r="BF18" s="65"/>
+      <c r="BG18" s="65"/>
+      <c r="BH18" s="65"/>
+      <c r="BI18" s="65"/>
+      <c r="BJ18" s="65"/>
+      <c r="BK18" s="65"/>
+      <c r="BL18" s="65"/>
+      <c r="BM18" s="65"/>
+      <c r="BN18" s="65"/>
+      <c r="BO18" s="65"/>
+      <c r="BP18" s="65"/>
+    </row>
+    <row r="19" spans="1:68" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="28">
+        <v>1</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="43"/>
+      <c r="BD19" s="29">
+        <v>1</v>
+      </c>
+      <c r="BF19" s="65"/>
+      <c r="BG19" s="65"/>
+      <c r="BH19" s="65"/>
+      <c r="BI19" s="65"/>
+      <c r="BJ19" s="65"/>
+      <c r="BK19" s="65"/>
+      <c r="BL19" s="65"/>
+      <c r="BM19" s="65"/>
+      <c r="BN19" s="65"/>
+      <c r="BO19" s="65"/>
+      <c r="BP19" s="65"/>
+    </row>
+    <row r="20" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A20" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="44">
         <v>0</v>
       </c>
-      <c r="BE17" s="37"/>
-      <c r="BF17" s="66"/>
-      <c r="BG17" s="66"/>
-      <c r="BH17" s="66">
-        <v>17</v>
-      </c>
-      <c r="BI17" s="66">
-        <v>70</v>
-      </c>
-      <c r="BJ17" s="66"/>
-      <c r="BK17" s="66"/>
-      <c r="BL17" s="66"/>
-      <c r="BM17" s="66">
-        <v>70</v>
-      </c>
-      <c r="BN17" s="66"/>
-      <c r="BO17" s="66"/>
-      <c r="BP17" s="66">
-        <v>70</v>
-      </c>
-      <c r="BQ17" s="37"/>
-      <c r="BR17" s="37"/>
-      <c r="BS17" s="37"/>
-      <c r="BT17" s="37"/>
-      <c r="BU17" s="37"/>
-      <c r="BV17" s="37"/>
-      <c r="BW17" s="37"/>
-      <c r="BX17" s="37"/>
-    </row>
-    <row r="18" spans="1:76" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="46">
-        <v>1</v>
-      </c>
-      <c r="D18" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="47"/>
-      <c r="BD18" s="48">
+      <c r="T20" s="1">
         <v>0</v>
       </c>
-      <c r="BF18" s="61"/>
-      <c r="BG18" s="61"/>
-      <c r="BH18" s="61"/>
-      <c r="BI18" s="61"/>
-      <c r="BJ18" s="61"/>
-      <c r="BK18" s="61"/>
-      <c r="BL18" s="61"/>
-      <c r="BM18" s="61"/>
-      <c r="BN18" s="61"/>
-      <c r="BO18" s="61"/>
-      <c r="BP18" s="61"/>
-    </row>
-    <row r="19" spans="1:76" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="46">
-        <v>1</v>
-      </c>
-      <c r="D19" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="47"/>
-      <c r="BD19" s="48">
-        <v>0</v>
-      </c>
-      <c r="BF19" s="61"/>
-      <c r="BG19" s="61"/>
-      <c r="BH19" s="61"/>
-      <c r="BI19" s="61"/>
-      <c r="BJ19" s="61"/>
-      <c r="BK19" s="61">
-        <v>50</v>
-      </c>
-      <c r="BL19" s="61"/>
-      <c r="BM19" s="61">
-        <v>50</v>
-      </c>
-      <c r="BN19" s="61"/>
-      <c r="BO19" s="61"/>
-      <c r="BP19" s="61">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:76" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="50">
-        <v>1</v>
-      </c>
-      <c r="D20" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="51">
-        <v>4.3099999999999996</v>
-      </c>
-      <c r="F20" s="52">
-        <v>4.84</v>
-      </c>
-      <c r="G20" s="52">
-        <v>5.44</v>
-      </c>
-      <c r="H20" s="52">
-        <v>6.11</v>
-      </c>
-      <c r="I20" s="52">
-        <v>6.86</v>
-      </c>
-      <c r="J20" s="52">
+      <c r="V20" s="1">
         <v>7.7</v>
       </c>
-      <c r="K20" s="52">
-        <v>8.68</v>
-      </c>
-      <c r="L20" s="52">
-        <v>9.0399999999999991</v>
-      </c>
-      <c r="M20" s="52">
-        <v>9.41</v>
-      </c>
-      <c r="N20" s="52">
-        <v>11.48</v>
-      </c>
-      <c r="O20" s="52">
-        <v>12.75</v>
-      </c>
-      <c r="P20" s="52">
-        <v>14.6</v>
-      </c>
-      <c r="Q20" s="52">
+      <c r="AI20" s="1">
+        <v>11.1</v>
+      </c>
+      <c r="AR20" s="1">
         <v>16.5</v>
       </c>
-      <c r="R20" s="52">
-        <v>18.38</v>
-      </c>
-      <c r="S20" s="52">
-        <v>19.670000000000002</v>
-      </c>
-      <c r="T20" s="52">
-        <v>20.87</v>
-      </c>
-      <c r="U20" s="52">
-        <v>22.5</v>
-      </c>
-      <c r="V20" s="52">
-        <v>25.9</v>
-      </c>
-      <c r="W20" s="52">
-        <v>28.8</v>
-      </c>
-      <c r="X20" s="52">
-        <v>30.8</v>
-      </c>
-      <c r="Y20" s="52">
-        <v>32.9</v>
-      </c>
-      <c r="Z20" s="52">
-        <v>34.6</v>
-      </c>
-      <c r="AA20" s="52">
-        <v>36.1</v>
-      </c>
-      <c r="AB20" s="52">
-        <v>36.799999999999997</v>
-      </c>
-      <c r="AC20" s="52">
-        <v>38.9</v>
-      </c>
-      <c r="AD20" s="52">
-        <v>43.4</v>
-      </c>
-      <c r="AE20" s="52">
-        <v>46.1</v>
-      </c>
-      <c r="AF20" s="52">
-        <v>49.9</v>
-      </c>
-      <c r="AG20" s="52">
-        <v>53.1</v>
-      </c>
-      <c r="AH20" s="52">
-        <v>55.7</v>
-      </c>
-      <c r="AI20" s="52">
-        <v>58.6</v>
-      </c>
-      <c r="AJ20" s="52">
-        <v>59.1</v>
-      </c>
-      <c r="AK20" s="52">
-        <v>60.4</v>
-      </c>
-      <c r="AL20" s="52">
-        <v>62.2</v>
-      </c>
-      <c r="AM20" s="52">
-        <v>64.3</v>
-      </c>
-      <c r="AN20" s="52">
-        <v>68</v>
-      </c>
-      <c r="AO20" s="52">
-        <v>69.3</v>
-      </c>
-      <c r="AP20" s="52">
-        <v>70.099999999999994</v>
-      </c>
-      <c r="AQ20" s="52">
-        <v>73.099999999999994</v>
-      </c>
-      <c r="AR20" s="52">
-        <v>73.599999999999994</v>
-      </c>
-      <c r="AS20" s="52">
-        <v>76.7</v>
-      </c>
-      <c r="AT20" s="52">
-        <v>78.900000000000006</v>
-      </c>
-      <c r="AU20" s="52">
-        <v>80.8</v>
-      </c>
-      <c r="AV20" s="52">
-        <v>82.8</v>
-      </c>
-      <c r="AW20" s="52">
-        <v>86.7</v>
-      </c>
-      <c r="AX20" s="52">
-        <v>93.4</v>
-      </c>
-      <c r="AY20" s="52">
-        <v>96.5</v>
-      </c>
-      <c r="AZ20" s="52">
-        <v>100</v>
-      </c>
-      <c r="BA20" s="52">
-        <v>107.3</v>
-      </c>
-      <c r="BB20" s="52">
-        <v>110.9</v>
-      </c>
-      <c r="BC20" s="52">
-        <v>114.2</v>
-      </c>
-      <c r="BD20" s="52">
-        <v>114.8</v>
-      </c>
-      <c r="BE20" s="52">
-        <v>116.4</v>
-      </c>
-      <c r="BF20" s="67"/>
-      <c r="BG20" s="67"/>
-      <c r="BH20" s="67"/>
-      <c r="BI20" s="67"/>
-      <c r="BJ20" s="67"/>
-      <c r="BK20" s="67"/>
-      <c r="BL20" s="67"/>
-      <c r="BM20" s="67"/>
-      <c r="BN20" s="67"/>
-      <c r="BO20" s="67"/>
-      <c r="BP20" s="67"/>
-    </row>
-    <row r="21" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="14">
-        <v>1</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="42">
-        <v>1</v>
-      </c>
-      <c r="K21" s="15">
-        <v>1</v>
-      </c>
-      <c r="U21" s="15">
-        <v>1</v>
-      </c>
-      <c r="V21" s="15">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="BA21" s="15">
-        <v>3.11</v>
-      </c>
-      <c r="BF21" s="64"/>
-      <c r="BG21" s="64"/>
-      <c r="BH21" s="64"/>
-      <c r="BI21" s="64"/>
-      <c r="BJ21" s="64"/>
-      <c r="BK21" s="64"/>
-      <c r="BL21" s="64"/>
-      <c r="BM21" s="64"/>
-      <c r="BN21" s="64"/>
-      <c r="BO21" s="64"/>
-      <c r="BP21" s="64"/>
-    </row>
-    <row r="22" spans="1:76" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="57"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="43"/>
-      <c r="BF22" s="65"/>
-      <c r="BG22" s="65"/>
-      <c r="BH22" s="65"/>
-      <c r="BI22" s="65"/>
-      <c r="BJ22" s="65"/>
-      <c r="BK22" s="65"/>
-      <c r="BL22" s="65"/>
-      <c r="BM22" s="65"/>
-      <c r="BN22" s="65"/>
-      <c r="BO22" s="65"/>
-      <c r="BP22" s="65"/>
-    </row>
-    <row r="23" spans="1:76" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="57" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="28">
-        <v>1</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="43"/>
-      <c r="BD23" s="29">
-        <v>1</v>
-      </c>
-      <c r="BF23" s="65"/>
-      <c r="BG23" s="65"/>
-      <c r="BH23" s="65"/>
-      <c r="BI23" s="65"/>
-      <c r="BJ23" s="65"/>
-      <c r="BK23" s="65"/>
-      <c r="BL23" s="65"/>
-      <c r="BM23" s="65"/>
-      <c r="BN23" s="65"/>
-      <c r="BO23" s="65"/>
-      <c r="BP23" s="65"/>
-    </row>
-    <row r="24" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="2">
-        <v>1</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="44">
-        <v>0</v>
-      </c>
-      <c r="T24" s="1">
-        <v>0</v>
-      </c>
-      <c r="V24" s="1">
-        <v>7.7</v>
-      </c>
-      <c r="AI24" s="1">
-        <v>11.1</v>
-      </c>
-      <c r="AR24" s="1">
-        <v>16.5</v>
-      </c>
-      <c r="AT24" s="1">
+      <c r="AT20" s="1">
         <v>14.5</v>
       </c>
-      <c r="AY24" s="1">
+      <c r="AY20" s="1">
         <v>16.100000000000001</v>
       </c>
-      <c r="BA24" s="1">
+      <c r="BA20" s="1">
         <v>15.6</v>
       </c>
-      <c r="BC24" s="1">
+      <c r="BC20" s="1">
         <v>15.6</v>
       </c>
-      <c r="BE24" s="1">
+      <c r="BE20" s="1">
         <v>15.6</v>
       </c>
-      <c r="BF24" s="68"/>
-      <c r="BG24" s="68"/>
-      <c r="BH24" s="68"/>
-      <c r="BI24" s="68"/>
-      <c r="BJ24" s="68"/>
-      <c r="BK24" s="68"/>
-      <c r="BL24" s="68"/>
-      <c r="BM24" s="68"/>
-      <c r="BN24" s="68"/>
-      <c r="BO24" s="68"/>
-      <c r="BP24" s="68"/>
+      <c r="BF20" s="68"/>
+      <c r="BG20" s="68"/>
+      <c r="BH20" s="68"/>
+      <c r="BI20" s="68"/>
+      <c r="BJ20" s="68"/>
+      <c r="BK20" s="68"/>
+      <c r="BL20" s="68"/>
+      <c r="BM20" s="68"/>
+      <c r="BN20" s="68"/>
+      <c r="BO20" s="68"/>
+      <c r="BP20" s="68"/>
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="5">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF15:BG15 F4:BG7">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF12:BG12 F4:BG6">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1:D1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:BG14 F15:BE15 F2:BG3">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F12:BE12 F2:BG3 F8:BG11">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C24:C1048576 C2:C21">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C20:C1048576 C2:C17">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Leave blank" sqref="B22:D23"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Leave blank" sqref="B18:D19"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3869,13 +3729,13 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B9:B15 B2:B7</xm:sqref>
+          <xm:sqref>B2:B6 B8:B12</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time-variant?" prompt="If no, the most recent value will be selected.">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D24:D1048576 D2:D21</xm:sqref>
+          <xm:sqref>D20:D1048576 D2:D17</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Simplify awareness raising code
Only slightly - removes one line
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="495" windowWidth="20370" windowHeight="7350" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="495" windowWidth="20370" windowHeight="7350" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
   <si>
     <t>parameter</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>int_perc_xpertacf</t>
+  </si>
+  <si>
+    <t>int_perc_awareness_raising</t>
+  </si>
+  <si>
+    <t>scenario_13</t>
   </si>
 </sst>
 </file>
@@ -2198,7 +2204,7 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2342,13 +2348,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BW20"/>
+  <dimension ref="A1:BX21"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="BH2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="BQ2" sqref="BQ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2375,12 +2381,14 @@
     <col min="53" max="54" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="55" max="56" width="7.85546875" style="1" customWidth="1"/>
     <col min="57" max="57" width="14" style="1" customWidth="1"/>
-    <col min="58" max="64" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="65" max="67" width="14.42578125" style="1" customWidth="1"/>
-    <col min="68" max="16384" width="9.140625" style="1"/>
+    <col min="58" max="62" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="14.42578125" style="1" customWidth="1"/>
+    <col min="64" max="65" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="66" max="68" width="14.42578125" style="1" customWidth="1"/>
+    <col min="69" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:76" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
@@ -2585,8 +2593,11 @@
       <c r="BP1" s="5" t="s">
         <v>40</v>
       </c>
+      <c r="BQ1" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="2" spans="1:75" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:76" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>43</v>
       </c>
@@ -2642,12 +2653,13 @@
       <c r="BK2" s="59"/>
       <c r="BL2" s="59"/>
       <c r="BM2" s="59"/>
-      <c r="BN2" s="59">
+      <c r="BN2" s="59"/>
+      <c r="BO2" s="59">
         <v>90</v>
       </c>
-      <c r="BO2" s="59"/>
+      <c r="BP2" s="59"/>
     </row>
-    <row r="3" spans="1:75" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:76" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -2745,8 +2757,9 @@
       <c r="BM3" s="60"/>
       <c r="BN3" s="60"/>
       <c r="BO3" s="60"/>
+      <c r="BP3" s="60"/>
     </row>
-    <row r="4" spans="1:75" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:76" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>44</v>
       </c>
@@ -2770,19 +2783,20 @@
       <c r="BH4" s="60"/>
       <c r="BI4" s="60"/>
       <c r="BJ4" s="60"/>
-      <c r="BK4" s="60">
-        <v>80</v>
-      </c>
+      <c r="BK4" s="60"/>
       <c r="BL4" s="60">
         <v>80</v>
       </c>
-      <c r="BM4" s="60"/>
+      <c r="BM4" s="60">
+        <v>80</v>
+      </c>
       <c r="BN4" s="60"/>
-      <c r="BO4" s="60">
+      <c r="BO4" s="60"/>
+      <c r="BP4" s="60">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:75" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:76" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>45</v>
       </c>
@@ -2800,19 +2814,20 @@
       <c r="BH5" s="60"/>
       <c r="BI5" s="60"/>
       <c r="BJ5" s="60"/>
-      <c r="BK5" s="60">
-        <v>80</v>
-      </c>
+      <c r="BK5" s="60"/>
       <c r="BL5" s="60">
         <v>80</v>
       </c>
-      <c r="BM5" s="60"/>
+      <c r="BM5" s="60">
+        <v>80</v>
+      </c>
       <c r="BN5" s="60"/>
-      <c r="BO5" s="60">
+      <c r="BO5" s="60"/>
+      <c r="BP5" s="60">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:75" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:76" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>46</v>
       </c>
@@ -2834,14 +2849,15 @@
       <c r="BL6" s="60"/>
       <c r="BM6" s="60"/>
       <c r="BN6" s="60"/>
-      <c r="BO6" s="9">
+      <c r="BO6" s="60"/>
+      <c r="BP6" s="9">
         <v>10</v>
       </c>
-      <c r="BP6" s="9">
+      <c r="BQ6" s="9">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:75" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:76" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="45" t="s">
         <v>47</v>
       </c>
@@ -2861,13 +2877,14 @@
       <c r="BJ7" s="61"/>
       <c r="BK7" s="61"/>
       <c r="BL7" s="61"/>
-      <c r="BM7" s="61">
+      <c r="BM7" s="61"/>
+      <c r="BN7" s="61">
         <v>10</v>
       </c>
-      <c r="BN7" s="61"/>
       <c r="BO7" s="61"/>
+      <c r="BP7" s="61"/>
     </row>
-    <row r="8" spans="1:75" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:76" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>32</v>
       </c>
@@ -2902,8 +2919,9 @@
       <c r="BM8" s="62"/>
       <c r="BN8" s="62"/>
       <c r="BO8" s="62"/>
+      <c r="BP8" s="62"/>
     </row>
-    <row r="9" spans="1:75" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>33</v>
       </c>
@@ -2932,8 +2950,9 @@
       <c r="BM9" s="64"/>
       <c r="BN9" s="64"/>
       <c r="BO9" s="64"/>
+      <c r="BP9" s="64"/>
     </row>
-    <row r="10" spans="1:75" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:76" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>34</v>
       </c>
@@ -2987,8 +3006,9 @@
       <c r="BM10" s="63"/>
       <c r="BN10" s="63"/>
       <c r="BO10" s="63"/>
+      <c r="BP10" s="63"/>
     </row>
-    <row r="11" spans="1:75" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:76" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>35</v>
       </c>
@@ -3043,8 +3063,9 @@
       <c r="BM11" s="63"/>
       <c r="BN11" s="63"/>
       <c r="BO11" s="63"/>
+      <c r="BP11" s="63"/>
     </row>
-    <row r="12" spans="1:75" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:76" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="27" t="s">
         <v>48</v>
       </c>
@@ -3084,16 +3105,17 @@
       </c>
       <c r="BJ12" s="65"/>
       <c r="BK12" s="65"/>
-      <c r="BL12" s="65">
+      <c r="BL12" s="65"/>
+      <c r="BM12" s="65">
         <v>100</v>
       </c>
-      <c r="BM12" s="65"/>
       <c r="BN12" s="65"/>
-      <c r="BO12" s="65">
+      <c r="BO12" s="65"/>
+      <c r="BP12" s="65">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:75" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>42</v>
       </c>
@@ -3165,15 +3187,15 @@
       <c r="BI13" s="66"/>
       <c r="BJ13" s="66"/>
       <c r="BK13" s="66"/>
-      <c r="BL13" s="66">
+      <c r="BL13" s="66"/>
+      <c r="BM13" s="66">
         <v>100</v>
       </c>
-      <c r="BM13" s="66"/>
       <c r="BN13" s="66"/>
-      <c r="BO13" s="66">
+      <c r="BO13" s="66"/>
+      <c r="BP13" s="66">
         <v>100</v>
       </c>
-      <c r="BP13" s="37"/>
       <c r="BQ13" s="37"/>
       <c r="BR13" s="37"/>
       <c r="BS13" s="37"/>
@@ -3181,8 +3203,9 @@
       <c r="BU13" s="37"/>
       <c r="BV13" s="37"/>
       <c r="BW13" s="37"/>
+      <c r="BX13" s="37"/>
     </row>
-    <row r="14" spans="1:75" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:76" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>49</v>
       </c>
@@ -3256,15 +3279,15 @@
       <c r="BI14" s="66"/>
       <c r="BJ14" s="66"/>
       <c r="BK14" s="66"/>
-      <c r="BL14" s="66">
+      <c r="BL14" s="66"/>
+      <c r="BM14" s="66">
         <v>70</v>
       </c>
-      <c r="BM14" s="66"/>
       <c r="BN14" s="66"/>
-      <c r="BO14" s="66">
+      <c r="BO14" s="66"/>
+      <c r="BP14" s="66">
         <v>70</v>
       </c>
-      <c r="BP14" s="37"/>
       <c r="BQ14" s="37"/>
       <c r="BR14" s="37"/>
       <c r="BS14" s="37"/>
@@ -3272,8 +3295,9 @@
       <c r="BU14" s="37"/>
       <c r="BV14" s="37"/>
       <c r="BW14" s="37"/>
+      <c r="BX14" s="37"/>
     </row>
-    <row r="15" spans="1:75" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:76" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="45" t="s">
         <v>50</v>
       </c>
@@ -3294,260 +3318,266 @@
         <v>50</v>
       </c>
       <c r="BK15" s="61"/>
-      <c r="BL15" s="61">
+      <c r="BL15" s="61"/>
+      <c r="BM15" s="61">
         <v>50</v>
       </c>
-      <c r="BM15" s="61"/>
       <c r="BN15" s="61"/>
-      <c r="BO15" s="61">
+      <c r="BO15" s="61"/>
+      <c r="BP15" s="61">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:75" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="49" t="s">
+    <row r="16" spans="1:76" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="46"/>
+      <c r="D16" s="47"/>
+      <c r="BC16" s="48">
+        <v>0</v>
+      </c>
+      <c r="BE16" s="61"/>
+      <c r="BF16" s="61"/>
+      <c r="BG16" s="61"/>
+      <c r="BH16" s="61"/>
+      <c r="BI16" s="61"/>
+      <c r="BJ16" s="61"/>
+      <c r="BK16" s="61">
+        <v>50</v>
+      </c>
+      <c r="BL16" s="61"/>
+      <c r="BM16" s="61"/>
+      <c r="BN16" s="61"/>
+      <c r="BO16" s="61"/>
+      <c r="BP16" s="61"/>
+    </row>
+    <row r="17" spans="1:68" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="50" t="s">
+      <c r="B17" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="50"/>
-      <c r="D16" s="51">
+      <c r="C17" s="50"/>
+      <c r="D17" s="51">
         <v>4.3099999999999996</v>
       </c>
-      <c r="E16" s="52">
+      <c r="E17" s="52">
         <v>4.84</v>
       </c>
-      <c r="F16" s="52">
+      <c r="F17" s="52">
         <v>5.44</v>
       </c>
-      <c r="G16" s="52">
+      <c r="G17" s="52">
         <v>6.11</v>
       </c>
-      <c r="H16" s="52">
+      <c r="H17" s="52">
         <v>6.86</v>
       </c>
-      <c r="I16" s="52">
+      <c r="I17" s="52">
         <v>7.7</v>
       </c>
-      <c r="J16" s="52">
+      <c r="J17" s="52">
         <v>8.68</v>
       </c>
-      <c r="K16" s="52">
+      <c r="K17" s="52">
         <v>9.0399999999999991</v>
       </c>
-      <c r="L16" s="52">
+      <c r="L17" s="52">
         <v>9.41</v>
       </c>
-      <c r="M16" s="52">
+      <c r="M17" s="52">
         <v>11.48</v>
       </c>
-      <c r="N16" s="52">
+      <c r="N17" s="52">
         <v>12.75</v>
       </c>
-      <c r="O16" s="52">
+      <c r="O17" s="52">
         <v>14.6</v>
       </c>
-      <c r="P16" s="52">
+      <c r="P17" s="52">
         <v>16.5</v>
       </c>
-      <c r="Q16" s="52">
+      <c r="Q17" s="52">
         <v>18.38</v>
       </c>
-      <c r="R16" s="52">
+      <c r="R17" s="52">
         <v>19.670000000000002</v>
       </c>
-      <c r="S16" s="52">
+      <c r="S17" s="52">
         <v>20.87</v>
       </c>
-      <c r="T16" s="52">
+      <c r="T17" s="52">
         <v>22.5</v>
       </c>
-      <c r="U16" s="52">
+      <c r="U17" s="52">
         <v>25.9</v>
       </c>
-      <c r="V16" s="52">
+      <c r="V17" s="52">
         <v>28.8</v>
       </c>
-      <c r="W16" s="52">
+      <c r="W17" s="52">
         <v>30.8</v>
       </c>
-      <c r="X16" s="52">
+      <c r="X17" s="52">
         <v>32.9</v>
       </c>
-      <c r="Y16" s="52">
+      <c r="Y17" s="52">
         <v>34.6</v>
       </c>
-      <c r="Z16" s="52">
+      <c r="Z17" s="52">
         <v>36.1</v>
       </c>
-      <c r="AA16" s="52">
+      <c r="AA17" s="52">
         <v>36.799999999999997</v>
       </c>
-      <c r="AB16" s="52">
+      <c r="AB17" s="52">
         <v>38.9</v>
       </c>
-      <c r="AC16" s="52">
+      <c r="AC17" s="52">
         <v>43.4</v>
       </c>
-      <c r="AD16" s="52">
+      <c r="AD17" s="52">
         <v>46.1</v>
       </c>
-      <c r="AE16" s="52">
+      <c r="AE17" s="52">
         <v>49.9</v>
       </c>
-      <c r="AF16" s="52">
+      <c r="AF17" s="52">
         <v>53.1</v>
       </c>
-      <c r="AG16" s="52">
+      <c r="AG17" s="52">
         <v>55.7</v>
       </c>
-      <c r="AH16" s="52">
+      <c r="AH17" s="52">
         <v>58.6</v>
       </c>
-      <c r="AI16" s="52">
+      <c r="AI17" s="52">
         <v>59.1</v>
       </c>
-      <c r="AJ16" s="52">
+      <c r="AJ17" s="52">
         <v>60.4</v>
       </c>
-      <c r="AK16" s="52">
+      <c r="AK17" s="52">
         <v>62.2</v>
       </c>
-      <c r="AL16" s="52">
+      <c r="AL17" s="52">
         <v>64.3</v>
       </c>
-      <c r="AM16" s="52">
+      <c r="AM17" s="52">
         <v>68</v>
       </c>
-      <c r="AN16" s="52">
+      <c r="AN17" s="52">
         <v>69.3</v>
       </c>
-      <c r="AO16" s="52">
+      <c r="AO17" s="52">
         <v>70.099999999999994</v>
       </c>
-      <c r="AP16" s="52">
+      <c r="AP17" s="52">
         <v>73.099999999999994</v>
       </c>
-      <c r="AQ16" s="52">
+      <c r="AQ17" s="52">
         <v>73.599999999999994</v>
       </c>
-      <c r="AR16" s="52">
+      <c r="AR17" s="52">
         <v>76.7</v>
       </c>
-      <c r="AS16" s="52">
+      <c r="AS17" s="52">
         <v>78.900000000000006</v>
       </c>
-      <c r="AT16" s="52">
+      <c r="AT17" s="52">
         <v>80.8</v>
       </c>
-      <c r="AU16" s="52">
+      <c r="AU17" s="52">
         <v>82.8</v>
       </c>
-      <c r="AV16" s="52">
+      <c r="AV17" s="52">
         <v>86.7</v>
       </c>
-      <c r="AW16" s="52">
+      <c r="AW17" s="52">
         <v>93.4</v>
       </c>
-      <c r="AX16" s="52">
+      <c r="AX17" s="52">
         <v>96.5</v>
       </c>
-      <c r="AY16" s="52">
+      <c r="AY17" s="52">
         <v>100</v>
       </c>
-      <c r="AZ16" s="52">
+      <c r="AZ17" s="52">
         <v>107.3</v>
       </c>
-      <c r="BA16" s="52">
+      <c r="BA17" s="52">
         <v>110.9</v>
       </c>
-      <c r="BB16" s="52">
+      <c r="BB17" s="52">
         <v>114.2</v>
       </c>
-      <c r="BC16" s="52">
+      <c r="BC17" s="52">
         <v>114.8</v>
       </c>
-      <c r="BD16" s="52">
+      <c r="BD17" s="52">
         <v>116.4</v>
       </c>
-      <c r="BE16" s="67"/>
-      <c r="BF16" s="67"/>
-      <c r="BG16" s="67"/>
-      <c r="BH16" s="67"/>
-      <c r="BI16" s="67"/>
-      <c r="BJ16" s="67"/>
-      <c r="BK16" s="67"/>
-      <c r="BL16" s="67"/>
-      <c r="BM16" s="67"/>
-      <c r="BN16" s="67"/>
-      <c r="BO16" s="67"/>
+      <c r="BE17" s="67"/>
+      <c r="BF17" s="67"/>
+      <c r="BG17" s="67"/>
+      <c r="BH17" s="67"/>
+      <c r="BI17" s="67"/>
+      <c r="BJ17" s="67"/>
+      <c r="BK17" s="67"/>
+      <c r="BL17" s="67"/>
+      <c r="BM17" s="67"/>
+      <c r="BN17" s="67"/>
+      <c r="BO17" s="67"/>
+      <c r="BP17" s="67"/>
     </row>
-    <row r="17" spans="1:67" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+    <row r="18" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B18" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="42">
+      <c r="C18" s="14"/>
+      <c r="D18" s="42">
         <v>1</v>
       </c>
-      <c r="J17" s="15">
+      <c r="J18" s="15">
         <v>1</v>
       </c>
-      <c r="T17" s="15">
+      <c r="T18" s="15">
         <v>1</v>
       </c>
-      <c r="U17" s="15">
+      <c r="U18" s="15">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AZ17" s="15">
+      <c r="AZ18" s="15">
         <v>3.11</v>
       </c>
-      <c r="BE17" s="64"/>
-      <c r="BF17" s="64"/>
-      <c r="BG17" s="64"/>
-      <c r="BH17" s="64"/>
-      <c r="BI17" s="64"/>
-      <c r="BJ17" s="64"/>
-      <c r="BK17" s="64"/>
-      <c r="BL17" s="64"/>
-      <c r="BM17" s="64"/>
-      <c r="BN17" s="64"/>
-      <c r="BO17" s="64"/>
+      <c r="BE18" s="64"/>
+      <c r="BF18" s="64"/>
+      <c r="BG18" s="64"/>
+      <c r="BH18" s="64"/>
+      <c r="BI18" s="64"/>
+      <c r="BJ18" s="64"/>
+      <c r="BK18" s="64"/>
+      <c r="BL18" s="64"/>
+      <c r="BM18" s="64"/>
+      <c r="BN18" s="64"/>
+      <c r="BO18" s="64"/>
+      <c r="BP18" s="64"/>
     </row>
-    <row r="18" spans="1:67" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
+    <row r="19" spans="1:68" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="43"/>
-      <c r="BE18" s="65"/>
-      <c r="BF18" s="65"/>
-      <c r="BG18" s="65"/>
-      <c r="BH18" s="65"/>
-      <c r="BI18" s="65"/>
-      <c r="BJ18" s="65"/>
-      <c r="BK18" s="65"/>
-      <c r="BL18" s="65"/>
-      <c r="BM18" s="65"/>
-      <c r="BN18" s="65"/>
-      <c r="BO18" s="65"/>
-    </row>
-    <row r="19" spans="1:67" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="57" t="s">
-        <v>4</v>
-      </c>
+      <c r="B19" s="57"/>
       <c r="C19" s="28"/>
       <c r="D19" s="43"/>
-      <c r="BC19" s="29">
-        <v>1</v>
-      </c>
       <c r="BE19" s="65"/>
       <c r="BF19" s="65"/>
       <c r="BG19" s="65"/>
@@ -3559,58 +3589,85 @@
       <c r="BM19" s="65"/>
       <c r="BN19" s="65"/>
       <c r="BO19" s="65"/>
+      <c r="BP19" s="65"/>
     </row>
-    <row r="20" spans="1:67" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
+    <row r="20" spans="1:68" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="28"/>
+      <c r="D20" s="43"/>
+      <c r="BC20" s="29">
+        <v>1</v>
+      </c>
+      <c r="BE20" s="65"/>
+      <c r="BF20" s="65"/>
+      <c r="BG20" s="65"/>
+      <c r="BH20" s="65"/>
+      <c r="BI20" s="65"/>
+      <c r="BJ20" s="65"/>
+      <c r="BK20" s="65"/>
+      <c r="BL20" s="65"/>
+      <c r="BM20" s="65"/>
+      <c r="BN20" s="65"/>
+      <c r="BO20" s="65"/>
+      <c r="BP20" s="65"/>
+    </row>
+    <row r="21" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="44">
+      <c r="D21" s="44">
         <v>0</v>
       </c>
-      <c r="S20" s="1">
+      <c r="S21" s="1">
         <v>0</v>
       </c>
-      <c r="U20" s="1">
+      <c r="U21" s="1">
         <v>7.7</v>
       </c>
-      <c r="AH20" s="1">
+      <c r="AH21" s="1">
         <v>11.1</v>
       </c>
-      <c r="AQ20" s="1">
+      <c r="AQ21" s="1">
         <v>16.5</v>
       </c>
-      <c r="AS20" s="1">
+      <c r="AS21" s="1">
         <v>14.5</v>
       </c>
-      <c r="AX20" s="1">
+      <c r="AX21" s="1">
         <v>16.100000000000001</v>
       </c>
-      <c r="AZ20" s="1">
+      <c r="AZ21" s="1">
         <v>15.6</v>
       </c>
-      <c r="BB20" s="1">
+      <c r="BB21" s="1">
         <v>15.6</v>
       </c>
-      <c r="BD20" s="1">
+      <c r="BD21" s="1">
         <v>15.6</v>
       </c>
-      <c r="BE20" s="68"/>
-      <c r="BF20" s="68"/>
-      <c r="BG20" s="68"/>
-      <c r="BH20" s="68"/>
-      <c r="BI20" s="68"/>
-      <c r="BJ20" s="68"/>
-      <c r="BK20" s="68"/>
-      <c r="BL20" s="68"/>
-      <c r="BM20" s="68"/>
-      <c r="BN20" s="68"/>
-      <c r="BO20" s="68"/>
+      <c r="BE21" s="68"/>
+      <c r="BF21" s="68"/>
+      <c r="BG21" s="68"/>
+      <c r="BH21" s="68"/>
+      <c r="BI21" s="68"/>
+      <c r="BJ21" s="68"/>
+      <c r="BK21" s="68"/>
+      <c r="BL21" s="68"/>
+      <c r="BM21" s="68"/>
+      <c r="BN21" s="68"/>
+      <c r="BO21" s="68"/>
+      <c r="BP21" s="68"/>
     </row>
   </sheetData>
-  <dataValidations xWindow="382" yWindow="552" count="5">
+  <dataValidations disablePrompts="1" xWindow="382" yWindow="552" count="5">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BE12:BF12 E4:BF6">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
@@ -3620,17 +3677,17 @@
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C20:C1048576 C2:C17">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C21:C1048576 C2:C18">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Leave blank" sqref="B18:C19"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Leave blank" sqref="B19:C20"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="382" yWindow="552" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" xWindow="382" yWindow="552" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$A$2:$A$4</xm:f>

</xml_diff>

<commit_message>
Automatic adjustment of starting population
Component of "automatic calibration" - starting population is adjusted after each accepted model run to better target the present day population (only if target_population parameter included in sheets).
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="495" windowWidth="20370" windowHeight="7350" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="495" windowWidth="20370" windowHeight="7350" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>parameter</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>int_perc_awareness_raising</t>
+  </si>
+  <si>
+    <t>target_population</t>
   </si>
 </sst>
 </file>
@@ -318,7 +321,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -409,17 +412,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="664">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1087,7 +1079,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1121,8 +1113,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1168,6 +1158,7 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2138,10 +2129,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2176,13 +2167,13 @@
       <c r="A2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="48">
+      <c r="B2" s="46">
         <v>7.55</v>
       </c>
-      <c r="F2" s="48">
+      <c r="F2" s="46">
         <v>7.55</v>
       </c>
-      <c r="G2" s="48">
+      <c r="G2" s="46">
         <v>7.85</v>
       </c>
       <c r="H2">
@@ -2190,16 +2181,16 @@
       </c>
     </row>
     <row r="3" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="49">
+      <c r="B3" s="47">
         <v>0.22</v>
       </c>
-      <c r="F3" s="49">
+      <c r="F3" s="47">
         <v>0.22</v>
       </c>
-      <c r="G3" s="49">
+      <c r="G3" s="47">
         <v>0.22</v>
       </c>
       <c r="H3">
@@ -2210,13 +2201,13 @@
       <c r="A4" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="50">
+      <c r="B4" s="48">
         <v>1865</v>
       </c>
-      <c r="F4" s="50">
+      <c r="F4" s="48">
         <v>1865</v>
       </c>
-      <c r="G4" s="50">
+      <c r="G4" s="48">
         <v>1865</v>
       </c>
       <c r="H4">
@@ -2224,33 +2215,43 @@
       </c>
     </row>
     <row r="5" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="51">
+      <c r="B5" s="49">
         <v>190000</v>
       </c>
-      <c r="F5" s="51">
+      <c r="F5" s="49">
         <v>190000</v>
       </c>
-      <c r="G5" s="51">
+      <c r="G5" s="49">
         <v>190000</v>
       </c>
       <c r="H5">
         <v>280000</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+    <row r="6" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="49">
+        <v>892000</v>
+      </c>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B7" s="28">
         <v>5</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C7" s="20">
         <v>15</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D7" s="20">
         <v>25</v>
       </c>
     </row>
@@ -2260,7 +2261,7 @@
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5 F5:G5">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B6 F5:G6">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
@@ -2286,7 +2287,7 @@
   </sheetPr>
   <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2298,7 +2299,7 @@
     <col min="1" max="1" width="56" style="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11" style="39" customWidth="1"/>
+    <col min="4" max="4" width="11" style="37" customWidth="1"/>
     <col min="5" max="5" width="7.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" style="1" customWidth="1"/>
     <col min="7" max="10" width="7" style="1" customWidth="1"/>
@@ -2385,7 +2386,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="6"/>
-      <c r="D2" s="34"/>
+      <c r="D2" s="32"/>
       <c r="J2" s="7">
         <v>0</v>
       </c>
@@ -2395,15 +2396,15 @@
       <c r="M2" s="7">
         <v>23.6</v>
       </c>
-      <c r="O2" s="52">
+      <c r="O2" s="50">
         <v>80</v>
       </c>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
-      <c r="R2" s="52"/>
-      <c r="S2" s="52"/>
-      <c r="T2" s="52"/>
-      <c r="U2" s="52">
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="50">
         <v>80</v>
       </c>
     </row>
@@ -2415,19 +2416,19 @@
         <v>3</v>
       </c>
       <c r="C3" s="6"/>
-      <c r="D3" s="34"/>
+      <c r="D3" s="32"/>
       <c r="M3" s="7">
         <v>0</v>
       </c>
-      <c r="O3" s="52">
+      <c r="O3" s="50">
         <v>80</v>
       </c>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="52"/>
-      <c r="R3" s="52"/>
-      <c r="S3" s="52"/>
-      <c r="T3" s="52"/>
-      <c r="U3" s="52">
+      <c r="P3" s="50"/>
+      <c r="Q3" s="50"/>
+      <c r="R3" s="50"/>
+      <c r="S3" s="50"/>
+      <c r="T3" s="50"/>
+      <c r="U3" s="50">
         <v>80</v>
       </c>
     </row>
@@ -2439,18 +2440,18 @@
         <v>4</v>
       </c>
       <c r="C4" s="8"/>
-      <c r="D4" s="35">
+      <c r="D4" s="33">
         <v>70</v>
       </c>
       <c r="L4" s="9">
         <v>85</v>
       </c>
-      <c r="P4" s="54"/>
-      <c r="Q4" s="54"/>
-      <c r="R4" s="54"/>
-      <c r="S4" s="54"/>
-      <c r="T4" s="54"/>
-      <c r="U4" s="54"/>
+      <c r="P4" s="52"/>
+      <c r="Q4" s="52"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="52"/>
+      <c r="T4" s="52"/>
+      <c r="U4" s="52"/>
     </row>
     <row r="5" spans="1:28" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
@@ -2460,7 +2461,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="10"/>
-      <c r="D5" s="36"/>
+      <c r="D5" s="34"/>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
@@ -2471,12 +2472,12 @@
       <c r="L5" s="19">
         <v>85</v>
       </c>
-      <c r="P5" s="55"/>
-      <c r="Q5" s="55"/>
-      <c r="R5" s="55"/>
-      <c r="S5" s="55"/>
-      <c r="T5" s="55"/>
-      <c r="U5" s="55"/>
+      <c r="P5" s="53"/>
+      <c r="Q5" s="53"/>
+      <c r="R5" s="53"/>
+      <c r="S5" s="53"/>
+      <c r="T5" s="53"/>
+      <c r="U5" s="53"/>
     </row>
     <row r="6" spans="1:28" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
@@ -2488,7 +2489,7 @@
       <c r="C6" s="10">
         <v>3</v>
       </c>
-      <c r="D6" s="36"/>
+      <c r="D6" s="34"/>
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
@@ -2498,12 +2499,12 @@
       <c r="M6" s="11">
         <v>5</v>
       </c>
-      <c r="P6" s="55"/>
-      <c r="Q6" s="55"/>
-      <c r="R6" s="55"/>
-      <c r="S6" s="55"/>
-      <c r="T6" s="55"/>
-      <c r="U6" s="55"/>
+      <c r="P6" s="53"/>
+      <c r="Q6" s="53"/>
+      <c r="R6" s="53"/>
+      <c r="S6" s="53"/>
+      <c r="T6" s="53"/>
+      <c r="U6" s="53"/>
     </row>
     <row r="7" spans="1:28" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
@@ -2513,7 +2514,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="24"/>
-      <c r="D7" s="38"/>
+      <c r="D7" s="36"/>
       <c r="G7" s="26"/>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2523,14 +2524,14 @@
       <c r="M7" s="25">
         <v>0</v>
       </c>
-      <c r="P7" s="57">
+      <c r="P7" s="55">
         <v>100</v>
       </c>
-      <c r="Q7" s="57"/>
-      <c r="R7" s="57"/>
-      <c r="S7" s="57"/>
-      <c r="T7" s="57"/>
-      <c r="U7" s="57">
+      <c r="Q7" s="55"/>
+      <c r="R7" s="55"/>
+      <c r="S7" s="55"/>
+      <c r="T7" s="55"/>
+      <c r="U7" s="55">
         <v>100</v>
       </c>
     </row>
@@ -2542,37 +2543,37 @@
         <v>3</v>
       </c>
       <c r="C8" s="12"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33">
+      <c r="D8" s="35"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31">
         <v>0</v>
       </c>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="58"/>
-      <c r="Q8" s="58">
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="56"/>
+      <c r="Q8" s="56">
         <v>100</v>
       </c>
-      <c r="R8" s="58"/>
-      <c r="S8" s="58"/>
-      <c r="T8" s="58"/>
-      <c r="U8" s="58">
+      <c r="R8" s="56"/>
+      <c r="S8" s="56"/>
+      <c r="T8" s="56"/>
+      <c r="U8" s="56">
         <v>100</v>
       </c>
-      <c r="V8" s="33"/>
-      <c r="W8" s="33"/>
-      <c r="X8" s="33"/>
-      <c r="Y8" s="33"/>
-      <c r="Z8" s="33"/>
-      <c r="AA8" s="33"/>
-      <c r="AB8" s="33"/>
+      <c r="V8" s="31"/>
+      <c r="W8" s="31"/>
+      <c r="X8" s="31"/>
+      <c r="Y8" s="31"/>
+      <c r="Z8" s="31"/>
+      <c r="AA8" s="31"/>
+      <c r="AB8" s="31"/>
     </row>
     <row r="9" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
@@ -2582,131 +2583,131 @@
         <v>3</v>
       </c>
       <c r="C9" s="12"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33">
+      <c r="D9" s="35"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31">
         <v>0</v>
       </c>
-      <c r="N9" s="33"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="58"/>
-      <c r="Q9" s="58"/>
-      <c r="R9" s="58">
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="56"/>
+      <c r="Q9" s="56"/>
+      <c r="R9" s="56">
         <v>70</v>
       </c>
-      <c r="S9" s="58"/>
-      <c r="T9" s="58"/>
-      <c r="U9" s="58">
+      <c r="S9" s="56"/>
+      <c r="T9" s="56"/>
+      <c r="U9" s="56">
         <v>70</v>
       </c>
-      <c r="V9" s="33"/>
-      <c r="W9" s="33"/>
-      <c r="X9" s="33"/>
-      <c r="Y9" s="33"/>
-      <c r="Z9" s="33"/>
-      <c r="AA9" s="33"/>
-      <c r="AB9" s="33"/>
+      <c r="V9" s="31"/>
+      <c r="W9" s="31"/>
+      <c r="X9" s="31"/>
+      <c r="Y9" s="31"/>
+      <c r="Z9" s="31"/>
+      <c r="AA9" s="31"/>
+      <c r="AB9" s="31"/>
     </row>
-    <row r="10" spans="1:28" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
+    <row r="10" spans="1:28" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="42"/>
-      <c r="M10" s="43">
+      <c r="C10" s="39"/>
+      <c r="D10" s="40"/>
+      <c r="M10" s="41">
         <v>0</v>
       </c>
-      <c r="P10" s="53"/>
-      <c r="Q10" s="53"/>
-      <c r="R10" s="53"/>
-      <c r="S10" s="53">
+      <c r="P10" s="51"/>
+      <c r="Q10" s="51"/>
+      <c r="R10" s="51"/>
+      <c r="S10" s="51">
         <v>50</v>
       </c>
-      <c r="T10" s="53"/>
-      <c r="U10" s="53">
+      <c r="T10" s="51"/>
+      <c r="U10" s="51">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:28" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
+    <row r="11" spans="1:28" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="42"/>
-      <c r="M11" s="43">
+      <c r="C11" s="39"/>
+      <c r="D11" s="40"/>
+      <c r="M11" s="41">
         <v>0</v>
       </c>
-      <c r="P11" s="53"/>
-      <c r="Q11" s="53"/>
-      <c r="R11" s="53"/>
-      <c r="S11" s="53"/>
-      <c r="T11" s="53">
+      <c r="P11" s="51"/>
+      <c r="Q11" s="51"/>
+      <c r="R11" s="51"/>
+      <c r="S11" s="51"/>
+      <c r="T11" s="51">
         <v>50</v>
       </c>
-      <c r="U11" s="53">
+      <c r="U11" s="51">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:28" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+    <row r="12" spans="1:28" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="46">
+      <c r="C12" s="43"/>
+      <c r="D12" s="44">
         <v>4.3099999999999996</v>
       </c>
-      <c r="E12" s="47">
+      <c r="E12" s="45">
         <v>25.9</v>
       </c>
-      <c r="F12" s="47">
+      <c r="F12" s="45">
         <v>58.6</v>
       </c>
-      <c r="G12" s="47">
+      <c r="G12" s="45">
         <v>73.599999999999994</v>
       </c>
-      <c r="H12" s="47">
+      <c r="H12" s="45">
         <v>78.900000000000006</v>
       </c>
-      <c r="I12" s="47">
+      <c r="I12" s="45">
         <v>96.5</v>
       </c>
-      <c r="J12" s="47">
+      <c r="J12" s="45">
         <v>107.3</v>
       </c>
-      <c r="K12" s="47">
+      <c r="K12" s="45">
         <v>110.9</v>
       </c>
-      <c r="L12" s="47">
+      <c r="L12" s="45">
         <v>114.2</v>
       </c>
-      <c r="M12" s="47">
+      <c r="M12" s="45">
         <v>114.8</v>
       </c>
-      <c r="N12" s="47">
+      <c r="N12" s="45">
         <v>116.4</v>
       </c>
-      <c r="P12" s="59"/>
-      <c r="Q12" s="59"/>
-      <c r="R12" s="59"/>
-      <c r="S12" s="59"/>
-      <c r="T12" s="59"/>
-      <c r="U12" s="59"/>
+      <c r="P12" s="57"/>
+      <c r="Q12" s="57"/>
+      <c r="R12" s="57"/>
+      <c r="S12" s="57"/>
+      <c r="T12" s="57"/>
+      <c r="U12" s="57"/>
     </row>
     <row r="13" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
@@ -2716,7 +2717,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="12"/>
-      <c r="D13" s="37">
+      <c r="D13" s="35">
         <v>1</v>
       </c>
       <c r="E13" s="13">
@@ -2725,12 +2726,12 @@
       <c r="J13" s="13">
         <v>3.11</v>
       </c>
-      <c r="P13" s="56"/>
-      <c r="Q13" s="56"/>
-      <c r="R13" s="56"/>
-      <c r="S13" s="56"/>
-      <c r="T13" s="56"/>
-      <c r="U13" s="56"/>
+      <c r="P13" s="54"/>
+      <c r="Q13" s="54"/>
+      <c r="R13" s="54"/>
+      <c r="S13" s="54"/>
+      <c r="T13" s="54"/>
+      <c r="U13" s="54"/>
     </row>
     <row r="14" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
@@ -2740,7 +2741,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="12"/>
-      <c r="D14" s="37">
+      <c r="D14" s="35">
         <v>0</v>
       </c>
       <c r="E14" s="13">
@@ -2767,12 +2768,12 @@
       <c r="N14" s="13">
         <v>15.6</v>
       </c>
-      <c r="P14" s="56"/>
-      <c r="Q14" s="56"/>
-      <c r="R14" s="56"/>
-      <c r="S14" s="56"/>
-      <c r="T14" s="56"/>
-      <c r="U14" s="56"/>
+      <c r="P14" s="54"/>
+      <c r="Q14" s="54"/>
+      <c r="R14" s="54"/>
+      <c r="S14" s="54"/>
+      <c r="T14" s="54"/>
+      <c r="U14" s="54"/>
     </row>
   </sheetData>
   <dataValidations xWindow="382" yWindow="552" count="4">

</xml_diff>

<commit_message>
Prevent treatment outcomes summing to >1
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -2291,7 +2291,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2461,7 +2461,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="34"/>
       <c r="G5" s="19"/>

</xml_diff>

<commit_message>
Revise values from last commit for Fiji
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -2291,7 +2291,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2461,7 +2461,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="10">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D5" s="34"/>
       <c r="G5" s="19"/>
@@ -2485,7 +2485,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="10">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="D6" s="34"/>
       <c r="G6" s="19"/>

</xml_diff>

<commit_message>
Writing calibration parameters back to sheets
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="495" windowWidth="20370" windowHeight="7350" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="495" windowWidth="20370" windowHeight="7350" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>parameter</t>
   </si>
@@ -87,16 +87,7 @@
     <t>runge_kutta</t>
   </si>
   <si>
-    <t>age_unstratified</t>
-  </si>
-  <si>
     <t>econ_cpi</t>
-  </si>
-  <si>
-    <t>without_diabetes</t>
-  </si>
-  <si>
-    <t>with_diabetes</t>
   </si>
   <si>
     <t>program_perc_algorithm_sensitivity</t>
@@ -2129,121 +2120,70 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.5703125" style="21" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" style="28" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="20"/>
-    <col min="6" max="6" width="13.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="20"/>
+    <col min="3" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="46">
         <v>7.55</v>
       </c>
-      <c r="F2" s="46">
-        <v>7.55</v>
-      </c>
-      <c r="G2" s="46">
-        <v>7.85</v>
-      </c>
-      <c r="H2">
-        <v>6.2</v>
-      </c>
     </row>
-    <row r="3" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="58" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="47">
         <v>0.22</v>
       </c>
-      <c r="F3" s="47">
-        <v>0.22</v>
-      </c>
-      <c r="G3" s="47">
-        <v>0.22</v>
-      </c>
-      <c r="H3">
-        <v>0.2</v>
-      </c>
     </row>
-    <row r="4" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="48">
         <v>1865</v>
       </c>
-      <c r="F4" s="48">
-        <v>1865</v>
-      </c>
-      <c r="G4" s="48">
-        <v>1865</v>
-      </c>
-      <c r="H4">
-        <v>1915</v>
-      </c>
     </row>
-    <row r="5" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="49">
         <v>190000</v>
       </c>
-      <c r="F5" s="49">
-        <v>190000</v>
-      </c>
-      <c r="G5" s="49">
-        <v>190000</v>
-      </c>
-      <c r="H5">
-        <v>280000</v>
-      </c>
     </row>
-    <row r="6" spans="1:8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B6" s="49">
         <v>892000</v>
       </c>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B7" s="28">
         <v>5</v>
@@ -2256,24 +2196,23 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 F4:G4">
+  <dataValidations count="4">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B6 F5:G6">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B6">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 F2:G2">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3 F3:G3">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age unstratified" prompt="Some values you can replace the ones to the left with if you want a manual calibration for the model without age stratification." sqref="H1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2287,7 +2226,7 @@
   </sheetPr>
   <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2380,7 +2319,7 @@
     </row>
     <row r="2" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>3</v>
@@ -2410,7 +2349,7 @@
     </row>
     <row r="3" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>3</v>
@@ -2434,7 +2373,7 @@
     </row>
     <row r="4" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>4</v>
@@ -2455,7 +2394,7 @@
     </row>
     <row r="5" spans="1:28" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>3</v>
@@ -2479,7 +2418,7 @@
     </row>
     <row r="6" spans="1:28" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>3</v>
@@ -2506,7 +2445,7 @@
     </row>
     <row r="7" spans="1:28" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B7" s="24" t="s">
         <v>3</v>
@@ -2535,7 +2474,7 @@
     </row>
     <row r="8" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>3</v>
@@ -2575,7 +2514,7 @@
     </row>
     <row r="9" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>3</v>
@@ -2615,7 +2554,7 @@
     </row>
     <row r="10" spans="1:28" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B10" s="39" t="s">
         <v>3</v>
@@ -2638,7 +2577,7 @@
     </row>
     <row r="11" spans="1:28" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B11" s="39" t="s">
         <v>3</v>
@@ -2661,7 +2600,7 @@
     </row>
     <row r="12" spans="1:28" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="43" t="s">
         <v>3</v>
@@ -2709,7 +2648,7 @@
     </row>
     <row r="13" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>3</v>
@@ -2733,7 +2672,7 @@
     </row>
     <row r="14" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Manually recalibrate Fiji with vaccination re-instated
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="495" windowWidth="20370" windowHeight="7350" tabRatio="807" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="495" windowWidth="20370" windowHeight="7350" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -2125,8 +2125,8 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2149,7 +2149,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="46">
-        <v>7.55</v>
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="3" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2229,7 +2229,7 @@
   </sheetPr>
   <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Remove unnecessary time-variant parameter for diabetes RR
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="495" windowWidth="20370" windowHeight="7350" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="495" windowWidth="20370" windowHeight="7350" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>parameter</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>program_perc_algorithm_sensitivity</t>
-  </si>
-  <si>
-    <t>epi_rr_diabetes</t>
   </si>
   <si>
     <t>age_breakpoints</t>
@@ -2125,7 +2122,7 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2178,7 +2175,7 @@
     </row>
     <row r="6" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="49">
         <v>892000</v>
@@ -2186,7 +2183,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="28">
         <v>5</v>
@@ -2227,13 +2224,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AB14"/>
+  <dimension ref="A1:AB13"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2320,12 +2317,12 @@
         <v>18</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>3</v>
@@ -2355,7 +2352,7 @@
     </row>
     <row r="3" spans="1:28" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>3</v>
@@ -2400,7 +2397,7 @@
     </row>
     <row r="5" spans="1:28" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>3</v>
@@ -2424,7 +2421,7 @@
     </row>
     <row r="6" spans="1:28" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>3</v>
@@ -2451,7 +2448,7 @@
     </row>
     <row r="7" spans="1:28" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="24" t="s">
         <v>3</v>
@@ -2480,7 +2477,7 @@
     </row>
     <row r="8" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>3</v>
@@ -2522,7 +2519,7 @@
     </row>
     <row r="9" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>3</v>
@@ -2562,7 +2559,7 @@
     </row>
     <row r="10" spans="1:28" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="39" t="s">
         <v>3</v>
@@ -2585,7 +2582,7 @@
     </row>
     <row r="11" spans="1:28" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="39" t="s">
         <v>3</v>
@@ -2656,20 +2653,38 @@
     </row>
     <row r="13" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="13">
-        <v>1.1000000000000001</v>
+        <v>7.7</v>
+      </c>
+      <c r="F13" s="13">
+        <v>11.1</v>
+      </c>
+      <c r="G13" s="13">
+        <v>16.5</v>
+      </c>
+      <c r="H13" s="13">
+        <v>14.5</v>
+      </c>
+      <c r="I13" s="13">
+        <v>16.100000000000001</v>
       </c>
       <c r="J13" s="13">
-        <v>3.11</v>
+        <v>15.6</v>
+      </c>
+      <c r="L13" s="13">
+        <v>15.6</v>
+      </c>
+      <c r="N13" s="13">
+        <v>15.6</v>
       </c>
       <c r="P13" s="54"/>
       <c r="Q13" s="54"/>
@@ -2677,48 +2692,6 @@
       <c r="S13" s="54"/>
       <c r="T13" s="54"/>
       <c r="U13" s="54"/>
-    </row>
-    <row r="14" spans="1:28" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="35">
-        <v>0</v>
-      </c>
-      <c r="E14" s="13">
-        <v>7.7</v>
-      </c>
-      <c r="F14" s="13">
-        <v>11.1</v>
-      </c>
-      <c r="G14" s="13">
-        <v>16.5</v>
-      </c>
-      <c r="H14" s="13">
-        <v>14.5</v>
-      </c>
-      <c r="I14" s="13">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="J14" s="13">
-        <v>15.6</v>
-      </c>
-      <c r="L14" s="13">
-        <v>15.6</v>
-      </c>
-      <c r="N14" s="13">
-        <v>15.6</v>
-      </c>
-      <c r="P14" s="54"/>
-      <c r="Q14" s="54"/>
-      <c r="R14" s="54"/>
-      <c r="S14" s="54"/>
-      <c r="T14" s="54"/>
-      <c r="U14" s="54"/>
     </row>
   </sheetData>
   <dataValidations xWindow="549" yWindow="311" count="4">
@@ -2727,11 +2700,11 @@
       <formula2>100000000000000000000</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="C1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:P6 E7:O7">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:P6 E7:O7">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C1048576">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Make diagnostic algorithm sensitivity constant in Fiji for simplicity
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -2230,7 +2230,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2383,10 +2383,10 @@
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="33">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="L4" s="9">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="P4" s="52"/>
       <c r="Q4" s="52"/>

</xml_diff>

<commit_message>
Change Fiji birth rate smoothness to zero
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>parameter</t>
   </si>
@@ -142,13 +142,16 @@
   </si>
   <si>
     <t>runge_kutta</t>
+  </si>
+  <si>
+    <t>demo_rate_birth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +240,13 @@
     <font>
       <sz val="11"/>
       <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1046,7 +1056,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="661" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="661" applyFont="1" applyBorder="1"/>
@@ -1128,6 +1138,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="661" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="661" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="661" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="661" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="661" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="663">
     <cellStyle name="Comma 2" xfId="614"/>
@@ -2231,13 +2244,13 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:AB13"/>
+  <dimension ref="A1:AB14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2328,47 +2341,34 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:28" s="63" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="61" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="25"/>
-      <c r="J2" s="6">
+      <c r="C2" s="62">
         <v>0</v>
-      </c>
-      <c r="K2" s="6">
-        <v>7</v>
-      </c>
-      <c r="M2" s="6">
-        <v>23.6</v>
-      </c>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39">
-        <v>80</v>
-      </c>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39">
-        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="25"/>
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
+      <c r="K3" s="6">
+        <v>7</v>
+      </c>
       <c r="M3" s="6">
-        <v>0</v>
+        <v>23.6</v>
       </c>
       <c r="O3" s="39"/>
       <c r="P3" s="39"/>
@@ -2382,60 +2382,60 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="25"/>
+      <c r="M4" s="6">
+        <v>0</v>
+      </c>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39">
+        <v>80</v>
+      </c>
+      <c r="S4" s="39"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="39">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="26">
+      <c r="C5" s="7"/>
+      <c r="D5" s="26">
         <v>80</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L5" s="8">
         <v>80</v>
       </c>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="41"/>
-      <c r="R4" s="41"/>
-      <c r="S4" s="41"/>
-      <c r="T4" s="41"/>
-      <c r="U4" s="41"/>
-    </row>
-    <row r="5" spans="1:28" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="9">
-        <v>0.4</v>
-      </c>
-      <c r="D5" s="27"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="P5" s="42"/>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="42"/>
-      <c r="S5" s="42"/>
-      <c r="T5" s="42"/>
-      <c r="U5" s="42"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="41"/>
+      <c r="T5" s="41"/>
+      <c r="U5" s="41"/>
     </row>
     <row r="6" spans="1:28" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="9">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="D6" s="27"/>
       <c r="G6" s="18"/>
@@ -2444,9 +2444,6 @@
       <c r="J6" s="18"/>
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
-      <c r="M6" s="10">
-        <v>5</v>
-      </c>
       <c r="P6" s="42"/>
       <c r="Q6" s="42"/>
       <c r="R6" s="42"/>
@@ -2454,78 +2451,65 @@
       <c r="T6" s="42"/>
       <c r="U6" s="42"/>
     </row>
-    <row r="7" spans="1:28" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+    <row r="7" spans="1:28" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="D7" s="27"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="10">
+        <v>5</v>
+      </c>
+      <c r="P7" s="42"/>
+      <c r="Q7" s="42"/>
+      <c r="R7" s="42"/>
+      <c r="S7" s="42"/>
+      <c r="T7" s="42"/>
+      <c r="U7" s="42"/>
+    </row>
+    <row r="8" spans="1:28" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B8" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="29"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="22">
+      <c r="C8" s="21"/>
+      <c r="D8" s="29"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="22">
         <v>0</v>
       </c>
-      <c r="P7" s="44"/>
-      <c r="Q7" s="44">
+      <c r="P8" s="44"/>
+      <c r="Q8" s="44">
         <v>100</v>
       </c>
-      <c r="R7" s="44"/>
-      <c r="S7" s="44"/>
-      <c r="T7" s="44"/>
-      <c r="U7" s="44">
+      <c r="R8" s="44"/>
+      <c r="S8" s="44"/>
+      <c r="T8" s="44"/>
+      <c r="U8" s="44">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24">
-        <v>0</v>
-      </c>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24">
-        <v>100</v>
-      </c>
-      <c r="P8" s="45"/>
-      <c r="Q8" s="45"/>
-      <c r="R8" s="45"/>
-      <c r="S8" s="45"/>
-      <c r="T8" s="45"/>
-      <c r="U8" s="45">
-        <v>100</v>
-      </c>
-      <c r="V8" s="24"/>
-      <c r="W8" s="24"/>
-      <c r="X8" s="24"/>
-      <c r="Y8" s="24"/>
-      <c r="Z8" s="24"/>
-      <c r="AA8" s="24"/>
-      <c r="AB8" s="24"/>
     </row>
     <row r="9" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>24</v>
@@ -2544,20 +2528,18 @@
         <v>0</v>
       </c>
       <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="45">
-        <v>70</v>
-      </c>
+      <c r="O9" s="24">
+        <v>100</v>
+      </c>
+      <c r="P9" s="45"/>
       <c r="Q9" s="45"/>
       <c r="R9" s="45"/>
       <c r="S9" s="45"/>
       <c r="T9" s="45"/>
       <c r="U9" s="45">
-        <v>70</v>
-      </c>
-      <c r="V9" s="24">
-        <v>70</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="V9" s="24"/>
       <c r="W9" s="24"/>
       <c r="X9" s="24"/>
       <c r="Y9" s="24"/>
@@ -2565,32 +2547,51 @@
       <c r="AA9" s="24"/>
       <c r="AB9" s="24"/>
     </row>
-    <row r="10" spans="1:28" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="32" t="s">
+    <row r="10" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="33"/>
-      <c r="M10" s="34">
+      <c r="C10" s="11"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24">
         <v>0</v>
       </c>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="40"/>
-      <c r="R10" s="40"/>
-      <c r="S10" s="40">
-        <v>50</v>
-      </c>
-      <c r="T10" s="40"/>
-      <c r="U10" s="40">
-        <v>50</v>
-      </c>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="45">
+        <v>70</v>
+      </c>
+      <c r="Q10" s="45"/>
+      <c r="R10" s="45"/>
+      <c r="S10" s="45"/>
+      <c r="T10" s="45"/>
+      <c r="U10" s="45">
+        <v>70</v>
+      </c>
+      <c r="V10" s="24">
+        <v>70</v>
+      </c>
+      <c r="W10" s="24"/>
+      <c r="X10" s="24"/>
+      <c r="Y10" s="24"/>
+      <c r="Z10" s="24"/>
+      <c r="AA10" s="24"/>
+      <c r="AB10" s="24"/>
     </row>
     <row r="11" spans="1:28" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="32" t="s">
         <v>24</v>
@@ -2603,122 +2604,145 @@
       <c r="P11" s="40"/>
       <c r="Q11" s="40"/>
       <c r="R11" s="40"/>
-      <c r="S11" s="40"/>
-      <c r="T11" s="40">
+      <c r="S11" s="40">
         <v>50</v>
       </c>
+      <c r="T11" s="40"/>
       <c r="U11" s="40">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:28" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+    <row r="12" spans="1:28" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="32"/>
+      <c r="D12" s="33"/>
+      <c r="M12" s="34">
+        <v>0</v>
+      </c>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="40"/>
+      <c r="R12" s="40"/>
+      <c r="S12" s="40"/>
+      <c r="T12" s="40">
+        <v>50</v>
+      </c>
+      <c r="U12" s="40">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B13" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="37">
+      <c r="C13" s="36"/>
+      <c r="D13" s="37">
         <v>4.3099999999999996</v>
       </c>
-      <c r="E12" s="38">
+      <c r="E13" s="38">
         <v>25.9</v>
       </c>
-      <c r="F12" s="38">
+      <c r="F13" s="38">
         <v>58.6</v>
       </c>
-      <c r="G12" s="38">
+      <c r="G13" s="38">
         <v>73.599999999999994</v>
       </c>
-      <c r="H12" s="38">
+      <c r="H13" s="38">
         <v>78.900000000000006</v>
       </c>
-      <c r="I12" s="38">
+      <c r="I13" s="38">
         <v>96.5</v>
       </c>
-      <c r="J12" s="38">
+      <c r="J13" s="38">
         <v>107.3</v>
       </c>
-      <c r="K12" s="38">
+      <c r="K13" s="38">
         <v>110.9</v>
       </c>
-      <c r="L12" s="38">
+      <c r="L13" s="38">
         <v>114.2</v>
       </c>
-      <c r="M12" s="38">
+      <c r="M13" s="38">
         <v>114.8</v>
       </c>
-      <c r="N12" s="38">
+      <c r="N13" s="38">
         <v>116.4</v>
       </c>
-      <c r="P12" s="46"/>
-      <c r="Q12" s="46"/>
-      <c r="R12" s="46"/>
-      <c r="S12" s="46"/>
-      <c r="T12" s="46"/>
-      <c r="U12" s="46"/>
+      <c r="P13" s="46"/>
+      <c r="Q13" s="46"/>
+      <c r="R13" s="46"/>
+      <c r="S13" s="46"/>
+      <c r="T13" s="46"/>
+      <c r="U13" s="46"/>
     </row>
-    <row r="13" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+    <row r="14" spans="1:28" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B14" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="28">
+      <c r="C14" s="11"/>
+      <c r="D14" s="28">
         <v>0</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E14" s="12">
         <v>7.7</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F14" s="12">
         <v>11.1</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G14" s="12">
         <v>16.5</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H14" s="12">
         <v>14.5</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I14" s="12">
         <v>16.100000000000001</v>
       </c>
-      <c r="J13" s="12">
+      <c r="J14" s="12">
         <v>15.6</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L14" s="12">
         <v>15.6</v>
       </c>
-      <c r="N13" s="12">
+      <c r="N14" s="12">
         <v>15.6</v>
       </c>
-      <c r="P13" s="43"/>
-      <c r="Q13" s="43"/>
-      <c r="R13" s="43"/>
-      <c r="S13" s="43"/>
-      <c r="T13" s="43"/>
-      <c r="U13" s="43"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="43"/>
+      <c r="S14" s="43"/>
+      <c r="T14" s="43"/>
+      <c r="U14" s="43"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3 F2:F3 G2:G3 H2:H3 I2:I3 J2:J3 K2:K3 L2:L3 M2:M3 N2:N3 P2:P3 P7">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E4 F3:F4 G3:G4 H3:H4 I3:I4 J3:J4 K3:K4 L3:L4 M3:M4 N3:N4 P3:P4 P8">
       <formula1>0</formula1>
       <formula2>100000000000000000000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E7 F4:F7 G4:G7 H4:H7 I4:I7 J4:J7 K4:K7 L4:L7 M4:M7 N4:N7 O4:O7 P4:P6">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C2"/>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E8 F5:F8 G5:G8 H5:H8 I5:I8 J5:J8 K5:K8 L5:L8 M5:M8 N5:N8 O5:O8 P5:P7">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C2:C1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Smoothness for fitting function" prompt="Must be positive." sqref="C3:C1048576">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
progress graphs in uncertainty runs
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -2138,7 +2138,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="48" t="n">
-        <v>10.02519178390472</v>
+        <v>9.817290327844651</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2146,7 +2146,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="51" t="n">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2154,7 +2154,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="53" t="n">
-        <v>1861.897013931144</v>
+        <v>1849.448887606751</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2162,7 +2162,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="55" t="n">
-        <v>32746.97856410749</v>
+        <v>24267.59167219321</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2192,7 +2192,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.6965859827417181</v>
+        <v>0.7705065931625953</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2200,7 +2200,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.73905411984906</v>
+        <v>0.6994721573256851</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2208,7 +2208,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="n">
-        <v>2.881191041849715</v>
+        <v>2.894718404854602</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2216,7 +2216,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="n">
-        <v>0.5163360806154627</v>
+        <v>0.3826378407848143</v>
       </c>
     </row>
     <row r="12" spans="1:4">

</xml_diff>

<commit_message>
changed colors for uncertainty graphs
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -2138,7 +2138,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="48" t="n">
-        <v>9.970903720917134</v>
+        <v>10.19985961024888</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2154,7 +2154,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="53" t="n">
-        <v>1852.351817929654</v>
+        <v>1856.545344897319</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2162,7 +2162,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="55" t="n">
-        <v>22187.12543323998</v>
+        <v>24358.99779796487</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2192,7 +2192,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.7746103891367108</v>
+        <v>0.809744300858402</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2200,7 +2200,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.7208279240945256</v>
+        <v>0.7073697945015182</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2208,7 +2208,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="n">
-        <v>2.876745655976449</v>
+        <v>2.822627157457899</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2216,7 +2216,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="n">
-        <v>0.3498342103194587</v>
+        <v>0.3840790815586094</v>
       </c>
     </row>
     <row r="12" spans="1:4">

</xml_diff>

<commit_message>
run local app without autoreload for stability
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -2138,7 +2138,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="48" t="n">
-        <v>10.19985961024888</v>
+        <v>10.00636840280725</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2146,7 +2146,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="51" t="n">
-        <v>0.12</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2154,7 +2154,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="53" t="n">
-        <v>1856.545344897319</v>
+        <v>1851.692682370092</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2162,7 +2162,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="55" t="n">
-        <v>24358.99779796487</v>
+        <v>22457.07626537552</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2192,7 +2192,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.809744300858402</v>
+        <v>0.9385700862638099</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2200,7 +2200,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.7073697945015182</v>
+        <v>0.7179030094017506</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2208,7 +2208,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="n">
-        <v>2.822627157457899</v>
+        <v>2.814137998255945</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2216,7 +2216,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="n">
-        <v>0.3840790815586094</v>
+        <v>0.3540906443703401</v>
       </c>
     </row>
     <row r="12" spans="1:4">

</xml_diff>

<commit_message>
bug in choosing country and updating country default
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -2138,7 +2138,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="48" t="n">
-        <v>10.00636840280725</v>
+        <v>10.37627124123017</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2146,7 +2146,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="51" t="n">
-        <v>0.18</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2154,7 +2154,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="53" t="n">
-        <v>1851.692682370092</v>
+        <v>1850.937149452345</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2162,7 +2162,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="55" t="n">
-        <v>22457.07626537552</v>
+        <v>21738.69177262505</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2192,7 +2192,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>0.9385700862638099</v>
+        <v>1.056396007190265</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2200,7 +2200,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.7179030094017506</v>
+        <v>0.6809103347581049</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2208,7 +2208,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="n">
-        <v>2.814137998255945</v>
+        <v>2.734361650964236</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2216,7 +2216,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="n">
-        <v>0.3540906443703401</v>
+        <v>0.3427635586474372</v>
       </c>
     </row>
     <row r="12" spans="1:4">

</xml_diff>

<commit_message>
Latest calibration for Fiji
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="0" windowHeight="5472" windowWidth="15336" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="constants" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,7 +11,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="dropdown_lists" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="171027" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -2138,7 +2138,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="48" t="n">
-        <v>10.17422281085064</v>
+        <v>10.03626685000244</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2146,7 +2146,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="51" t="n">
-        <v>0.18</v>
+        <v>0.09999999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2154,7 +2154,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="53" t="n">
-        <v>1845.018986338566</v>
+        <v>1845.010175260038</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2162,7 +2162,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="55" t="n">
-        <v>18623.57973254978</v>
+        <v>18409.4206532835</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2192,7 +2192,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>1.124099367268158</v>
+        <v>0.624659011346387</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2200,7 +2200,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>0.7104247120638858</v>
+        <v>0.7262650305460934</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2208,7 +2208,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="n">
-        <v>2.735528866520372</v>
+        <v>2.816856563164909</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2216,7 +2216,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="n">
-        <v>0.2936462106667154</v>
+        <v>0.2902694698354936</v>
       </c>
     </row>
     <row r="12" spans="1:4">

</xml_diff>

<commit_message>
Put Fiji cost inputs in Fiji spreadsheet
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -5,23 +5,23 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Google Drive\GitHub\AuTuMN\AuTuMN\autumn\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\GitHub\AuTuMN\AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="5484"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="5472"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
     <sheet name="time_variants" sheetId="2" r:id="rId2"/>
     <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
   <si>
     <t>parameter</t>
   </si>
@@ -155,16 +155,37 @@
     <t>runge_kutta</t>
   </si>
   <si>
+    <t>econ_unitcost_treatment_support</t>
+  </si>
+  <si>
+    <t>econ_unitcost_xpert</t>
+  </si>
+  <si>
+    <t>econ_unitcost_ipt</t>
+  </si>
+  <si>
     <t>econ_unitcost_ipt_age0to5</t>
   </si>
   <si>
+    <t>econ_unitcost_ipt_age5to15</t>
+  </si>
+  <si>
+    <t>econ_unitcost_ipt_age15up</t>
+  </si>
+  <si>
+    <t>econ_startupcost_ipt_age15up</t>
+  </si>
+  <si>
+    <t>econ_startupcost_ipt_age5to15</t>
+  </si>
+  <si>
     <t>econ_startupcost_ipt_age0to5</t>
   </si>
   <si>
-    <t>econ_unitcost_ipt_age5to15</t>
-  </si>
-  <si>
-    <t>econ_startupcost_ipt_age5to15</t>
+    <t>econ_startupcost_ipt</t>
+  </si>
+  <si>
+    <t>econ_unitcost_xpertacf</t>
   </si>
 </sst>
 </file>
@@ -276,7 +297,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -340,12 +361,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1093,7 +1108,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="661" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="661" applyFont="1" applyBorder="1"/>
@@ -1176,11 +1191,10 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="661" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="661" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="663" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma" xfId="663" builtinId="3"/>
@@ -2151,10 +2165,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2165,7 +2179,7 @@
     <col min="9" max="16384" width="9.109375" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
@@ -2173,39 +2187,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="48">
-        <v>10.036266850002439</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>10.025191783904701</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="51">
-        <v>9.9999999999999978E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="52" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="53">
-        <v>1845.0101752600381</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1861.8970139311441</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="54" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="55">
-        <v>18409.420653283501</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32746.978564107489</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="54" t="s">
         <v>6</v>
       </c>
@@ -2213,7 +2227,7 @@
         <v>892000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="56" t="s">
         <v>7</v>
       </c>
@@ -2227,39 +2241,39 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.62465901134638702</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.69658598274171812</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.72626503054609337</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.73905411984906</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>2.816856563164909</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.8811910418497151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.29026946983549362</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.51633608061546266</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="61" t="s">
         <v>12</v>
       </c>
@@ -2267,53 +2281,93 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="13" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="62">
-        <v>222</v>
-      </c>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="62"/>
-    </row>
-    <row r="14" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="63">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="64">
-        <v>118944</v>
-      </c>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="66"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="62" t="s">
+      <c r="B14" s="63">
+        <v>22.63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="62">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="62" t="s">
+      <c r="B15" s="64">
+        <v>178.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="65">
+        <v>70800</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="64">
-        <v>118944</v>
-      </c>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="66"/>
-    </row>
-    <row r="17" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="62"/>
-      <c r="B17" s="62"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="66"/>
+      <c r="B17" s="64">
+        <v>178.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="64" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="65">
+        <v>70800</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="64">
+        <v>178.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="65">
+        <v>70800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="64">
+        <v>178.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="64" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="65">
+        <v>70800</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="64">
+        <v>95.73</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -2347,10 +2401,10 @@
   <dimension ref="A1:AB14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R4" sqref="R4"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Revert "Put Fiji cost inputs in Fiji spreadsheet"
This reverts commit e1b52da5da07804f2ff8bd78ba8ae573b62db273.
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -5,23 +5,23 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\GitHub\AuTuMN\AuTuMN\autumn\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Google Drive\GitHub\AuTuMN\AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="5472"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15336" windowHeight="5484"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
     <sheet name="time_variants" sheetId="2" r:id="rId2"/>
     <sheet name="dropdown_lists" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>parameter</t>
   </si>
@@ -155,37 +155,16 @@
     <t>runge_kutta</t>
   </si>
   <si>
-    <t>econ_unitcost_treatment_support</t>
-  </si>
-  <si>
-    <t>econ_unitcost_xpert</t>
-  </si>
-  <si>
-    <t>econ_unitcost_ipt</t>
-  </si>
-  <si>
     <t>econ_unitcost_ipt_age0to5</t>
   </si>
   <si>
+    <t>econ_startupcost_ipt_age0to5</t>
+  </si>
+  <si>
     <t>econ_unitcost_ipt_age5to15</t>
   </si>
   <si>
-    <t>econ_unitcost_ipt_age15up</t>
-  </si>
-  <si>
-    <t>econ_startupcost_ipt_age15up</t>
-  </si>
-  <si>
     <t>econ_startupcost_ipt_age5to15</t>
-  </si>
-  <si>
-    <t>econ_startupcost_ipt_age0to5</t>
-  </si>
-  <si>
-    <t>econ_startupcost_ipt</t>
-  </si>
-  <si>
-    <t>econ_unitcost_xpertacf</t>
   </si>
 </sst>
 </file>
@@ -297,7 +276,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,6 +340,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1108,7 +1093,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="661" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="661" applyFont="1" applyBorder="1"/>
@@ -1191,10 +1176,11 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="661" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="661" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="663" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="663" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma" xfId="663" builtinId="3"/>
@@ -2165,10 +2151,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2179,7 +2165,7 @@
     <col min="9" max="16384" width="9.109375" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="45" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="45" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
@@ -2187,39 +2173,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="47" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="48">
-        <v>10.025191783904701</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10.036266850002439</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="50" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="51">
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9.9999999999999978E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="52" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="53">
-        <v>1861.8970139311441</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1845.0101752600381</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="54" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="55">
-        <v>32746.978564107489</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>18409.420653283501</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="54" t="s">
         <v>6</v>
       </c>
@@ -2227,7 +2213,7 @@
         <v>892000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="56" t="s">
         <v>7</v>
       </c>
@@ -2241,39 +2227,39 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.69658598274171812</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.62465901134638702</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.73905411984906</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.72626503054609337</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>2.8811910418497151</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2.816856563164909</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.51633608061546266</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.29026946983549362</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="61" t="s">
         <v>12</v>
       </c>
@@ -2281,93 +2267,53 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="63">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="62">
+        <v>222</v>
+      </c>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="62"/>
+    </row>
+    <row r="14" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="63">
-        <v>22.63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="64" t="s">
+      <c r="B14" s="64">
+        <v>118944</v>
+      </c>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="66"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="64">
-        <v>178.9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="64" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="65">
-        <v>70800</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="64" t="s">
+      <c r="B15" s="62">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="64">
-        <v>178.9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="64" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="65">
-        <v>70800</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="64" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="64">
-        <v>178.9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="64" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="65">
-        <v>70800</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="64" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="64">
-        <v>178.9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="64" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="65">
-        <v>70800</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="62" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="64">
-        <v>95.73</v>
-      </c>
+      <c r="B16" s="64">
+        <v>118944</v>
+      </c>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="66"/>
+    </row>
+    <row r="17" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="62"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="66"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -2401,10 +2347,10 @@
   <dimension ref="A1:AB14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Redo Fiji spreadsheet update
</commit_message>
<xml_diff>
--- a/autumn/xls/data_fiji.xlsx
+++ b/autumn/xls/data_fiji.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>parameter</t>
   </si>
@@ -165,6 +165,18 @@
   </si>
   <si>
     <t>econ_startupcost_ipt_age5to15</t>
+  </si>
+  <si>
+    <t>econ_unitcost_treatment_support</t>
+  </si>
+  <si>
+    <t>econ_unitcost_xpert</t>
+  </si>
+  <si>
+    <t>econ_unitcost_ipt</t>
+  </si>
+  <si>
+    <t>econ_startupcost_ipt</t>
   </si>
 </sst>
 </file>
@@ -2151,10 +2163,10 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2269,10 +2281,10 @@
     </row>
     <row r="13" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="62" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B13" s="62">
-        <v>222</v>
+        <v>534</v>
       </c>
       <c r="C13" s="63"/>
       <c r="D13" s="63"/>
@@ -2280,10 +2292,10 @@
     </row>
     <row r="14" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="62" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B14" s="64">
-        <v>118944</v>
+        <v>22.63</v>
       </c>
       <c r="C14" s="65"/>
       <c r="D14" s="65"/>
@@ -2291,29 +2303,57 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="62" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B15" s="62">
-        <v>222</v>
+        <v>178.9</v>
       </c>
     </row>
     <row r="16" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="62" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B16" s="64">
-        <v>118944</v>
+        <v>70800</v>
       </c>
       <c r="C16" s="65"/>
       <c r="D16" s="65"/>
       <c r="E16" s="66"/>
     </row>
     <row r="17" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="62"/>
-      <c r="B17" s="62"/>
+      <c r="A17" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="62">
+        <v>178.9</v>
+      </c>
       <c r="C17" s="65"/>
       <c r="D17" s="65"/>
       <c r="E17" s="66"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="57">
+        <v>70800</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="57">
+        <v>178.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="57">
+        <v>70800</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="4">

</xml_diff>